<commit_message>
gams map/set -> dataframe
</commit_message>
<xml_diff>
--- a/data/readfiles/generate_yaml.xlsx
+++ b/data/readfiles/generate_yaml.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chughes/Documents/Git/SLiDE/data/readfiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD2A81F4-6F7E-8144-A36B-6E65B0EA45EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1406F349-9C3B-7B44-8387-E719DE0AAA91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{3E1837C3-4AC3-0440-9699-55C5376D9610}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="1" xr2:uid="{3E1837C3-4AC3-0440-9699-55C5376D9610}"/>
   </bookViews>
   <sheets>
-    <sheet name="2_standardize" sheetId="1" r:id="rId1"/>
-    <sheet name="0_auto" sheetId="2" r:id="rId2"/>
+    <sheet name="parse" sheetId="1" r:id="rId1"/>
+    <sheet name="map_parse" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="491">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="484">
   <si>
     <t>bea_supply</t>
   </si>
@@ -1344,156 +1344,15 @@
     <t>Path: ["..", "data", "mapsources", "WiNDC", "windc_datastream", "core_maps"]</t>
   </si>
   <si>
-    <t>PathOut: ["..", "data", "coremaps", "std", "bea.csv"]</t>
-  </si>
-  <si>
-    <t>- {col: bea_code, type: String}</t>
-  </si>
-  <si>
-    <t>- {col: bea_desc, type: String}</t>
-  </si>
-  <si>
-    <t>- {col: bea_windc, type: String}</t>
-  </si>
-  <si>
-    <t>- {col: category, type: Any}</t>
-  </si>
-  <si>
-    <t>- {from: from, to: bea_code}</t>
-  </si>
-  <si>
-    <t>- {from: description, to: bea_desc}</t>
-  </si>
-  <si>
-    <t>- {from: to, to: bea_windc}</t>
-  </si>
-  <si>
-    <t>- {name: bea_all.csv, descriptor: summary}</t>
-  </si>
-  <si>
-    <t>- {name: bea_all_detailed.csv, descriptor: detail}</t>
-  </si>
-  <si>
     <t>Path: ["..", "data", "mapsources", "WiNDC", "windc_datastream", "core_maps", "gams"]</t>
   </si>
   <si>
-    <t>PathOut: ["..", "data", "coremaps", "std", "gsp.csv"]</t>
-  </si>
-  <si>
     <t xml:space="preserve">  name: map_gsp.csv</t>
   </si>
   <si>
     <t>Path: ["..", "data", "mapsources", "NAICS"]</t>
   </si>
   <si>
-    <t>PathOut: ["..", "data", "coremaps", "std", "naics.csv"]</t>
-  </si>
-  <si>
-    <t>name: "2-6 digit_2017_Codes.xlsx"</t>
-  </si>
-  <si>
-    <t>sheet: tbl_2017_title_description_coun</t>
-  </si>
-  <si>
-    <t>range: B1:C2198</t>
-  </si>
-  <si>
-    <t>descriptor: 2017</t>
-  </si>
-  <si>
-    <t>- {from: 2017 NAICS US Code, to: naics_code}</t>
-  </si>
-  <si>
-    <t>- {from: 2017 NAICS US Title, to: naics_desc}</t>
-  </si>
-  <si>
-    <t>on: "(?&lt;naics_level&gt;\\d*)"</t>
-  </si>
-  <si>
-    <t>input: naics_code</t>
-  </si>
-  <si>
-    <t>output: naics_level</t>
-  </si>
-  <si>
-    <t>col: naics_level</t>
-  </si>
-  <si>
-    <t>from: [2,3,4,5,6]</t>
-  </si>
-  <si>
-    <t>to:</t>
-  </si>
-  <si>
-    <t>- sector</t>
-  </si>
-  <si>
-    <t>- subsector</t>
-  </si>
-  <si>
-    <t>- industry_group</t>
-  </si>
-  <si>
-    <t>- naics_industry</t>
-  </si>
-  <si>
-    <t>- national_industry</t>
-  </si>
-  <si>
-    <t>PathOut: ["..", "data", "coremaps", "std", "regions.csv"]</t>
-  </si>
-  <si>
-    <t>PathOut: ["..", "data", "coremaps", "std", "sgf.csv"]</t>
-  </si>
-  <si>
-    <t>- {col: from, type: Any}</t>
-  </si>
-  <si>
-    <t>- {col: sgf_desc, type: String}</t>
-  </si>
-  <si>
-    <t>- {col: sgf_windc, type: Any}</t>
-  </si>
-  <si>
-    <t>- {col: units, type: String}</t>
-  </si>
-  <si>
-    <t>- col: from</t>
-  </si>
-  <si>
-    <t>val: missing</t>
-  </si>
-  <si>
-    <t>operation: "=="</t>
-  </si>
-  <si>
-    <t>val: unique</t>
-  </si>
-  <si>
-    <t>file: ../mapsources/WiNDC/windc_datastream/core_maps/gams/map_sgf.csv</t>
-  </si>
-  <si>
-    <t>from: from</t>
-  </si>
-  <si>
-    <t>to: to</t>
-  </si>
-  <si>
-    <t>input: sgf_desc</t>
-  </si>
-  <si>
-    <t>output: sgf_windc</t>
-  </si>
-  <si>
-    <t>- {name: map_seds_energy_tech.csv, descriptor: tech}</t>
-  </si>
-  <si>
-    <t>- {name: map_emissions.csv,        descriptor: emissions}</t>
-  </si>
-  <si>
-    <t>PathOut: ["..", "data", "coremaps", "std", "tech.csv"]</t>
-  </si>
-  <si>
     <t xml:space="preserve">  name: sgf.csv</t>
   </si>
   <si>
@@ -1507,6 +1366,126 @@
   </si>
   <si>
     <t xml:space="preserve">  descriptor: gsp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  name: "2-6 digit_2017_Codes.xlsx"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  sheet: tbl_2017_title_description_coun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  range: B1:C2198</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  descriptor: 2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  output: naics_level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - {name: bea_all.csv, descriptor: summary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - {name: map_emissions.csv,        descriptor: emissions}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - {name: bea_all_detailed.csv, descriptor: detail}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - {name: map_seds_energy_tech.csv, descriptor: tech}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - {col: bea_code, type: String}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - {col: from, type: Any}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - {col: bea_desc, type: String}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - {col: sgf_desc, type: String}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - {col: bea_windc, type: String}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - {col: sgf_windc, type: Any}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - {col: category, type: Any}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - {from: from, to: bea_code}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - {from: 2017 NAICS US Code, to: naics_code}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - {from: description, to: bea_desc}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - {from: 2017 NAICS US Title, to: naics_desc}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - {from: to, to: bea_windc}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  file:   ../mapsources/WiNDC/windc_datastream/core_maps/gams/map_sgf.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  on:     "(?&lt;naics_level&gt;\\d*)"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  col: naics_level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  from: [2,3,4,5,6]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  to:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - sector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - subsector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - industry_group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - naics_industry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - national_industry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - col: from</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    val: unique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  output: sgf_windc</t>
+  </si>
+  <si>
+    <t>PathOut: ["..", "data", "coremaps", "parse", "bea.csv"]</t>
+  </si>
+  <si>
+    <t>PathOut: ["..", "data", "coremaps", "parse", "gsp.csv"]</t>
+  </si>
+  <si>
+    <t>PathOut: ["..", "data", "coremaps", "parse", "naics.csv"]</t>
+  </si>
+  <si>
+    <t>PathOut: ["..", "data", "coremaps", "parse", "regions.csv"]</t>
+  </si>
+  <si>
+    <t>PathOut: ["..", "data", "coremaps", "parse", "sgf.csv"]</t>
+  </si>
+  <si>
+    <t>PathOut: ["..", "data", "coremaps", "parse", "tech.csv"]</t>
   </si>
 </sst>
 </file>
@@ -1929,7 +1908,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC6F1FC0-97F0-044C-906D-1FF8A7B5F9B8}">
   <dimension ref="A1:V148"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -6506,11 +6485,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7AB9832-7F74-B245-B43D-5B870966A3CC}">
   <dimension ref="A1:G77"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomRight" activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6544,10 +6523,10 @@
         <v>435</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>446</v>
+        <v>436</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>449</v>
+        <v>438</v>
       </c>
       <c r="E5" s="16" t="s">
         <v>435</v>
@@ -6556,7 +6535,7 @@
         <v>435</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>446</v>
+        <v>436</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="17" customFormat="1"/>
@@ -6565,22 +6544,22 @@
         <v>353</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>436</v>
+        <v>478</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>447</v>
+        <v>479</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>450</v>
+        <v>480</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>468</v>
+        <v>481</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>469</v>
+        <v>482</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="17" customFormat="1"/>
@@ -6609,52 +6588,52 @@
     </row>
     <row r="10" spans="1:7">
       <c r="B10" s="16" t="s">
+        <v>449</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>437</v>
+      </c>
+      <c r="D10" s="16" t="s">
         <v>444</v>
       </c>
-      <c r="C10" s="16" t="s">
-        <v>448</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>451</v>
-      </c>
       <c r="E10" s="16" t="s">
-        <v>488</v>
+        <v>441</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>486</v>
+        <v>439</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>484</v>
+        <v>450</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="B11" s="16" t="s">
+        <v>451</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>443</v>
+      </c>
+      <c r="D11" s="16" t="s">
         <v>445</v>
       </c>
-      <c r="C11" s="16" t="s">
-        <v>490</v>
-      </c>
-      <c r="D11" s="16" t="s">
+      <c r="E11" s="16" t="s">
+        <v>442</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>440</v>
+      </c>
+      <c r="G11" s="16" t="s">
         <v>452</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>489</v>
-      </c>
-      <c r="F11" s="16" t="s">
-        <v>487</v>
-      </c>
-      <c r="G11" s="16" t="s">
-        <v>483</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="D12" s="16" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="D13" s="16" t="s">
-        <v>454</v>
+        <v>447</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="17" customFormat="1"/>
@@ -6677,34 +6656,34 @@
     </row>
     <row r="19" spans="1:6">
       <c r="B19" s="16" t="s">
-        <v>437</v>
+        <v>453</v>
       </c>
       <c r="F19" s="16" t="s">
-        <v>470</v>
+        <v>454</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="B20" s="16" t="s">
-        <v>438</v>
+        <v>455</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>471</v>
+        <v>456</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="B21" s="16" t="s">
-        <v>439</v>
+        <v>457</v>
       </c>
       <c r="F21" s="16" t="s">
-        <v>472</v>
+        <v>458</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="B22" s="16" t="s">
-        <v>440</v>
+        <v>459</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>473</v>
+        <v>311</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="17" customFormat="1"/>
@@ -6721,23 +6700,23 @@
     </row>
     <row r="25" spans="1:6">
       <c r="B25" s="16" t="s">
-        <v>441</v>
+        <v>460</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>455</v>
+        <v>461</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="B26" s="16" t="s">
-        <v>442</v>
+        <v>462</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>456</v>
+        <v>463</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="B27" s="16" t="s">
-        <v>443</v>
+        <v>464</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="17" customFormat="1"/>
@@ -6757,17 +6736,17 @@
     </row>
     <row r="41" spans="1:4">
       <c r="D41" s="16" t="s">
-        <v>457</v>
+        <v>466</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="D42" s="16" t="s">
-        <v>458</v>
+        <v>348</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="D43" s="16" t="s">
-        <v>459</v>
+        <v>448</v>
       </c>
     </row>
     <row r="44" spans="1:4" s="17" customFormat="1"/>
@@ -6793,27 +6772,27 @@
     </row>
     <row r="54" spans="1:6">
       <c r="F54" s="16" t="s">
-        <v>478</v>
+        <v>465</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="F55" s="16" t="s">
-        <v>479</v>
+        <v>213</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="F56" s="16" t="s">
-        <v>480</v>
+        <v>214</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="F57" s="16" t="s">
-        <v>481</v>
+        <v>215</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="F58" s="16" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
     </row>
     <row r="59" spans="1:6" s="17" customFormat="1"/>
@@ -6827,42 +6806,42 @@
     </row>
     <row r="61" spans="1:6">
       <c r="D61" s="16" t="s">
-        <v>460</v>
+        <v>467</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="D62" s="16" t="s">
-        <v>461</v>
+        <v>468</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="D63" s="16" t="s">
-        <v>462</v>
+        <v>469</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="D64" s="16" t="s">
-        <v>463</v>
+        <v>470</v>
       </c>
     </row>
     <row r="65" spans="1:6">
       <c r="D65" s="16" t="s">
-        <v>464</v>
+        <v>471</v>
       </c>
     </row>
     <row r="66" spans="1:6">
       <c r="D66" s="16" t="s">
-        <v>465</v>
+        <v>472</v>
       </c>
     </row>
     <row r="67" spans="1:6">
       <c r="D67" s="16" t="s">
-        <v>466</v>
+        <v>473</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="D68" s="16" t="s">
-        <v>467</v>
+        <v>474</v>
       </c>
     </row>
     <row r="70" spans="1:6" s="17" customFormat="1"/>
@@ -6876,32 +6855,32 @@
     </row>
     <row r="72" spans="1:6">
       <c r="F72" s="16" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
     </row>
     <row r="73" spans="1:6">
       <c r="F73" s="16" t="s">
-        <v>475</v>
+        <v>103</v>
       </c>
     </row>
     <row r="74" spans="1:6">
       <c r="F74" s="16" t="s">
-        <v>476</v>
+        <v>52</v>
       </c>
     </row>
     <row r="75" spans="1:6">
       <c r="F75" s="16" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
     </row>
     <row r="76" spans="1:6">
       <c r="F76" s="16" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="77" spans="1:6">
       <c r="F77" s="16" t="s">
-        <v>476</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
gams to dataframe done
</commit_message>
<xml_diff>
--- a/data/readfiles/generate_yaml.xlsx
+++ b/data/readfiles/generate_yaml.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chughes/Documents/Git/SLiDE/data/readfiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A116683E-2C44-7C4E-A34A-2F7A192E0326}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16DAFF50-3C4F-8B4B-BEBA-6EEE92F00A06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{3E1837C3-4AC3-0440-9699-55C5376D9610}"/>
+    <workbookView xWindow="-2640" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{3E1837C3-4AC3-0440-9699-55C5376D9610}"/>
   </bookViews>
   <sheets>
     <sheet name="map_parse" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1331" uniqueCount="678">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1328" uniqueCount="676">
   <si>
     <t>bea_supply</t>
   </si>
@@ -1201,9 +1201,6 @@
     <t xml:space="preserve">  output: sgf_windc</t>
   </si>
   <si>
-    <t>missing_temp_bea_det</t>
-  </si>
-  <si>
     <t>gsp</t>
   </si>
   <si>
@@ -1847,9 +1844,6 @@
   </si>
   <si>
     <t>Path: [.., data, mapsources]</t>
-  </si>
-  <si>
-    <t>Path: [.., data, mapsources, WiNDC, windc_build, build_files, maps]</t>
   </si>
   <si>
     <t>Path: [.., data, mapsources, WiNDC, windc_datastream, core_maps]</t>
@@ -2507,51 +2501,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7AB9832-7F74-B245-B43D-5B870966A3CC}">
-  <dimension ref="A1:L81"/>
+  <dimension ref="A1:K81"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B25" sqref="B25"/>
+      <selection pane="bottomRight" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="15"/>
-    <col min="2" max="4" width="93" style="15" customWidth="1"/>
-    <col min="5" max="5" width="92.33203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="92.83203125" style="15" customWidth="1"/>
-    <col min="7" max="8" width="67" style="15" customWidth="1"/>
-    <col min="9" max="9" width="92.83203125" style="15" customWidth="1"/>
-    <col min="10" max="10" width="92.33203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="102" style="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="93.33203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="92.83203125" style="15" customWidth="1"/>
-    <col min="14" max="16384" width="10.83203125" style="15"/>
+    <col min="2" max="3" width="93" style="15" customWidth="1"/>
+    <col min="4" max="4" width="92.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="92.83203125" style="15" customWidth="1"/>
+    <col min="6" max="7" width="67" style="15" customWidth="1"/>
+    <col min="8" max="8" width="92.83203125" style="15" customWidth="1"/>
+    <col min="9" max="9" width="92.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="102" style="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="93.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="92.83203125" style="15" customWidth="1"/>
+    <col min="13" max="16384" width="10.83203125" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="9" customFormat="1">
+    <row r="1" spans="1:11" s="9" customFormat="1">
       <c r="B1" s="9" t="s">
+        <v>658</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>362</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>388</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>660</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>661</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>362</v>
       </c>
       <c r="F1" s="9" t="s">
         <v>389</v>
       </c>
       <c r="G1" s="9" t="s">
+        <v>595</v>
+      </c>
+      <c r="H1" s="9" t="s">
         <v>390</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>596</v>
       </c>
       <c r="I1" s="9" t="s">
         <v>391</v>
@@ -2560,133 +2554,127 @@
         <v>392</v>
       </c>
       <c r="K1" s="9" t="s">
-        <v>393</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
-      <c r="E2" s="15" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" s="16" customFormat="1"/>
-    <row r="4" spans="1:12">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="D2" s="15" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="16" customFormat="1"/>
+    <row r="4" spans="1:11">
       <c r="B4" s="15" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F4" s="15" t="s">
         <v>396</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="I4" s="15" t="s">
         <v>396</v>
       </c>
       <c r="J4" s="15" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="K4" s="15" t="s">
-        <v>396</v>
-      </c>
-      <c r="L4" s="15" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" s="16" customFormat="1"/>
-    <row r="6" spans="1:12">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="16" customFormat="1"/>
+    <row r="6" spans="1:11">
       <c r="A6" s="15" t="s">
         <v>291</v>
       </c>
       <c r="B6" s="15" t="s">
+        <v>603</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>603</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>603</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>602</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>605</v>
+      </c>
+      <c r="G6" s="15" t="s">
         <v>604</v>
       </c>
-      <c r="C6" s="15" t="s">
-        <v>605</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>605</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>605</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>603</v>
-      </c>
-      <c r="G6" s="15" t="s">
-        <v>607</v>
-      </c>
       <c r="H6" s="15" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="I6" s="15" t="s">
         <v>603</v>
       </c>
       <c r="J6" s="15" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="K6" s="15" t="s">
-        <v>606</v>
-      </c>
-      <c r="L6" s="15" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" s="16" customFormat="1"/>
-    <row r="8" spans="1:12">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="16" customFormat="1"/>
+    <row r="8" spans="1:11">
       <c r="A8" s="15" t="s">
         <v>292</v>
       </c>
+      <c r="B8" s="15" t="s">
+        <v>660</v>
+      </c>
       <c r="C8" s="15" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>663</v>
+        <v>607</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="F8" s="15" t="s">
         <v>608</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="G8" s="17" t="s">
+        <v>609</v>
+      </c>
+      <c r="H8" s="15" t="s">
         <v>610</v>
       </c>
-      <c r="H8" s="17" t="s">
+      <c r="I8" s="17" t="s">
         <v>611</v>
       </c>
-      <c r="I8" s="15" t="s">
+      <c r="J8" s="17" t="s">
         <v>612</v>
       </c>
-      <c r="J8" s="17" t="s">
+      <c r="K8" s="15" t="s">
         <v>613</v>
       </c>
-      <c r="K8" s="17" t="s">
-        <v>614</v>
-      </c>
-      <c r="L8" s="15" t="s">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" s="16" customFormat="1"/>
-    <row r="10" spans="1:12">
+    </row>
+    <row r="9" spans="1:11" s="16" customFormat="1"/>
+    <row r="10" spans="1:11">
       <c r="A10" s="15" t="s">
         <v>293</v>
       </c>
+      <c r="B10" s="15" t="s">
+        <v>8</v>
+      </c>
       <c r="C10" s="15" t="s">
         <v>8</v>
       </c>
@@ -2697,474 +2685,471 @@
         <v>8</v>
       </c>
       <c r="F10" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="G10" s="15" t="s">
         <v>8</v>
-      </c>
-      <c r="G10" s="15" t="s">
-        <v>129</v>
       </c>
       <c r="H10" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="I10" s="15" t="s">
+      <c r="I10" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="J10" s="17" t="s">
+      <c r="J10" s="15" t="s">
         <v>8</v>
       </c>
       <c r="K10" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="L10" s="15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
+    </row>
+    <row r="11" spans="1:11">
+      <c r="B11" s="15" t="s">
+        <v>666</v>
+      </c>
       <c r="C11" s="15" t="s">
-        <v>668</v>
+        <v>371</v>
       </c>
       <c r="D11" s="15" t="s">
+        <v>572</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>591</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>365</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>596</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>598</v>
+      </c>
+      <c r="I11" s="15" t="s">
+        <v>363</v>
+      </c>
+      <c r="J11" s="15" t="s">
+        <v>370</v>
+      </c>
+      <c r="K11" s="15" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="D12" s="15" t="s">
         <v>371</v>
       </c>
-      <c r="E11" s="15" t="s">
-        <v>573</v>
-      </c>
-      <c r="F11" s="15" t="s">
+      <c r="E12" s="15" t="s">
         <v>592</v>
       </c>
-      <c r="G11" s="15" t="s">
-        <v>365</v>
-      </c>
-      <c r="H11" s="15" t="s">
+      <c r="F12" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="G12" s="15" t="s">
         <v>597</v>
       </c>
-      <c r="I11" s="15" t="s">
+      <c r="H12" s="15" t="s">
         <v>599</v>
       </c>
-      <c r="J11" s="15" t="s">
-        <v>363</v>
-      </c>
-      <c r="K11" s="15" t="s">
-        <v>370</v>
-      </c>
-      <c r="L11" s="15" t="s">
+      <c r="I12" s="15" t="s">
+        <v>364</v>
+      </c>
+      <c r="J12" s="15" t="s">
+        <v>372</v>
+      </c>
+      <c r="K12" s="15" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
-      <c r="E12" s="15" t="s">
-        <v>371</v>
-      </c>
-      <c r="F12" s="15" t="s">
+    <row r="13" spans="1:11">
+      <c r="E13" s="15" t="s">
         <v>593</v>
       </c>
-      <c r="G12" s="15" t="s">
-        <v>366</v>
-      </c>
-      <c r="H12" s="15" t="s">
-        <v>598</v>
-      </c>
-      <c r="I12" s="15" t="s">
+      <c r="F13" s="15" t="s">
+        <v>367</v>
+      </c>
+      <c r="H13" s="15" t="s">
         <v>600</v>
       </c>
-      <c r="J12" s="15" t="s">
-        <v>364</v>
-      </c>
-      <c r="K12" s="15" t="s">
-        <v>372</v>
-      </c>
-      <c r="L12" s="15" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="F13" s="15" t="s">
+    </row>
+    <row r="14" spans="1:11">
+      <c r="E14" s="15" t="s">
         <v>594</v>
       </c>
-      <c r="G13" s="15" t="s">
-        <v>367</v>
-      </c>
-      <c r="I13" s="15" t="s">
+      <c r="F14" s="15" t="s">
+        <v>368</v>
+      </c>
+      <c r="H14" s="15" t="s">
         <v>601</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
-      <c r="F14" s="15" t="s">
-        <v>595</v>
-      </c>
-      <c r="G14" s="15" t="s">
-        <v>368</v>
-      </c>
-      <c r="I14" s="15" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" s="16" customFormat="1"/>
-    <row r="16" spans="1:12">
+    <row r="15" spans="1:11" s="16" customFormat="1"/>
+    <row r="16" spans="1:11">
       <c r="A16" s="15" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="16" customFormat="1"/>
-    <row r="19" spans="1:10">
+    <row r="18" spans="1:9" s="16" customFormat="1"/>
+    <row r="19" spans="1:9">
       <c r="A19" s="15" t="s">
         <v>295</v>
       </c>
+      <c r="B19" s="15" t="s">
+        <v>11</v>
+      </c>
       <c r="C19" s="15" t="s">
         <v>11</v>
       </c>
       <c r="D19" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E19" s="15" t="s">
+      <c r="F19" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="G19" s="15" t="s">
+      <c r="I19" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="J19" s="15" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
+    </row>
+    <row r="20" spans="1:9">
+      <c r="B20" s="15" t="s">
+        <v>565</v>
+      </c>
       <c r="C20" s="15" t="s">
+        <v>565</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>565</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="I20" s="15" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="B21" s="15" t="s">
         <v>566</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="C21" s="15" t="s">
         <v>566</v>
       </c>
-      <c r="E20" s="15" t="s">
+      <c r="D21" s="15" t="s">
         <v>566</v>
       </c>
-      <c r="G20" s="15" t="s">
-        <v>204</v>
-      </c>
-      <c r="J20" s="15" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10">
-      <c r="C21" s="15" t="s">
-        <v>567</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>567</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>567</v>
-      </c>
-      <c r="G21" s="15" t="s">
-        <v>577</v>
-      </c>
-      <c r="J21" s="15" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
+      <c r="F21" s="15" t="s">
+        <v>576</v>
+      </c>
+      <c r="I21" s="15" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="B22" s="15" t="s">
+        <v>373</v>
+      </c>
       <c r="C22" s="15" t="s">
         <v>373</v>
       </c>
       <c r="D22" s="15" t="s">
         <v>373</v>
       </c>
-      <c r="E22" s="15" t="s">
-        <v>373</v>
-      </c>
-      <c r="G22" s="15" t="s">
-        <v>576</v>
-      </c>
-      <c r="J22" s="15" t="s">
+      <c r="F22" s="15" t="s">
+        <v>575</v>
+      </c>
+      <c r="I22" s="15" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:9">
+      <c r="B23" s="15" t="s">
+        <v>564</v>
+      </c>
       <c r="C23" s="15" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>565</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>565</v>
-      </c>
-      <c r="J23" s="15" t="s">
+        <v>564</v>
+      </c>
+      <c r="I23" s="15" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="24" spans="1:10" s="16" customFormat="1"/>
-    <row r="25" spans="1:10">
+    <row r="24" spans="1:9" s="16" customFormat="1"/>
+    <row r="25" spans="1:9">
       <c r="A25" s="15" t="s">
         <v>296</v>
       </c>
+      <c r="B25" s="15" t="s">
+        <v>19</v>
+      </c>
       <c r="C25" s="15" t="s">
         <v>19</v>
       </c>
       <c r="D25" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="E25" s="15" t="s">
+      <c r="F25" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="G25" s="15" t="s">
+      <c r="I25" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="J25" s="15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10">
+    </row>
+    <row r="26" spans="1:9">
+      <c r="B26" s="15" t="s">
+        <v>567</v>
+      </c>
       <c r="C26" s="15" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>568</v>
-      </c>
-      <c r="E26" s="15" t="s">
-        <v>568</v>
-      </c>
-      <c r="G26" s="15" t="s">
-        <v>574</v>
-      </c>
-      <c r="J26" s="15" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10">
+        <v>567</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>573</v>
+      </c>
+      <c r="I26" s="15" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="B27" s="15" t="s">
+        <v>375</v>
+      </c>
       <c r="C27" s="15" t="s">
         <v>375</v>
       </c>
       <c r="D27" s="15" t="s">
         <v>375</v>
       </c>
-      <c r="E27" s="15" t="s">
-        <v>375</v>
-      </c>
-      <c r="G27" s="15" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10">
+      <c r="F27" s="15" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="B28" s="15" t="s">
+        <v>568</v>
+      </c>
       <c r="C28" s="15" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>569</v>
-      </c>
-      <c r="E28" s="15" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" s="16" customFormat="1"/>
-    <row r="34" spans="1:7">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" s="16" customFormat="1"/>
+    <row r="34" spans="1:6">
       <c r="A34" s="15" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="40" spans="1:7" s="16" customFormat="1"/>
-    <row r="41" spans="1:7">
+    <row r="40" spans="1:6" s="16" customFormat="1"/>
+    <row r="41" spans="1:6">
       <c r="A41" s="15" t="s">
         <v>298</v>
       </c>
-      <c r="G41" s="15" t="s">
+      <c r="F41" s="15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
-      <c r="G42" s="15" t="s">
+    <row r="42" spans="1:6">
+      <c r="F42" s="15" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
-      <c r="G43" s="15" t="s">
+    <row r="43" spans="1:6">
+      <c r="F43" s="15" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
-      <c r="G44" s="15" t="s">
+    <row r="44" spans="1:6">
+      <c r="F44" s="15" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="45" spans="1:7" s="16" customFormat="1"/>
-    <row r="46" spans="1:7">
+    <row r="45" spans="1:6" s="16" customFormat="1"/>
+    <row r="46" spans="1:6">
       <c r="A46" s="15" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="50" spans="1:10" s="16" customFormat="1"/>
-    <row r="51" spans="1:10">
+    <row r="50" spans="1:9" s="16" customFormat="1"/>
+    <row r="51" spans="1:9">
       <c r="A51" s="15" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="53" spans="1:10" s="16" customFormat="1"/>
-    <row r="54" spans="1:10">
+    <row r="53" spans="1:9" s="16" customFormat="1"/>
+    <row r="54" spans="1:9">
       <c r="A54" s="15" t="s">
         <v>301</v>
       </c>
-      <c r="J54" s="15" t="s">
+      <c r="I54" s="15" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
-      <c r="J55" s="15" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10">
-      <c r="J56" s="15" t="s">
+    <row r="55" spans="1:9">
+      <c r="I55" s="15" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="I56" s="15" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
-      <c r="J57" s="15" t="s">
+    <row r="57" spans="1:9">
+      <c r="I57" s="15" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
-      <c r="J58" s="15" t="s">
+    <row r="58" spans="1:9">
+      <c r="I58" s="15" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="59" spans="1:10">
-      <c r="J59" s="15" t="s">
+    <row r="59" spans="1:9">
+      <c r="I59" s="15" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="60" spans="1:10" s="16" customFormat="1"/>
-    <row r="61" spans="1:10">
+    <row r="60" spans="1:9" s="16" customFormat="1"/>
+    <row r="61" spans="1:9">
       <c r="A61" s="15" t="s">
         <v>302</v>
       </c>
+      <c r="B61" s="15" t="s">
+        <v>76</v>
+      </c>
       <c r="C61" s="15" t="s">
         <v>76</v>
       </c>
       <c r="D61" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="E61" s="15" t="s">
+      <c r="F61" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="G61" s="15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10">
+    </row>
+    <row r="62" spans="1:9">
+      <c r="B62" s="15" t="s">
+        <v>673</v>
+      </c>
       <c r="C62" s="15" t="s">
+        <v>673</v>
+      </c>
+      <c r="D62" s="15" t="s">
+        <v>673</v>
+      </c>
+      <c r="F62" s="15" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="B63" s="15" t="s">
+        <v>674</v>
+      </c>
+      <c r="C63" s="15" t="s">
+        <v>674</v>
+      </c>
+      <c r="D63" s="15" t="s">
+        <v>674</v>
+      </c>
+      <c r="F63" s="15" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="B64" s="15" t="s">
         <v>675</v>
       </c>
-      <c r="D62" s="15" t="s">
+      <c r="C64" s="15" t="s">
         <v>675</v>
       </c>
-      <c r="E62" s="15" t="s">
+      <c r="D64" s="15" t="s">
         <v>675</v>
       </c>
-      <c r="G62" s="15" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10">
-      <c r="C63" s="15" t="s">
-        <v>676</v>
-      </c>
-      <c r="D63" s="15" t="s">
-        <v>676</v>
-      </c>
-      <c r="E63" s="15" t="s">
-        <v>676</v>
-      </c>
-      <c r="G63" s="15" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10">
-      <c r="C64" s="15" t="s">
-        <v>677</v>
-      </c>
-      <c r="D64" s="15" t="s">
-        <v>677</v>
-      </c>
-      <c r="E64" s="15" t="s">
-        <v>677</v>
-      </c>
-      <c r="G64" s="15" t="s">
+      <c r="F64" s="15" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
-      <c r="G65" s="15" t="s">
+    <row r="65" spans="1:9">
+      <c r="F65" s="15" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
-      <c r="G66" s="15" t="s">
+    <row r="66" spans="1:9">
+      <c r="F66" s="15" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
-      <c r="G67" s="15" t="s">
+    <row r="67" spans="1:9">
+      <c r="F67" s="15" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
-      <c r="G68" s="15" t="s">
+    <row r="68" spans="1:9">
+      <c r="F68" s="15" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="69" spans="1:10">
-      <c r="G69" s="15" t="s">
+    <row r="69" spans="1:9">
+      <c r="F69" s="15" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="71" spans="1:10" s="16" customFormat="1"/>
-    <row r="72" spans="1:10">
+    <row r="71" spans="1:9" s="16" customFormat="1"/>
+    <row r="72" spans="1:9">
       <c r="A72" s="15" t="s">
         <v>303</v>
       </c>
-      <c r="J72" s="15" t="s">
+      <c r="I72" s="15" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="73" spans="1:10">
-      <c r="J73" s="15" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10">
-      <c r="J74" s="15" t="s">
+    <row r="73" spans="1:9">
+      <c r="I73" s="15" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9">
+      <c r="I74" s="15" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="75" spans="1:10">
-      <c r="J75" s="15" t="s">
+    <row r="75" spans="1:9">
+      <c r="I75" s="15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="76" spans="1:10">
-      <c r="J76" s="15" t="s">
+    <row r="76" spans="1:9">
+      <c r="I76" s="15" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="77" spans="1:10">
-      <c r="J77" s="15" t="s">
+    <row r="77" spans="1:9">
+      <c r="I77" s="15" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="78" spans="1:10">
-      <c r="J78" s="15" t="s">
+    <row r="78" spans="1:9">
+      <c r="I78" s="15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="79" spans="1:10">
-      <c r="J79" s="15" t="s">
+    <row r="79" spans="1:9">
+      <c r="I79" s="15" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="80" spans="1:10">
-      <c r="J80" s="15" t="s">
+    <row r="80" spans="1:9">
+      <c r="I80" s="15" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="81" spans="10:10">
-      <c r="J81" s="15" t="s">
+    <row r="81" spans="9:9">
+      <c r="I81" s="15" t="s">
         <v>47</v>
       </c>
     </row>
@@ -3178,11 +3163,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4987CBB-E748-D040-83F8-8A97947A4656}">
   <dimension ref="A1:F90"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:XFD1"/>
+      <selection activeCell="B33" sqref="B33"/>
+      <selection pane="topRight" activeCell="B33" sqref="B33"/>
+      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
+      <selection pane="bottomRight" activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="93" defaultRowHeight="14"/>
@@ -3195,36 +3181,36 @@
     <row r="1" spans="1:6" s="18" customFormat="1">
       <c r="A1" s="12"/>
       <c r="B1" s="12" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C1" s="12" t="s">
+        <v>401</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>402</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="E1" s="12" t="s">
         <v>403</v>
       </c>
-      <c r="E1" s="12" t="s">
-        <v>404</v>
-      </c>
       <c r="F1" s="12" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="B2" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>396</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>396</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>396</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>396</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -3240,19 +3226,19 @@
         <v>291</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>620</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>622</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>624</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -3268,19 +3254,19 @@
         <v>292</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>618</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>620</v>
-      </c>
       <c r="E7" s="2" t="s">
+        <v>621</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>623</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>625</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -3313,120 +3299,120 @@
     </row>
     <row r="10" spans="1:6">
       <c r="B10" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="B11" s="2" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="B12" s="2" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="B13" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="B14" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>477</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>522</v>
-      </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>478</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="B15" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>480</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>481</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="B16" s="2" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="B17" s="2" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -3456,16 +3442,16 @@
     </row>
     <row r="21" spans="1:6">
       <c r="B21" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -3498,184 +3484,184 @@
     </row>
     <row r="24" spans="1:6">
       <c r="B24" s="2" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="B25" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>401</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>401</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>407</v>
-      </c>
       <c r="F25" s="2" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="B26" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="D26" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="E26" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="E26" s="2" t="s">
-        <v>411</v>
-      </c>
       <c r="F26" s="2" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="B27" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="D27" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>414</v>
-      </c>
       <c r="F27" s="2" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="B28" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="E28" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="E28" s="2" t="s">
-        <v>418</v>
-      </c>
       <c r="F28" s="2" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="B29" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="D29" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>420</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>421</v>
-      </c>
       <c r="F29" s="2" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="B30" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>422</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="E30" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="E30" s="2" t="s">
-        <v>425</v>
-      </c>
       <c r="F30" s="2" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="B31" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>426</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>427</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="E31" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="E31" s="2" t="s">
-        <v>429</v>
-      </c>
       <c r="F31" s="2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="B32" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>430</v>
       </c>
-      <c r="E32" s="2" t="s">
-        <v>431</v>
-      </c>
       <c r="F32" s="2" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="B33" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="E33" s="2" t="s">
-        <v>433</v>
-      </c>
       <c r="F33" s="2" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="B34" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>434</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="B35" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="E35" s="2" t="s">
         <v>436</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>437</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="B36" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>438</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -3705,131 +3691,131 @@
     </row>
     <row r="39" spans="1:6">
       <c r="B39" s="10" t="s">
+        <v>439</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="D39" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="E39" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="B40" s="10" t="s">
+        <v>443</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>444</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="D40" s="2" t="s">
         <v>445</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="E40" s="2" t="s">
         <v>446</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="B41" s="10" t="s">
+        <v>447</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>448</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="D41" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="E41" s="2" t="s">
         <v>450</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="B42" s="10" t="s">
+        <v>451</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>452</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="D42" s="2" t="s">
         <v>453</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="E42" s="2" t="s">
         <v>454</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="B43" s="10" t="s">
+        <v>455</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>456</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="D43" s="2" t="s">
         <v>457</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="E43" s="2" t="s">
         <v>458</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="B44" s="10" t="s">
+        <v>459</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>460</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="D44" s="2" t="s">
         <v>461</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="E44" s="2" t="s">
         <v>462</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>463</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="B45" s="10" t="s">
+        <v>463</v>
+      </c>
+      <c r="E45" s="2" t="s">
         <v>464</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="B46" s="10" t="s">
+        <v>465</v>
+      </c>
+      <c r="E46" s="2" t="s">
         <v>466</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="B47" s="10" t="s">
+        <v>467</v>
+      </c>
+      <c r="E47" s="2" t="s">
         <v>468</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>469</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="B48" s="10" t="s">
+        <v>469</v>
+      </c>
+      <c r="E48" s="2" t="s">
         <v>470</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="B49" s="10" t="s">
+        <v>471</v>
+      </c>
+      <c r="E49" s="2" t="s">
         <v>472</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>473</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="B50" s="11" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -3866,50 +3852,50 @@
     </row>
     <row r="60" spans="1:6">
       <c r="D60" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="61" spans="1:6">
       <c r="D61" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="D62" s="2" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="D63" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="D64" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="65" spans="1:6">
       <c r="D65" s="2" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -3946,10 +3932,10 @@
     </row>
     <row r="73" spans="1:6">
       <c r="C73" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="D73" s="2" t="s">
         <v>475</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -3970,27 +3956,27 @@
     </row>
     <row r="76" spans="1:6">
       <c r="E76" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="77" spans="1:6">
       <c r="E77" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="78" spans="1:6">
       <c r="E78" s="2" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="79" spans="1:6">
       <c r="E79" s="2" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="80" spans="1:6">
       <c r="E80" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -4020,68 +4006,68 @@
     </row>
     <row r="83" spans="1:6">
       <c r="B83" s="2" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="84" spans="1:6">
       <c r="B84" s="2" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="85" spans="1:6">
       <c r="B85" s="2" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="86" spans="1:6">
       <c r="B86" s="2" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="87" spans="1:6">
       <c r="B87" s="2" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="88" spans="1:6">
       <c r="B88" s="2" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -4107,11 +4093,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC6F1FC0-97F0-044C-906D-1FF8A7B5F9B8}">
   <dimension ref="A1:V126"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F69" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F80" sqref="F80"/>
+    <sheetView showGridLines="0" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B69" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="B33" sqref="B33"/>
+      <selection pane="topRight" activeCell="B33" sqref="B33"/>
+      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
+      <selection pane="bottomRight" activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -4223,67 +4210,67 @@
     <row r="4" spans="1:22" s="5" customFormat="1"/>
     <row r="5" spans="1:22">
       <c r="B5" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="6" spans="1:22" s="5" customFormat="1"/>
@@ -4292,67 +4279,67 @@
         <v>291</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="G7" s="2" t="s">
+        <v>630</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>632</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>634</v>
-      </c>
       <c r="I7" s="2" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="J7" s="1" t="s">
+        <v>636</v>
+      </c>
+      <c r="K7" s="2" t="s">
         <v>638</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="L7" s="2" t="s">
         <v>640</v>
       </c>
-      <c r="L7" s="2" t="s">
-        <v>642</v>
-      </c>
       <c r="M7" s="2" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="T7" s="2" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="U7" s="2" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="V7" s="2" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
     </row>
     <row r="8" spans="1:22" s="5" customFormat="1">
@@ -4364,67 +4351,67 @@
         <v>292</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>627</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>628</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="E9" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>629</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>630</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>671</v>
-      </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>631</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>633</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>635</v>
-      </c>
       <c r="I9" s="1" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="J9" s="1" t="s">
+        <v>637</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="L9" s="1" t="s">
         <v>639</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="M9" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>642</v>
+      </c>
+      <c r="O9" s="1" t="s">
         <v>643</v>
       </c>
-      <c r="L9" s="1" t="s">
-        <v>641</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>672</v>
-      </c>
-      <c r="N9" s="1" t="s">
+      <c r="P9" s="1" t="s">
         <v>644</v>
       </c>
-      <c r="O9" s="1" t="s">
-        <v>645</v>
-      </c>
-      <c r="P9" s="1" t="s">
+      <c r="Q9" s="1" t="s">
         <v>646</v>
       </c>
-      <c r="Q9" s="1" t="s">
-        <v>648</v>
-      </c>
       <c r="R9" s="1" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="S9" s="1" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="V9" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
     </row>
     <row r="10" spans="1:22" s="5" customFormat="1"/>
@@ -4510,13 +4497,13 @@
         <v>333</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>9</v>
@@ -4528,7 +4515,7 @@
         <v>276</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="M12" s="1" t="s">
         <v>130</v>
@@ -4543,7 +4530,7 @@
         <v>133</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="R12" s="1" t="s">
         <v>197</v>
@@ -4575,10 +4562,10 @@
         <v>331</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>345</v>
@@ -4599,7 +4586,7 @@
         <v>135</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="O13" s="1" t="s">
         <v>136</v>
@@ -4608,7 +4595,7 @@
         <v>137</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="R13" s="1" t="s">
         <v>198</v>
@@ -4640,10 +4627,10 @@
         <v>334</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>346</v>
@@ -4655,7 +4642,7 @@
         <v>139</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="P14" s="1" t="s">
         <v>140</v>
@@ -4684,7 +4671,7 @@
         <v>332</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>55</v>
@@ -4699,7 +4686,7 @@
         <v>143</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="Q15" s="1" t="s">
         <v>144</v>
@@ -4713,10 +4700,10 @@
     </row>
     <row r="16" spans="1:22">
       <c r="F16" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="Q16" s="1" t="s">
         <v>145</v>
@@ -4727,7 +4714,7 @@
     </row>
     <row r="17" spans="1:22">
       <c r="F17" s="1" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="N17" s="1" t="s">
         <v>146</v>
@@ -4738,10 +4725,10 @@
     </row>
     <row r="18" spans="1:22">
       <c r="F18" s="1" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="T18" s="1" t="s">
         <v>244</v>
@@ -4749,10 +4736,10 @@
     </row>
     <row r="19" spans="1:22">
       <c r="F19" s="1" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="T19" s="1" t="s">
         <v>245</v>
@@ -4763,7 +4750,7 @@
         <v>56</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="T20" s="1" t="s">
         <v>246</v>
@@ -4771,7 +4758,7 @@
     </row>
     <row r="21" spans="1:22">
       <c r="N21" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="T21" s="1" t="s">
         <v>247</v>
@@ -4779,7 +4766,7 @@
     </row>
     <row r="22" spans="1:22">
       <c r="N22" s="1" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="T22" s="1" t="s">
         <v>248</v>
@@ -4787,7 +4774,7 @@
     </row>
     <row r="23" spans="1:22">
       <c r="N23" s="1" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="T23" s="1" t="s">
         <v>249</v>
@@ -4795,7 +4782,7 @@
     </row>
     <row r="24" spans="1:22">
       <c r="N24" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="25" spans="1:22" s="5" customFormat="1"/>
@@ -5813,7 +5800,7 @@
     </row>
     <row r="64" spans="1:22">
       <c r="L64" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="65" spans="1:22">
@@ -6206,7 +6193,7 @@
         <v>308</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="J85" s="1" t="s">
         <v>112</v>
@@ -6310,55 +6297,55 @@
     </row>
     <row r="90" spans="1:22">
       <c r="B90" s="1" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="C90" s="1" t="s">
+        <v>663</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>662</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>663</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="G90" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="H90" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="I90" s="13" t="s">
         <v>665</v>
       </c>
-      <c r="D90" s="1" t="s">
-        <v>664</v>
-      </c>
-      <c r="E90" s="1" t="s">
-        <v>665</v>
-      </c>
-      <c r="F90" s="1" t="s">
-        <v>530</v>
-      </c>
-      <c r="G90" s="1" t="s">
-        <v>530</v>
-      </c>
-      <c r="H90" s="1" t="s">
+      <c r="J90" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="I90" s="13" t="s">
-        <v>667</v>
-      </c>
-      <c r="J90" s="1" t="s">
+      <c r="K90" s="3" t="s">
+        <v>531</v>
+      </c>
+      <c r="L90" s="1" t="s">
         <v>532</v>
       </c>
-      <c r="K90" s="3" t="s">
-        <v>532</v>
-      </c>
-      <c r="L90" s="1" t="s">
+      <c r="M90" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="M90" s="1" t="s">
+      <c r="N90" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="O90" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="P90" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="R90" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="U90" s="2" t="s">
         <v>534</v>
-      </c>
-      <c r="N90" s="1" t="s">
-        <v>534</v>
-      </c>
-      <c r="O90" s="1" t="s">
-        <v>534</v>
-      </c>
-      <c r="P90" s="1" t="s">
-        <v>534</v>
-      </c>
-      <c r="R90" s="1" t="s">
-        <v>532</v>
-      </c>
-      <c r="U90" s="2" t="s">
-        <v>535</v>
       </c>
     </row>
     <row r="91" spans="1:22">
@@ -6575,52 +6562,52 @@
     </row>
     <row r="95" spans="1:22">
       <c r="B95" s="1" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="J95" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="K95" s="3" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="M95" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="N95" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="O95" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="P95" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="R95" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="T95" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="V95" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="96" spans="1:22">
@@ -6825,19 +6812,19 @@
     </row>
     <row r="100" spans="1:22">
       <c r="F100" s="1" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="I100" s="1" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="R100" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="V100" s="1" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="101" spans="1:22">
@@ -6876,13 +6863,13 @@
     </row>
     <row r="103" spans="1:22">
       <c r="F103" s="1" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="I103" s="1" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="R103" s="1" t="s">
         <v>215</v>
@@ -6893,13 +6880,13 @@
     </row>
     <row r="104" spans="1:22">
       <c r="F104" s="1" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="I104" s="1" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="R104" s="1" t="s">
         <v>216</v>
@@ -7028,7 +7015,7 @@
         <v>78</v>
       </c>
       <c r="H108" s="1" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="I108" s="2"/>
       <c r="J108" s="1" t="s">

</xml_diff>

<commit_message>
documentation and comments updated
</commit_message>
<xml_diff>
--- a/data/readfiles/generate_yaml.xlsx
+++ b/data/readfiles/generate_yaml.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chughes/Documents/Git/SLiDE/data/readfiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F1D9654-558C-5749-AB3C-CCAF5B503274}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEBB17E3-D6F4-B145-951A-ED0339A455F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" xr2:uid="{3E1837C3-4AC3-0440-9699-55C5376D9610}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" activeTab="2" xr2:uid="{3E1837C3-4AC3-0440-9699-55C5376D9610}"/>
   </bookViews>
   <sheets>
     <sheet name="map_parse" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2296" uniqueCount="702">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2297" uniqueCount="703">
   <si>
     <t>bea_supply</t>
   </si>
@@ -2069,12 +2069,6 @@
     <t xml:space="preserve">  - {from: SCTG Group,  to: sctg_group}</t>
   </si>
   <si>
-    <t xml:space="preserve">  file:   ../mapsources/WiNDC/windc_build/build_files/maps/mapcfs.map</t>
-  </si>
-  <si>
-    <t># file:   [.., mapsources, WiNDC, windc_build, build_files, maps, mapcfs.map]</t>
-  </si>
-  <si>
     <t xml:space="preserve">  input:  sctg_code</t>
   </si>
   <si>
@@ -2108,18 +2102,12 @@
     <t xml:space="preserve">    output: windc_code</t>
   </si>
   <si>
-    <t># - file:   [.., mapsources, WiNDC, windc_build, build_files, maps, mapsgf.map]</t>
-  </si>
-  <si>
     <t xml:space="preserve">  - {col: units,      type: Any}</t>
   </si>
   <si>
     <t># - {col: sctg_group, type: Any}</t>
   </si>
   <si>
-    <t xml:space="preserve">  - file:   ../mapsources/WiNDC/windc_build/build_files/maps/mapsgf.map</t>
-  </si>
-  <si>
     <t xml:space="preserve">    from:   missing_1</t>
   </si>
   <si>
@@ -2142,6 +2130,21 @@
   </si>
   <si>
     <t>Map:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  file:   [.., mapsources, WiNDC, windc_build, build_files, maps, mapcfs.map]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - file:   [.., mapsources, WiNDC, windc_build, build_files, maps, mapsgf.map]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - col: value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    operation: "&lt;"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    val: 10.0</t>
   </si>
 </sst>
 </file>
@@ -2592,11 +2595,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7AB9832-7F74-B245-B43D-5B870966A3CC}">
   <dimension ref="A1:L88"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="I42" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="H71" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I55" sqref="I55"/>
+      <selection pane="bottomRight" activeCell="J80" sqref="J80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2657,37 +2660,37 @@
     <row r="3" spans="1:12" s="16" customFormat="1"/>
     <row r="4" spans="1:12">
       <c r="B4" s="15" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="J4" s="15" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
       <c r="K4" s="15" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="L4" s="15" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="16" customFormat="1"/>
@@ -2946,7 +2949,7 @@
         <v>672</v>
       </c>
       <c r="J20" s="15" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -2966,7 +2969,7 @@
         <v>671</v>
       </c>
       <c r="J21" s="15" t="s">
-        <v>698</v>
+        <v>694</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -2983,10 +2986,10 @@
         <v>567</v>
       </c>
       <c r="I22" s="15" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="J22" s="15" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -3000,15 +3003,15 @@
         <v>559</v>
       </c>
       <c r="I23" s="15" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="J23" s="15" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="J24" s="15" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
     </row>
     <row r="25" spans="1:10" s="16" customFormat="1"/>
@@ -3052,7 +3055,7 @@
         <v>675</v>
       </c>
       <c r="J27" s="15" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -3134,23 +3137,23 @@
         <v>300</v>
       </c>
       <c r="I55" s="15" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="J55" s="15" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
     </row>
     <row r="56" spans="1:10">
       <c r="I56" s="15" t="s">
-        <v>678</v>
+        <v>698</v>
       </c>
       <c r="J56" s="15" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
     </row>
     <row r="57" spans="1:10">
       <c r="I57" s="15" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="J57" s="15" t="s">
         <v>33</v>
@@ -3158,7 +3161,7 @@
     </row>
     <row r="58" spans="1:10">
       <c r="I58" s="15" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="J58" s="15" t="s">
         <v>34</v>
@@ -3166,7 +3169,7 @@
     </row>
     <row r="59" spans="1:10">
       <c r="I59" s="15" t="s">
-        <v>683</v>
+        <v>677</v>
       </c>
       <c r="J59" s="15" t="s">
         <v>174</v>
@@ -3174,43 +3177,35 @@
     </row>
     <row r="60" spans="1:10">
       <c r="I60" s="15" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="J60" s="15" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
     </row>
     <row r="61" spans="1:10">
-      <c r="I61" s="15" t="s">
-        <v>682</v>
-      </c>
       <c r="J61" s="15" t="s">
-        <v>690</v>
+        <v>699</v>
       </c>
     </row>
     <row r="62" spans="1:10">
       <c r="J62" s="15" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
     </row>
     <row r="63" spans="1:10">
       <c r="J63" s="15" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
     </row>
     <row r="64" spans="1:10">
       <c r="J64" s="15" t="s">
-        <v>695</v>
+        <v>686</v>
       </c>
     </row>
     <row r="65" spans="1:10">
       <c r="J65" s="15" t="s">
-        <v>688</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10">
-      <c r="J66" s="15" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
     </row>
     <row r="67" spans="1:10" s="16" customFormat="1"/>
@@ -3309,7 +3304,7 @@
     </row>
     <row r="80" spans="1:10">
       <c r="J80" s="15" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
     </row>
     <row r="81" spans="10:10">
@@ -3397,19 +3392,19 @@
     </row>
     <row r="2" spans="1:6">
       <c r="B2" s="2" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -4150,7 +4145,7 @@
         <v>300</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -4290,14 +4285,14 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9947295B-8D1F-FB48-972A-B6AD7BBC4112}">
-  <dimension ref="A1:V126"/>
+  <dimension ref="A1:V129"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B66" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="E98" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B33" sqref="B33"/>
       <selection pane="topRight" activeCell="B33" sqref="B33"/>
       <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
-      <selection pane="bottomRight" activeCell="B78" sqref="B78"/>
+      <selection pane="bottomRight" activeCell="F129" sqref="F129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -4409,67 +4404,67 @@
     <row r="4" spans="1:22" s="5" customFormat="1"/>
     <row r="5" spans="1:22">
       <c r="B5" s="2" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
     </row>
     <row r="6" spans="1:22" s="5" customFormat="1"/>
@@ -6437,61 +6432,61 @@
         <v>300</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="J89" s="2" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="K89" s="1" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="L89" s="1" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="M89" s="1" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="N89" s="1" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="O89" s="1" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="P89" s="1" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="R89" s="1" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="T89" s="1" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="U89" s="2" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="V89" s="1" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
     </row>
     <row r="90" spans="1:22">
@@ -7555,6 +7550,21 @@
       </c>
       <c r="I126" s="1" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="127" spans="1:22">
+      <c r="F127" s="1" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="128" spans="1:22">
+      <c r="F128" s="1" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="129" spans="6:6">
+      <c r="F129" s="1" t="s">
+        <v>701</v>
       </c>
     </row>
   </sheetData>
@@ -7688,67 +7698,67 @@
     <row r="4" spans="1:22" s="5" customFormat="1"/>
     <row r="5" spans="1:22">
       <c r="B5" s="2" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
     </row>
     <row r="6" spans="1:22" s="5" customFormat="1"/>
@@ -9716,61 +9726,61 @@
         <v>300</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="J89" s="2" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="K89" s="1" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="L89" s="1" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="M89" s="1" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="N89" s="1" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="O89" s="1" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="P89" s="1" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="R89" s="1" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="T89" s="1" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="U89" s="2" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="V89" s="1" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
     </row>
     <row r="90" spans="1:22">

</xml_diff>

<commit_message>
shorten kwarg can now specify length
</commit_message>
<xml_diff>
--- a/data/readfiles/generate_yaml.xlsx
+++ b/data/readfiles/generate_yaml.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chughes/Documents/Git/SLiDE/data/readfiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEBB17E3-D6F4-B145-951A-ED0339A455F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32327C01-5585-A545-B6A9-7977F810D6E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" activeTab="2" xr2:uid="{3E1837C3-4AC3-0440-9699-55C5376D9610}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2297" uniqueCount="703">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2294" uniqueCount="700">
   <si>
     <t>bea_supply</t>
   </si>
@@ -2136,15 +2136,6 @@
   </si>
   <si>
     <t xml:space="preserve">  - file:   [.., mapsources, WiNDC, windc_build, build_files, maps, mapsgf.map]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  - col: value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    operation: "&lt;"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    val: 10.0</t>
   </si>
 </sst>
 </file>
@@ -4285,14 +4276,14 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9947295B-8D1F-FB48-972A-B6AD7BBC4112}">
-  <dimension ref="A1:V129"/>
+  <dimension ref="A1:V126"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E98" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B33" sqref="B33"/>
       <selection pane="topRight" activeCell="B33" sqref="B33"/>
       <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
-      <selection pane="bottomRight" activeCell="F129" sqref="F129"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -7550,21 +7541,6 @@
       </c>
       <c r="I126" s="1" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="127" spans="1:22">
-      <c r="F127" s="1" t="s">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="128" spans="1:22">
-      <c r="F128" s="1" t="s">
-        <v>702</v>
-      </c>
-    </row>
-    <row r="129" spans="6:6">
-      <c r="F129" s="1" t="s">
-        <v>701</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated documentation - datastream examples
</commit_message>
<xml_diff>
--- a/data/readfiles/generate_yaml.xlsx
+++ b/data/readfiles/generate_yaml.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chughes/Documents/Git/SLiDE/data/readfiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32327C01-5585-A545-B6A9-7977F810D6E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4154836E-CC5C-0943-8883-DAE0B980712E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" activeTab="2" xr2:uid="{3E1837C3-4AC3-0440-9699-55C5376D9610}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="2" xr2:uid="{3E1837C3-4AC3-0440-9699-55C5376D9610}"/>
   </bookViews>
   <sheets>
     <sheet name="map_parse" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2294" uniqueCount="700">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2320" uniqueCount="723">
   <si>
     <t>bea_supply</t>
   </si>
@@ -2136,6 +2136,75 @@
   </si>
   <si>
     <t xml:space="preserve">  - file:   [.., mapsources, WiNDC, windc_build, build_files, maps, mapsgf.map]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  name: seds.csv</t>
+  </si>
+  <si>
+    <t>msn</t>
+  </si>
+  <si>
+    <t>PathOut: [.., data, coremaps, parse, msn.csv]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - {col: sector_desc, type: String}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - {col: source_desc, type: String}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - {col: msn_desc,    type: String}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - {col: msn_code,    type: String}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - {from: full_desc, to: msn_desc}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - {from: from,      to: msn_code}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - {from: source,    to: source_code}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - {from: sector,    to: sector_code}</t>
+  </si>
+  <si>
+    <t># Match:</t>
+  </si>
+  <si>
+    <t>#   output: ["source_code", "sector_code", "units"]</t>
+  </si>
+  <si>
+    <t>#   on:     (?&lt;source_code&gt;.{2})(?&lt;sector_code&gt;.{2})(?&lt;units&gt;.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - file:   [parse, msn.csv]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    from:   msn_code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    to:     [source_code, sector_code, units]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    output: [source_code, sector_code, units]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - {from: msn,       to: msn_code}</t>
+  </si>
+  <si>
+    <t>#   input:  msn_code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    input:  msn_code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  to:   0.0</t>
+  </si>
+  <si>
+    <t># - {col: msn,         type: String}</t>
   </si>
 </sst>
 </file>
@@ -2584,13 +2653,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7AB9832-7F74-B245-B43D-5B870966A3CC}">
-  <dimension ref="A1:L88"/>
+  <dimension ref="A1:M91"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="H71" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J80" sqref="J80"/>
+      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2598,17 +2667,17 @@
     <col min="1" max="1" width="10.83203125" style="15"/>
     <col min="2" max="3" width="93" style="15" customWidth="1"/>
     <col min="4" max="4" width="92.33203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="92.83203125" style="15" customWidth="1"/>
-    <col min="6" max="7" width="67" style="15" customWidth="1"/>
-    <col min="8" max="9" width="92.83203125" style="15" customWidth="1"/>
-    <col min="10" max="10" width="92.33203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="102" style="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="93.33203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="92.83203125" style="15" customWidth="1"/>
-    <col min="14" max="16384" width="10.83203125" style="15"/>
+    <col min="5" max="6" width="92.83203125" style="15" customWidth="1"/>
+    <col min="7" max="8" width="67" style="15" customWidth="1"/>
+    <col min="9" max="10" width="92.83203125" style="15" customWidth="1"/>
+    <col min="11" max="11" width="92.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="102" style="15" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="93.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="92.83203125" style="15" customWidth="1"/>
+    <col min="15" max="16384" width="10.83203125" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="9" customFormat="1">
+    <row r="1" spans="1:13" s="9" customFormat="1">
       <c r="B1" s="9" t="s">
         <v>648</v>
       </c>
@@ -2622,34 +2691,37 @@
         <v>385</v>
       </c>
       <c r="F1" s="9" t="s">
+        <v>701</v>
+      </c>
+      <c r="G1" s="9" t="s">
         <v>386</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>585</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>387</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="J1" s="9" t="s">
         <v>673</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="K1" s="9" t="s">
         <v>388</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>389</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="M1" s="9" t="s">
         <v>558</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:13">
       <c r="D2" s="15" t="s">
         <v>647</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="16" customFormat="1"/>
-    <row r="4" spans="1:12">
+    <row r="3" spans="1:13" s="16" customFormat="1"/>
+    <row r="4" spans="1:13">
       <c r="B4" s="15" t="s">
         <v>695</v>
       </c>
@@ -2663,10 +2735,10 @@
         <v>695</v>
       </c>
       <c r="F4" s="15" t="s">
+        <v>695</v>
+      </c>
+      <c r="G4" s="15" t="s">
         <v>696</v>
-      </c>
-      <c r="G4" s="15" t="s">
-        <v>695</v>
       </c>
       <c r="H4" s="15" t="s">
         <v>695</v>
@@ -2675,17 +2747,20 @@
         <v>695</v>
       </c>
       <c r="J4" s="15" t="s">
+        <v>695</v>
+      </c>
+      <c r="K4" s="15" t="s">
         <v>696</v>
-      </c>
-      <c r="K4" s="15" t="s">
-        <v>695</v>
       </c>
       <c r="L4" s="15" t="s">
         <v>695</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" s="16" customFormat="1"/>
-    <row r="6" spans="1:12">
+      <c r="M4" s="15" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" s="16" customFormat="1"/>
+    <row r="6" spans="1:13">
       <c r="A6" s="15" t="s">
         <v>290</v>
       </c>
@@ -2702,29 +2777,32 @@
         <v>592</v>
       </c>
       <c r="F6" s="15" t="s">
+        <v>593</v>
+      </c>
+      <c r="G6" s="15" t="s">
         <v>595</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="H6" s="15" t="s">
         <v>594</v>
       </c>
-      <c r="H6" s="15" t="s">
+      <c r="I6" s="15" t="s">
         <v>592</v>
       </c>
-      <c r="I6" s="15" t="s">
+      <c r="J6" s="15" t="s">
         <v>626</v>
       </c>
-      <c r="J6" s="15" t="s">
+      <c r="K6" s="15" t="s">
         <v>593</v>
       </c>
-      <c r="K6" s="15" t="s">
+      <c r="L6" s="15" t="s">
         <v>594</v>
       </c>
-      <c r="L6" s="15" t="s">
+      <c r="M6" s="15" t="s">
         <v>593</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="16" customFormat="1"/>
-    <row r="8" spans="1:12">
+    <row r="7" spans="1:13" s="16" customFormat="1"/>
+    <row r="8" spans="1:13">
       <c r="A8" s="15" t="s">
         <v>291</v>
       </c>
@@ -2740,30 +2818,33 @@
       <c r="E8" s="15" t="s">
         <v>596</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="17" t="s">
+        <v>702</v>
+      </c>
+      <c r="G8" s="15" t="s">
         <v>598</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="H8" s="17" t="s">
         <v>599</v>
       </c>
-      <c r="H8" s="15" t="s">
+      <c r="I8" s="15" t="s">
         <v>600</v>
       </c>
-      <c r="I8" s="17" t="s">
+      <c r="J8" s="17" t="s">
         <v>670</v>
       </c>
-      <c r="J8" s="17" t="s">
+      <c r="K8" s="17" t="s">
         <v>601</v>
       </c>
-      <c r="K8" s="17" t="s">
+      <c r="L8" s="17" t="s">
         <v>602</v>
       </c>
-      <c r="L8" s="15" t="s">
+      <c r="M8" s="15" t="s">
         <v>603</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="16" customFormat="1"/>
-    <row r="10" spans="1:12">
+    <row r="9" spans="1:13" s="16" customFormat="1"/>
+    <row r="10" spans="1:13">
       <c r="A10" s="15" t="s">
         <v>292</v>
       </c>
@@ -2779,29 +2860,32 @@
       <c r="E10" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="15" t="s">
+      <c r="F10" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="15" t="s">
         <v>128</v>
-      </c>
-      <c r="G10" s="15" t="s">
-        <v>8</v>
       </c>
       <c r="H10" s="15" t="s">
         <v>8</v>
       </c>
       <c r="I10" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="J10" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="J10" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="K10" s="15" t="s">
+      <c r="K10" s="17" t="s">
         <v>8</v>
       </c>
       <c r="L10" s="15" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="M10" s="15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="B11" s="15" t="s">
         <v>656</v>
       </c>
@@ -2815,28 +2899,31 @@
         <v>581</v>
       </c>
       <c r="F11" s="15" t="s">
+        <v>700</v>
+      </c>
+      <c r="G11" s="15" t="s">
         <v>364</v>
       </c>
-      <c r="G11" s="15" t="s">
+      <c r="H11" s="15" t="s">
         <v>586</v>
       </c>
-      <c r="H11" s="15" t="s">
+      <c r="I11" s="15" t="s">
         <v>588</v>
       </c>
-      <c r="I11" s="15" t="s">
+      <c r="J11" s="15" t="s">
         <v>666</v>
       </c>
-      <c r="J11" s="15" t="s">
+      <c r="K11" s="15" t="s">
         <v>362</v>
       </c>
-      <c r="K11" s="15" t="s">
+      <c r="L11" s="15" t="s">
         <v>369</v>
       </c>
-      <c r="L11" s="15" t="s">
+      <c r="M11" s="15" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:13">
       <c r="D12" s="15" t="s">
         <v>370</v>
       </c>
@@ -2844,63 +2931,66 @@
         <v>582</v>
       </c>
       <c r="F12" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="G12" s="15" t="s">
         <v>365</v>
       </c>
-      <c r="G12" s="15" t="s">
+      <c r="H12" s="15" t="s">
         <v>587</v>
       </c>
-      <c r="H12" s="15" t="s">
+      <c r="I12" s="15" t="s">
         <v>589</v>
       </c>
-      <c r="I12" s="15" t="s">
+      <c r="J12" s="15" t="s">
         <v>667</v>
       </c>
-      <c r="J12" s="15" t="s">
+      <c r="K12" s="15" t="s">
         <v>363</v>
       </c>
-      <c r="K12" s="15" t="s">
+      <c r="L12" s="15" t="s">
         <v>371</v>
       </c>
-      <c r="L12" s="15" t="s">
+      <c r="M12" s="15" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:13">
       <c r="E13" s="15" t="s">
         <v>583</v>
       </c>
-      <c r="F13" s="15" t="s">
+      <c r="G13" s="15" t="s">
         <v>366</v>
       </c>
-      <c r="H13" s="15" t="s">
+      <c r="I13" s="15" t="s">
         <v>590</v>
       </c>
-      <c r="I13" s="15" t="s">
+      <c r="J13" s="15" t="s">
         <v>668</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:13">
       <c r="E14" s="15" t="s">
         <v>584</v>
       </c>
-      <c r="F14" s="15" t="s">
+      <c r="G14" s="15" t="s">
         <v>367</v>
       </c>
-      <c r="H14" s="15" t="s">
+      <c r="I14" s="15" t="s">
         <v>591</v>
       </c>
-      <c r="I14" s="15" t="s">
+      <c r="J14" s="15" t="s">
         <v>669</v>
       </c>
     </row>
-    <row r="15" spans="1:12" s="16" customFormat="1"/>
-    <row r="16" spans="1:12">
+    <row r="15" spans="1:13" s="16" customFormat="1"/>
+    <row r="16" spans="1:13">
       <c r="A16" s="15" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="16" customFormat="1"/>
-    <row r="19" spans="1:10">
+    <row r="18" spans="1:11" s="16" customFormat="1"/>
+    <row r="19" spans="1:11">
       <c r="A19" s="15" t="s">
         <v>294</v>
       </c>
@@ -2916,14 +3006,17 @@
       <c r="F19" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="I19" s="15" t="s">
+      <c r="G19" s="15" t="s">
         <v>11</v>
       </c>
       <c r="J19" s="15" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="20" spans="1:10">
+      <c r="K19" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
       <c r="B20" s="15" t="s">
         <v>560</v>
       </c>
@@ -2934,16 +3027,19 @@
         <v>560</v>
       </c>
       <c r="F20" s="15" t="s">
+        <v>706</v>
+      </c>
+      <c r="G20" s="15" t="s">
         <v>203</v>
       </c>
-      <c r="I20" s="15" t="s">
+      <c r="J20" s="15" t="s">
         <v>672</v>
       </c>
-      <c r="J20" s="15" t="s">
+      <c r="K20" s="15" t="s">
         <v>693</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:11">
       <c r="B21" s="15" t="s">
         <v>561</v>
       </c>
@@ -2954,16 +3050,19 @@
         <v>561</v>
       </c>
       <c r="F21" s="15" t="s">
+        <v>705</v>
+      </c>
+      <c r="G21" s="15" t="s">
         <v>568</v>
       </c>
-      <c r="I21" s="15" t="s">
+      <c r="J21" s="15" t="s">
         <v>671</v>
       </c>
-      <c r="J21" s="15" t="s">
+      <c r="K21" s="15" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:11">
       <c r="B22" s="15" t="s">
         <v>372</v>
       </c>
@@ -2974,16 +3073,19 @@
         <v>372</v>
       </c>
       <c r="F22" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="G22" s="15" t="s">
         <v>567</v>
       </c>
-      <c r="I22" s="15" t="s">
+      <c r="J22" s="15" t="s">
         <v>679</v>
       </c>
-      <c r="J22" s="15" t="s">
+      <c r="K22" s="15" t="s">
         <v>692</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:11">
       <c r="B23" s="15" t="s">
         <v>559</v>
       </c>
@@ -2993,348 +3095,381 @@
       <c r="D23" s="15" t="s">
         <v>559</v>
       </c>
-      <c r="I23" s="15" t="s">
+      <c r="F23" s="15" t="s">
+        <v>704</v>
+      </c>
+      <c r="J23" s="15" t="s">
         <v>689</v>
       </c>
-      <c r="J23" s="15" t="s">
+      <c r="K23" s="15" t="s">
         <v>679</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
-      <c r="J24" s="15" t="s">
+    <row r="24" spans="1:11">
+      <c r="F24" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="K24" s="15" t="s">
         <v>688</v>
       </c>
     </row>
-    <row r="25" spans="1:10" s="16" customFormat="1"/>
-    <row r="26" spans="1:10">
-      <c r="A26" s="15" t="s">
+    <row r="25" spans="1:11">
+      <c r="F25" s="15" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="F26" s="15" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" s="16" customFormat="1"/>
+    <row r="29" spans="1:11">
+      <c r="A29" s="15" t="s">
         <v>295</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B29" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="15" t="s">
+      <c r="C29" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D26" s="15" t="s">
+      <c r="D29" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="F26" s="15" t="s">
+      <c r="F29" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="I26" s="15" t="s">
+      <c r="G29" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="J26" s="15" t="s">
+      <c r="J29" s="15" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="27" spans="1:10">
-      <c r="B27" s="15" t="s">
+      <c r="K29" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="B30" s="15" t="s">
         <v>562</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="C30" s="15" t="s">
         <v>562</v>
       </c>
-      <c r="D27" s="15" t="s">
+      <c r="D30" s="15" t="s">
         <v>562</v>
       </c>
-      <c r="F27" s="15" t="s">
+      <c r="F30" s="15" t="s">
+        <v>708</v>
+      </c>
+      <c r="G30" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="I27" s="15" t="s">
+      <c r="J30" s="15" t="s">
         <v>675</v>
       </c>
-      <c r="J27" s="15" t="s">
+      <c r="K30" s="15" t="s">
         <v>682</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
-      <c r="B28" s="15" t="s">
+    <row r="31" spans="1:11">
+      <c r="B31" s="15" t="s">
         <v>373</v>
       </c>
-      <c r="C28" s="15" t="s">
+      <c r="C31" s="15" t="s">
         <v>373</v>
       </c>
-      <c r="D28" s="15" t="s">
+      <c r="D31" s="15" t="s">
         <v>373</v>
       </c>
-      <c r="F28" s="15" t="s">
+      <c r="F31" s="15" t="s">
+        <v>707</v>
+      </c>
+      <c r="G31" s="15" t="s">
         <v>566</v>
       </c>
-      <c r="I28" s="15" t="s">
+      <c r="J31" s="15" t="s">
         <v>674</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
-      <c r="B29" s="15" t="s">
+    <row r="32" spans="1:11">
+      <c r="B32" s="15" t="s">
         <v>563</v>
       </c>
-      <c r="C29" s="15" t="s">
+      <c r="C32" s="15" t="s">
         <v>563</v>
       </c>
-      <c r="D29" s="15" t="s">
+      <c r="D32" s="15" t="s">
         <v>563</v>
       </c>
-      <c r="I29" s="15" t="s">
+      <c r="F32" s="15" t="s">
+        <v>709</v>
+      </c>
+      <c r="J32" s="15" t="s">
         <v>676</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="16" customFormat="1"/>
-    <row r="35" spans="1:6">
-      <c r="A35" s="15" t="s">
+    <row r="33" spans="1:7">
+      <c r="F33" s="15" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" s="16" customFormat="1"/>
+    <row r="38" spans="1:7">
+      <c r="A38" s="15" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="41" spans="1:6" s="16" customFormat="1"/>
-    <row r="42" spans="1:6">
-      <c r="A42" s="15" t="s">
+    <row r="44" spans="1:7" s="16" customFormat="1"/>
+    <row r="45" spans="1:7">
+      <c r="A45" s="15" t="s">
         <v>297</v>
       </c>
-      <c r="F42" s="15" t="s">
+      <c r="G45" s="15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
-      <c r="F43" s="15" t="s">
+    <row r="46" spans="1:7">
+      <c r="G46" s="15" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
-      <c r="F44" s="15" t="s">
+    <row r="47" spans="1:7">
+      <c r="G47" s="15" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
-      <c r="F45" s="15" t="s">
+    <row r="48" spans="1:7">
+      <c r="G48" s="15" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="46" spans="1:6" s="16" customFormat="1"/>
-    <row r="47" spans="1:6">
-      <c r="A47" s="15" t="s">
+    <row r="49" spans="1:11" s="16" customFormat="1"/>
+    <row r="50" spans="1:11">
+      <c r="A50" s="15" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="51" spans="1:10" s="16" customFormat="1"/>
-    <row r="52" spans="1:10">
-      <c r="A52" s="15" t="s">
+    <row r="54" spans="1:11" s="16" customFormat="1"/>
+    <row r="55" spans="1:11">
+      <c r="A55" s="15" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="54" spans="1:10" s="16" customFormat="1"/>
-    <row r="55" spans="1:10">
-      <c r="A55" s="15" t="s">
+    <row r="57" spans="1:11" s="16" customFormat="1"/>
+    <row r="58" spans="1:11">
+      <c r="A58" s="15" t="s">
         <v>300</v>
       </c>
-      <c r="I55" s="15" t="s">
+      <c r="J58" s="15" t="s">
         <v>697</v>
       </c>
-      <c r="J55" s="15" t="s">
+      <c r="K58" s="15" t="s">
         <v>697</v>
       </c>
     </row>
-    <row r="56" spans="1:10">
-      <c r="I56" s="15" t="s">
+    <row r="59" spans="1:11">
+      <c r="J59" s="15" t="s">
         <v>698</v>
       </c>
-      <c r="J56" s="15" t="s">
+      <c r="K59" s="15" t="s">
         <v>684</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
-      <c r="I57" s="15" t="s">
+    <row r="60" spans="1:11">
+      <c r="J60" s="15" t="s">
         <v>678</v>
       </c>
-      <c r="J57" s="15" t="s">
+      <c r="K60" s="15" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
-      <c r="I58" s="15" t="s">
+    <row r="61" spans="1:11">
+      <c r="J61" s="15" t="s">
         <v>681</v>
       </c>
-      <c r="J58" s="15" t="s">
+      <c r="K61" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="59" spans="1:10">
-      <c r="I59" s="15" t="s">
+    <row r="62" spans="1:11">
+      <c r="J62" s="15" t="s">
         <v>677</v>
       </c>
-      <c r="J59" s="15" t="s">
+      <c r="K62" s="15" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="60" spans="1:10">
-      <c r="I60" s="15" t="s">
+    <row r="63" spans="1:11">
+      <c r="J63" s="15" t="s">
         <v>680</v>
       </c>
-      <c r="J60" s="15" t="s">
+      <c r="K63" s="15" t="s">
         <v>685</v>
       </c>
     </row>
-    <row r="61" spans="1:10">
-      <c r="J61" s="15" t="s">
+    <row r="64" spans="1:11">
+      <c r="K64" s="15" t="s">
         <v>699</v>
       </c>
     </row>
-    <row r="62" spans="1:10">
-      <c r="J62" s="15" t="s">
+    <row r="65" spans="1:11">
+      <c r="K65" s="15" t="s">
         <v>690</v>
       </c>
     </row>
-    <row r="63" spans="1:10">
-      <c r="J63" s="15" t="s">
+    <row r="66" spans="1:11">
+      <c r="K66" s="15" t="s">
         <v>691</v>
       </c>
     </row>
-    <row r="64" spans="1:10">
-      <c r="J64" s="15" t="s">
+    <row r="67" spans="1:11">
+      <c r="K67" s="15" t="s">
         <v>686</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
-      <c r="J65" s="15" t="s">
+    <row r="68" spans="1:11">
+      <c r="K68" s="15" t="s">
         <v>687</v>
       </c>
     </row>
-    <row r="67" spans="1:10" s="16" customFormat="1"/>
-    <row r="68" spans="1:10">
-      <c r="A68" s="15" t="s">
+    <row r="70" spans="1:11" s="16" customFormat="1"/>
+    <row r="71" spans="1:11">
+      <c r="A71" s="15" t="s">
         <v>301</v>
       </c>
-      <c r="B68" s="15" t="s">
+      <c r="B71" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="C68" s="15" t="s">
+      <c r="C71" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="D68" s="15" t="s">
+      <c r="D71" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="F68" s="15" t="s">
+      <c r="G71" s="15" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="69" spans="1:10">
-      <c r="B69" s="15" t="s">
+    <row r="72" spans="1:11">
+      <c r="B72" s="15" t="s">
         <v>663</v>
       </c>
-      <c r="C69" s="15" t="s">
+      <c r="C72" s="15" t="s">
         <v>663</v>
       </c>
-      <c r="D69" s="15" t="s">
+      <c r="D72" s="15" t="s">
         <v>663</v>
       </c>
-      <c r="F69" s="15" t="s">
+      <c r="G72" s="15" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
-      <c r="B70" s="15" t="s">
+    <row r="73" spans="1:11">
+      <c r="B73" s="15" t="s">
         <v>664</v>
       </c>
-      <c r="C70" s="15" t="s">
+      <c r="C73" s="15" t="s">
         <v>664</v>
       </c>
-      <c r="D70" s="15" t="s">
+      <c r="D73" s="15" t="s">
         <v>664</v>
       </c>
-      <c r="F70" s="15" t="s">
+      <c r="G73" s="15" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="71" spans="1:10">
-      <c r="B71" s="15" t="s">
+    <row r="74" spans="1:11">
+      <c r="B74" s="15" t="s">
         <v>665</v>
       </c>
-      <c r="C71" s="15" t="s">
+      <c r="C74" s="15" t="s">
         <v>665</v>
       </c>
-      <c r="D71" s="15" t="s">
+      <c r="D74" s="15" t="s">
         <v>665</v>
       </c>
-      <c r="F71" s="15" t="s">
+      <c r="G74" s="15" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="72" spans="1:10">
-      <c r="F72" s="15" t="s">
+    <row r="75" spans="1:11">
+      <c r="G75" s="15" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="73" spans="1:10">
-      <c r="F73" s="15" t="s">
+    <row r="76" spans="1:11">
+      <c r="G76" s="15" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="74" spans="1:10">
-      <c r="F74" s="15" t="s">
+    <row r="77" spans="1:11">
+      <c r="G77" s="15" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="75" spans="1:10">
-      <c r="F75" s="15" t="s">
+    <row r="78" spans="1:11">
+      <c r="G78" s="15" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="76" spans="1:10">
-      <c r="F76" s="15" t="s">
+    <row r="79" spans="1:11">
+      <c r="G79" s="15" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="78" spans="1:10" s="16" customFormat="1"/>
-    <row r="79" spans="1:10">
-      <c r="A79" s="15" t="s">
+    <row r="81" spans="1:11" s="16" customFormat="1"/>
+    <row r="82" spans="1:11">
+      <c r="A82" s="15" t="s">
         <v>302</v>
       </c>
-      <c r="J79" s="15" t="s">
+      <c r="K82" s="15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="80" spans="1:10">
-      <c r="J80" s="15" t="s">
+    <row r="83" spans="1:11">
+      <c r="K83" s="15" t="s">
         <v>683</v>
       </c>
     </row>
-    <row r="81" spans="10:10">
-      <c r="J81" s="15" t="s">
+    <row r="84" spans="1:11">
+      <c r="K84" s="15" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="82" spans="10:10">
-      <c r="J82" s="15" t="s">
+    <row r="85" spans="1:11">
+      <c r="K85" s="15" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="83" spans="10:10">
-      <c r="J83" s="15" t="s">
+    <row r="86" spans="1:11">
+      <c r="K86" s="15" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="84" spans="10:10">
-      <c r="J84" s="15" t="s">
+    <row r="87" spans="1:11">
+      <c r="K87" s="15" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="85" spans="10:10">
-      <c r="J85" s="15" t="s">
+    <row r="88" spans="1:11">
+      <c r="K88" s="15" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="86" spans="10:10">
-      <c r="J86" s="15" t="s">
+    <row r="89" spans="1:11">
+      <c r="K89" s="15" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="87" spans="10:10">
-      <c r="J87" s="15" t="s">
+    <row r="90" spans="1:11">
+      <c r="K90" s="15" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="88" spans="10:10">
-      <c r="J88" s="15" t="s">
+    <row r="91" spans="1:11">
+      <c r="K91" s="15" t="s">
         <v>46</v>
       </c>
     </row>
@@ -4279,11 +4414,11 @@
   <dimension ref="A1:V126"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B33" sqref="B33"/>
       <selection pane="topRight" activeCell="B33" sqref="B33"/>
       <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="V37" sqref="V37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -5305,7 +5440,7 @@
         <v>256</v>
       </c>
       <c r="V32" s="1" t="s">
-        <v>219</v>
+        <v>722</v>
       </c>
     </row>
     <row r="33" spans="2:22">
@@ -5512,7 +5647,7 @@
         <v>205</v>
       </c>
       <c r="V36" s="1" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
     </row>
     <row r="37" spans="2:22">
@@ -5920,7 +6055,7 @@
         <v>208</v>
       </c>
       <c r="V57" s="1" t="s">
-        <v>225</v>
+        <v>718</v>
       </c>
     </row>
     <row r="58" spans="1:22">
@@ -5940,6 +6075,9 @@
         <v>160</v>
       </c>
       <c r="S58" s="2"/>
+      <c r="V58" s="1" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="59" spans="1:22">
       <c r="F59" s="1" t="s">
@@ -6030,7 +6168,7 @@
         <v>25</v>
       </c>
       <c r="V70" s="1" t="s">
-        <v>25</v>
+        <v>711</v>
       </c>
     </row>
     <row r="71" spans="1:22">
@@ -6051,7 +6189,7 @@
         <v>209</v>
       </c>
       <c r="V71" s="1" t="s">
-        <v>226</v>
+        <v>713</v>
       </c>
     </row>
     <row r="72" spans="1:22">
@@ -6072,7 +6210,7 @@
         <v>210</v>
       </c>
       <c r="V72" s="1" t="s">
-        <v>227</v>
+        <v>719</v>
       </c>
     </row>
     <row r="73" spans="1:22">
@@ -6093,7 +6231,7 @@
         <v>211</v>
       </c>
       <c r="V73" s="1" t="s">
-        <v>228</v>
+        <v>712</v>
       </c>
     </row>
     <row r="74" spans="1:22">
@@ -6532,6 +6670,9 @@
       <c r="U90" s="2" t="s">
         <v>529</v>
       </c>
+      <c r="V90" s="1" t="s">
+        <v>714</v>
+      </c>
     </row>
     <row r="91" spans="1:22">
       <c r="B91" s="1" t="s">
@@ -6585,6 +6726,9 @@
       <c r="U91" s="2" t="s">
         <v>164</v>
       </c>
+      <c r="V91" s="1" t="s">
+        <v>715</v>
+      </c>
     </row>
     <row r="92" spans="1:22">
       <c r="B92" s="1" t="s">
@@ -6638,6 +6782,9 @@
       <c r="U92" s="2" t="s">
         <v>165</v>
       </c>
+      <c r="V92" s="1" t="s">
+        <v>716</v>
+      </c>
     </row>
     <row r="93" spans="1:22">
       <c r="B93" s="1" t="s">
@@ -6691,6 +6838,9 @@
       <c r="U93" s="2" t="s">
         <v>269</v>
       </c>
+      <c r="V93" s="1" t="s">
+        <v>720</v>
+      </c>
     </row>
     <row r="94" spans="1:22">
       <c r="B94" s="1" t="s">
@@ -6744,6 +6894,9 @@
       <c r="U94" s="2" t="s">
         <v>270</v>
       </c>
+      <c r="V94" s="1" t="s">
+        <v>717</v>
+      </c>
     </row>
     <row r="95" spans="1:22">
       <c r="B95" s="1" t="s">
@@ -7009,7 +7162,7 @@
         <v>525</v>
       </c>
       <c r="V100" s="1" t="s">
-        <v>530</v>
+        <v>654</v>
       </c>
     </row>
     <row r="101" spans="1:22">
@@ -7026,7 +7179,7 @@
         <v>33</v>
       </c>
       <c r="V101" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="102" spans="1:22">
@@ -7043,7 +7196,7 @@
         <v>34</v>
       </c>
       <c r="V102" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="103" spans="1:22">
@@ -7060,7 +7213,7 @@
         <v>214</v>
       </c>
       <c r="V103" s="1" t="s">
-        <v>41</v>
+        <v>657</v>
       </c>
     </row>
     <row r="104" spans="1:22">
@@ -7077,7 +7230,7 @@
         <v>215</v>
       </c>
       <c r="V104" s="1" t="s">
-        <v>42</v>
+        <v>658</v>
       </c>
     </row>
     <row r="105" spans="1:22" s="5" customFormat="1"/>
@@ -7273,7 +7426,7 @@
         <v>182</v>
       </c>
       <c r="V109" s="1" t="s">
-        <v>182</v>
+        <v>721</v>
       </c>
     </row>
     <row r="110" spans="1:22">

</xml_diff>

<commit_message>
FileInput <: Check struct to compare files
</commit_message>
<xml_diff>
--- a/data/readfiles/generate_yaml.xlsx
+++ b/data/readfiles/generate_yaml.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chughes/Documents/Git/SLiDE/data/readfiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABEF7497-0510-A846-BC7C-DC279B21E6DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93CCC5F1-4034-C64F-B405-82DEA2840693}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23600" yWindow="0" windowWidth="10000" windowHeight="21000" activeTab="2" xr2:uid="{3E1837C3-4AC3-0440-9699-55C5376D9610}"/>
   </bookViews>
@@ -4908,11 +4908,11 @@
   <dimension ref="A1:V143"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B31" sqref="B31"/>
       <selection pane="topRight" activeCell="B31" sqref="B31"/>
       <selection pane="bottomLeft" activeCell="B31" sqref="B31"/>
-      <selection pane="bottomRight" activeCell="I35" sqref="I35"/>
+      <selection pane="bottomRight" activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -6100,7 +6100,7 @@
         <v>14</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>14</v>
+        <v>774</v>
       </c>
       <c r="J35" s="2" t="s">
         <v>78</v>

</xml_diff>

<commit_message>
fixed bug in load_from
</commit_message>
<xml_diff>
--- a/data/readfiles/generate_yaml.xlsx
+++ b/data/readfiles/generate_yaml.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chughes/Documents/Git/SLiDE/data/readfiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{964CE547-9CD0-1B42-923E-C7C639CEC783}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9D012F-2400-E94E-A691-B51CED9346F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" activeTab="3" xr2:uid="{3E1837C3-4AC3-0440-9699-55C5376D9610}"/>
+    <workbookView xWindow="-2640" yWindow="-21600" windowWidth="38400" windowHeight="21600" activeTab="3" xr2:uid="{3E1837C3-4AC3-0440-9699-55C5376D9610}"/>
   </bookViews>
   <sheets>
     <sheet name="map_bluenote" sheetId="5" r:id="rId1"/>
@@ -2724,7 +2724,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="29">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -5019,7 +5029,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="N59:N63">
-    <cfRule type="containsText" dxfId="27" priority="1" operator="containsText" text="col: units">
+    <cfRule type="containsText" dxfId="28" priority="1" operator="containsText" text="col: units">
       <formula>NOT(ISERROR(SEARCH("col: units",N59)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5963,11 +5973,11 @@
   <dimension ref="A1:X144"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B31" sqref="B31"/>
       <selection pane="topRight" activeCell="B31" sqref="B31"/>
       <selection pane="bottomLeft" activeCell="B31" sqref="B31"/>
-      <selection pane="bottomRight" activeCell="C32" sqref="C32:E32"/>
+      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -10114,132 +10124,132 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="X90:XFD91 J40:K46 J48:K48 J50:K57 A105:E109 S105:W109 N173:XFD178 U110:XFD114 M37:M39 Y105:XFD109 N41:XFD44 S30:XFD40 Z134:XFD136 X127:XFD127 S131:XFD133 J138:K138 J139:J141 M1:XFD29 M92:XFD104 M30:M35 M127:V127 M115:XFD126 M134:X136 M131:M133 M137:XFD172 M45:XFD89 M110:S114 M179:XFD1048576 M90:V91 A39:I46 A47:H47 A48:I57 A37:K38 A145:K1048576 A138:H141 A142:J144 J100:J104 G105:K109 A95:I104 J95:K99 A58:K93 A94:J94 L50:L93 L105:L138 K94:K104 A110:K128 K129:K131 A132:K137 A129:I131 M128:R130 T128:XFD130 S129:S131 A1:K29 F30:K32 F33:J33 A30:B36 F34:K36">
-    <cfRule type="containsText" dxfId="26" priority="40" operator="containsText" text="col: units">
+    <cfRule type="containsText" dxfId="27" priority="40" operator="containsText" text="col: units">
       <formula>NOT(ISERROR(SEARCH("col: units",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W90:W91">
-    <cfRule type="containsText" dxfId="25" priority="39" operator="containsText" text="col: units">
+    <cfRule type="containsText" dxfId="26" priority="39" operator="containsText" text="col: units">
       <formula>NOT(ISERROR(SEARCH("col: units",W90)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X105:X109">
-    <cfRule type="containsText" dxfId="24" priority="35" operator="containsText" text="col: units">
+    <cfRule type="containsText" dxfId="25" priority="35" operator="containsText" text="col: units">
       <formula>NOT(ISERROR(SEARCH("col: units",X105)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M105:M109">
-    <cfRule type="containsText" dxfId="23" priority="37" operator="containsText" text="col: units">
+    <cfRule type="containsText" dxfId="24" priority="37" operator="containsText" text="col: units">
       <formula>NOT(ISERROR(SEARCH("col: units",M105)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T110:T114">
-    <cfRule type="containsText" dxfId="22" priority="36" operator="containsText" text="col: units">
+    <cfRule type="containsText" dxfId="23" priority="36" operator="containsText" text="col: units">
       <formula>NOT(ISERROR(SEARCH("col: units",T110)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F105:F109">
-    <cfRule type="containsText" dxfId="21" priority="34" operator="containsText" text="col: units">
+    <cfRule type="containsText" dxfId="22" priority="34" operator="containsText" text="col: units">
       <formula>NOT(ISERROR(SEARCH("col: units",F105)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N105:N109">
-    <cfRule type="containsText" dxfId="20" priority="32" operator="containsText" text="col: units">
+    <cfRule type="containsText" dxfId="21" priority="32" operator="containsText" text="col: units">
       <formula>NOT(ISERROR(SEARCH("col: units",N105)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N34:N37 N30:N31">
-    <cfRule type="containsText" dxfId="19" priority="19" operator="containsText" text="col: units">
+    <cfRule type="containsText" dxfId="20" priority="19" operator="containsText" text="col: units">
       <formula>NOT(ISERROR(SEARCH("col: units",N30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O105:O109">
-    <cfRule type="containsText" dxfId="18" priority="30" operator="containsText" text="col: units">
+    <cfRule type="containsText" dxfId="19" priority="30" operator="containsText" text="col: units">
       <formula>NOT(ISERROR(SEARCH("col: units",O105)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q34:Q37 Q30:Q31">
-    <cfRule type="containsText" dxfId="17" priority="16" operator="containsText" text="col: units">
+    <cfRule type="containsText" dxfId="18" priority="16" operator="containsText" text="col: units">
       <formula>NOT(ISERROR(SEARCH("col: units",Q30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P34:P37 P30:P31">
-    <cfRule type="containsText" dxfId="16" priority="28" operator="containsText" text="col: units">
+    <cfRule type="containsText" dxfId="17" priority="28" operator="containsText" text="col: units">
       <formula>NOT(ISERROR(SEARCH("col: units",P30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P105:P109">
-    <cfRule type="containsText" dxfId="15" priority="26" operator="containsText" text="col: units">
+    <cfRule type="containsText" dxfId="16" priority="26" operator="containsText" text="col: units">
       <formula>NOT(ISERROR(SEARCH("col: units",P105)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q105:Q109">
-    <cfRule type="containsText" dxfId="14" priority="25" operator="containsText" text="col: units">
+    <cfRule type="containsText" dxfId="15" priority="25" operator="containsText" text="col: units">
       <formula>NOT(ISERROR(SEARCH("col: units",Q105)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R105:R109">
-    <cfRule type="containsText" dxfId="13" priority="24" operator="containsText" text="col: units">
+    <cfRule type="containsText" dxfId="14" priority="24" operator="containsText" text="col: units">
       <formula>NOT(ISERROR(SEARCH("col: units",R105)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O34:O37 O30:O31">
-    <cfRule type="containsText" dxfId="12" priority="22" operator="containsText" text="col: units">
+    <cfRule type="containsText" dxfId="13" priority="22" operator="containsText" text="col: units">
       <formula>NOT(ISERROR(SEARCH("col: units",O30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R34:R37 R30:R31">
-    <cfRule type="containsText" dxfId="11" priority="13" operator="containsText" text="col: units">
+    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="col: units">
       <formula>NOT(ISERROR(SEARCH("col: units",R30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N38:R40">
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="col: units">
+    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="col: units">
       <formula>NOT(ISERROR(SEARCH("col: units",N38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K139:K144">
-    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="col: units">
+    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="col: units">
       <formula>NOT(ISERROR(SEARCH("col: units",K139)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L40:L46 L48 L34:L38 L145:L1048576 L1:L32">
-    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="col: units">
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="col: units">
       <formula>NOT(ISERROR(SEARCH("col: units",L1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L139:L144">
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="col: units">
+    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="col: units">
       <formula>NOT(ISERROR(SEARCH("col: units",L139)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J133">
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="col: units">
+    <cfRule type="containsText" dxfId="7" priority="6" operator="containsText" text="col: units">
       <formula>NOT(ISERROR(SEARCH("col: units",J133)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C31 C35:C36 C33">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="col: units">
+    <cfRule type="containsText" dxfId="6" priority="5" operator="containsText" text="col: units">
       <formula>NOT(ISERROR(SEARCH("col: units",C30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30:D31 D35:D36 D33">
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="col: units">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="col: units">
       <formula>NOT(ISERROR(SEARCH("col: units",D30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30:E31 E35:E36 E33">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="col: units">
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="col: units">
       <formula>NOT(ISERROR(SEARCH("col: units",E30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34:E34">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="col: units">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="col: units">
       <formula>NOT(ISERROR(SEARCH("col: units",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32:E32">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="col: units">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="col: units">
       <formula>NOT(ISERROR(SEARCH("col: units",C32)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10256,7 +10266,7 @@
       <selection activeCell="B31" sqref="B31"/>
       <selection pane="topRight" activeCell="B31" sqref="B31"/>
       <selection pane="bottomLeft" activeCell="B31" sqref="B31"/>
-      <selection pane="bottomRight" activeCell="B30" sqref="B30"/>
+      <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -10537,7 +10547,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A39:A57 D134:XFD136 A33 B40:B46 B48 B50:B57 A58:XFD133 A34:B38 A134:B136 A30:B32 A137:XFD1048576 C30:XFD57 A1:XFD29">
-    <cfRule type="containsText" dxfId="2" priority="17" operator="containsText" text="col: units">
+    <cfRule type="containsText" dxfId="3" priority="17" operator="containsText" text="col: units">
       <formula>NOT(ISERROR(SEARCH("col: units",A1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
run data/buildstreams in one file
</commit_message>
<xml_diff>
--- a/data/readfiles/generate_yaml.xlsx
+++ b/data/readfiles/generate_yaml.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chughes/Documents/Git/SLiDE/data/readfiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5471376C-6FC8-7844-8418-FB27C71B8166}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16C9A016-C4F6-124A-A861-E266A1C10CBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="1" xr2:uid="{3E1837C3-4AC3-0440-9699-55C5376D9610}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" activeTab="3" xr2:uid="{3E1837C3-4AC3-0440-9699-55C5376D9610}"/>
   </bookViews>
   <sheets>
     <sheet name="map_bluenote" sheetId="5" r:id="rId1"/>
@@ -3965,12 +3965,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7AB9832-7F74-B245-B43D-5B870966A3CC}">
   <dimension ref="A1:N92"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B31" sqref="B31"/>
       <selection pane="topRight" activeCell="B31" sqref="B31"/>
       <selection pane="bottomLeft" activeCell="B31" sqref="B31"/>
-      <selection pane="bottomRight" activeCell="N21" sqref="N21"/>
+      <selection pane="bottomRight" activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -4916,11 +4916,11 @@
   <dimension ref="A1:F95"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B55" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B31" sqref="B31"/>
       <selection pane="topRight" activeCell="B31" sqref="B31"/>
       <selection pane="bottomLeft" activeCell="B31" sqref="B31"/>
-      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomRight" activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="93" defaultRowHeight="14"/>
@@ -5969,12 +5969,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9947295B-8D1F-FB48-972A-B6AD7BBC4112}">
   <dimension ref="A1:X145"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F9" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="L108" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B31" sqref="B31"/>
       <selection pane="topRight" activeCell="B31" sqref="B31"/>
       <selection pane="bottomLeft" activeCell="B31" sqref="B31"/>
-      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomRight" activeCell="M119" sqref="M119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -11345,7 +11345,7 @@
         <v>483</v>
       </c>
       <c r="L145" s="1" t="str">
-        <f t="shared" ref="L145:L146" si="35">IF(ISBLANK($K145), "", $K145)</f>
+        <f t="shared" ref="L145" si="35">IF(ISBLANK($K145), "", $K145)</f>
         <v xml:space="preserve">  output: value</v>
       </c>
       <c r="M145" s="1" t="s">
@@ -11379,32 +11379,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="expression" dxfId="0" priority="7">
+    <cfRule type="expression" dxfId="5" priority="7">
       <formula>_xlfn.ISFORMULA(A1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G63:G67">
-    <cfRule type="expression" dxfId="5" priority="5">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>_xlfn.ISFORMULA(G63)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G30:G31">
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>_xlfn.ISFORMULA(G30)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G26:G27">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>_xlfn.ISFORMULA(G26)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G33:G58">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>_xlfn.ISFORMULA(G33)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M32">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>_xlfn.ISFORMULA(M32)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
added comments, fixed bug in scale/naics parsing
</commit_message>
<xml_diff>
--- a/data/readfiles/generate_yaml.xlsx
+++ b/data/readfiles/generate_yaml.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chughes/Documents/Git/SLiDE/data/readfiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B8C3F9-6210-1D47-9178-3BBA4CC245D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C5F90EE-ED05-4E49-9169-9E61A924DA53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" activeTab="3" xr2:uid="{3E1837C3-4AC3-0440-9699-55C5376D9610}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="1" xr2:uid="{3E1837C3-4AC3-0440-9699-55C5376D9610}"/>
   </bookViews>
   <sheets>
     <sheet name="map_bluenote" sheetId="5" r:id="rId1"/>
@@ -3208,8 +3208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{146E3C27-1365-884B-A69E-493300A2017A}">
   <dimension ref="A1:I86"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A46" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C70" sqref="C70"/>
+    <sheetView showGridLines="0" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -3965,12 +3965,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7AB9832-7F74-B245-B43D-5B870966A3CC}">
   <dimension ref="A1:N92"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="F60" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B31" sqref="B31"/>
       <selection pane="topRight" activeCell="B31" sqref="B31"/>
       <selection pane="bottomLeft" activeCell="B31" sqref="B31"/>
-      <selection pane="bottomRight" activeCell="M18" sqref="M18"/>
+      <selection pane="bottomRight" activeCell="G76" sqref="G76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -4916,11 +4916,11 @@
   <dimension ref="A1:F95"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B55" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B31" sqref="B31"/>
       <selection pane="topRight" activeCell="B31" sqref="B31"/>
       <selection pane="bottomLeft" activeCell="B31" sqref="B31"/>
-      <selection pane="bottomRight" activeCell="B61" sqref="B61"/>
+      <selection pane="bottomRight" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="93" defaultRowHeight="14"/>
@@ -5969,12 +5969,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9947295B-8D1F-FB48-972A-B6AD7BBC4112}">
   <dimension ref="A1:X145"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="T128" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B31" sqref="B31"/>
       <selection pane="topRight" activeCell="B31" sqref="B31"/>
       <selection pane="bottomLeft" activeCell="B31" sqref="B31"/>
-      <selection pane="bottomRight" activeCell="U14" sqref="U14"/>
+      <selection pane="bottomRight" activeCell="T144" sqref="T144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>

</xml_diff>

<commit_message>
working after update to 1.4
</commit_message>
<xml_diff>
--- a/data/readfiles/generate_yaml.xlsx
+++ b/data/readfiles/generate_yaml.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chughes/Documents/Git/SLiDE/data/readfiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CB5F243-59A3-BD4D-B0DA-306257EDDB20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{613A85E9-27E1-0E4B-A614-5083461B4A8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="5" xr2:uid="{ECEEE8D6-CC61-454D-945D-45D0FFF64D45}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18900" activeTab="3" xr2:uid="{ECEEE8D6-CC61-454D-945D-45D0FFF64D45}"/>
   </bookViews>
   <sheets>
     <sheet name="map_bluenote" sheetId="5" state="hidden" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2911" uniqueCount="1108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2911" uniqueCount="1107">
   <si>
     <t>bea_supply</t>
   </si>
@@ -3342,9 +3342,6 @@
   </si>
   <si>
     <t>PathOut: [data, coremaps, crosswalk, pce.csv]</t>
-  </si>
-  <si>
-    <t>PathIn:  [data, mapso\urces, WiNDC, windc_build, build_files, maps]</t>
   </si>
   <si>
     <t xml:space="preserve">  - {col: sctg_code,         type: String}</t>
@@ -3616,14 +3613,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="50">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="39">
     <dxf>
       <font>
         <color theme="9"/>
@@ -3681,6 +3671,13 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3974,107 +3971,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -7582,12 +7478,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCC9497B-7600-374B-8989-8C7FAD24A60F}">
   <dimension ref="A1:H90"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B10" sqref="B10"/>
       <selection pane="topRight" activeCell="B10" sqref="B10"/>
       <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
-      <selection pane="bottomRight" activeCell="B35" sqref="B35"/>
+      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="40.83203125" defaultRowHeight="13" customHeight="1"/>
@@ -7699,7 +7595,7 @@
         <v>865</v>
       </c>
       <c r="D7" s="43" t="s">
-        <v>1101</v>
+        <v>853</v>
       </c>
       <c r="E7" s="33" t="s">
         <v>852</v>
@@ -7951,7 +7847,7 @@
         <v>972</v>
       </c>
       <c r="F22" s="44" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="G22" s="43" t="s">
         <v>973</v>
@@ -7966,7 +7862,7 @@
         <v>1047</v>
       </c>
       <c r="F23" s="44" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="13" customHeight="1">
@@ -7987,7 +7883,7 @@
         <v>1075</v>
       </c>
       <c r="F25" s="43" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="13" customHeight="1">
@@ -8004,14 +7900,14 @@
       <c r="A27" s="42"/>
       <c r="E27" s="44"/>
       <c r="F27" s="44" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="13" customHeight="1">
       <c r="A28" s="42"/>
       <c r="E28" s="44"/>
       <c r="F28" s="44" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="13" customHeight="1">
@@ -9411,12 +9307,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9947295B-8D1F-FB48-972A-B6AD7BBC4112}">
   <dimension ref="A1:X147"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="U72" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B10" sqref="B10"/>
       <selection pane="topRight" activeCell="B10" sqref="B10"/>
       <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
-      <selection pane="bottomRight" activeCell="W110" sqref="W110"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="46.83203125" defaultRowHeight="13" customHeight="1"/>
@@ -14312,7 +14208,7 @@
         <v>658</v>
       </c>
       <c r="J131" s="36" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="M131" s="36" t="s">
         <v>823</v>
@@ -15140,7 +15036,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X38:X40">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="6" priority="1">
       <formula>AND(COUNTA($A39:$Z39)=0, NOT(ISBLANK($A40)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20556,32 +20452,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="expression" dxfId="6" priority="6">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>_xlfn.ISFORMULA(A1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G63:G67">
-    <cfRule type="expression" dxfId="5" priority="5">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>_xlfn.ISFORMULA(G63)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G30:G31">
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>_xlfn.ISFORMULA(G30)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G26:G27">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>_xlfn.ISFORMULA(G26)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G33:G58">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>_xlfn.ISFORMULA(G33)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M32">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>_xlfn.ISFORMULA(M32)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
CFS, PCE, GSP, UTD sharing complete; SGF sharing TBD
</commit_message>
<xml_diff>
--- a/data/readfiles/generate_yaml.xlsx
+++ b/data/readfiles/generate_yaml.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chughes/Documents/Git/SLiDE/data/readfiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41149EE2-764A-2042-AD7E-6556B1334D33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C2BF313-1118-204F-9E30-84D6C8301A13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18900" activeTab="5" xr2:uid="{ECEEE8D6-CC61-454D-945D-45D0FFF64D45}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18900" activeTab="6" xr2:uid="{ECEEE8D6-CC61-454D-945D-45D0FFF64D45}"/>
   </bookViews>
   <sheets>
     <sheet name="map_bluenote" sheetId="5" state="hidden" r:id="rId1"/>
@@ -19,7 +19,8 @@
     <sheet name="map_crosswalk" sheetId="7" r:id="rId4"/>
     <sheet name="map_experiment" sheetId="8" state="hidden" r:id="rId5"/>
     <sheet name="parse" sheetId="4" r:id="rId6"/>
-    <sheet name="parse (2)" sheetId="6" state="hidden" r:id="rId7"/>
+    <sheet name="share" sheetId="10" r:id="rId7"/>
+    <sheet name="parse (2)" sheetId="6" state="hidden" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2973" uniqueCount="1142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3080" uniqueCount="1178">
   <si>
     <t>bea_supply</t>
   </si>
@@ -3465,6 +3466,114 @@
   </si>
   <si>
     <t xml:space="preserve">  from: [missing, ...]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  name:  cfs_state.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  name:  gsp_state.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  name:  pce.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  name:  sgf.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  name:  utd.csv</t>
+  </si>
+  <si>
+    <t>cfs</t>
+  </si>
+  <si>
+    <t>utd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    from:   gsp_code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    input:  si</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    output: s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    kind:   inner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  input:  [yr, r, gdpcat, s, units]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    input:  sg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    output: g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  input:  [orig_state, dest_state, g, units]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  col: g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  val: missing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - file:   [crosswalk, pce.csv]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    from:   pg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    to:     g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    input:  pg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  input:  [yr, r, g, units]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - file:   [crosswalk, naics.csv]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    input:  n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  col: share</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  val: 0.0</t>
+  </si>
+  <si>
+    <t>PathOut: [data, share, cfs.csv]</t>
+  </si>
+  <si>
+    <t>PathOut: [data, share, pce.csv]</t>
+  </si>
+  <si>
+    <t>PathOut: [data, share, gsp.csv]</t>
+  </si>
+  <si>
+    <t>PathOut: [data, share, sgf.csv]</t>
+  </si>
+  <si>
+    <t>PathOut: [data, share, utd.csv]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  input:  [yr, r, s, t, units]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - {col: value, type: String}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - {col: g,     type: String}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - {col: t,     type: String}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - {col: s,     type: String}</t>
   </si>
 </sst>
 </file>
@@ -3718,7 +3827,48 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="33">
+  <dxfs count="49">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="9"/>
@@ -3766,6 +3916,92 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -6030,15 +6266,15 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="32" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="1" operator="equal">
       <formula>" "</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="3">
+    <cfRule type="expression" dxfId="47" priority="3">
       <formula>_xlfn.ISFORMULA(A1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:XFD1048576">
-    <cfRule type="expression" dxfId="30" priority="2">
+    <cfRule type="expression" dxfId="46" priority="2">
       <formula>AND(ISBLANK($A2), NOT(ISBLANK($A3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7418,15 +7654,15 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="29" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="2" operator="equal">
       <formula>" "</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="56">
+    <cfRule type="expression" dxfId="44" priority="56">
       <formula>_xlfn.ISFORMULA(A1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:XFD1048576">
-    <cfRule type="expression" dxfId="27" priority="3">
+    <cfRule type="expression" dxfId="43" priority="3">
       <formula>AND(ISBLANK($A2), NOT(ISBLANK($A3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7440,11 +7676,11 @@
   <dimension ref="A1:H90"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B10" sqref="B10"/>
       <selection pane="topRight" activeCell="B10" sqref="B10"/>
       <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
-      <selection pane="bottomRight" activeCell="H12" sqref="H12"/>
+      <selection pane="bottomRight" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="40.83203125" defaultRowHeight="13" customHeight="1"/>
@@ -8471,15 +8707,15 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="26" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="1" operator="equal">
       <formula>" "</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="36">
+    <cfRule type="expression" dxfId="41" priority="36">
       <formula>_xlfn.ISFORMULA(A1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:XFD1048576">
-    <cfRule type="expression" dxfId="24" priority="2">
+    <cfRule type="expression" dxfId="40" priority="2">
       <formula>AND(ISBLANK($A3), NOT(ISBLANK($A4)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9186,77 +9422,77 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D81:D83">
-    <cfRule type="expression" dxfId="23" priority="5">
+    <cfRule type="expression" dxfId="39" priority="5">
       <formula>_xlfn.ISFORMULA(D81)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:C7">
-    <cfRule type="expression" dxfId="22" priority="16">
+    <cfRule type="expression" dxfId="38" priority="16">
       <formula>_xlfn.ISFORMULA(C6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18:E22">
-    <cfRule type="expression" dxfId="21" priority="15">
+    <cfRule type="expression" dxfId="37" priority="15">
       <formula>_xlfn.ISFORMULA(E18)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:C31">
-    <cfRule type="expression" dxfId="20" priority="14">
+    <cfRule type="expression" dxfId="36" priority="14">
       <formula>_xlfn.ISFORMULA(C28)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C82:C84">
-    <cfRule type="expression" dxfId="19" priority="13">
+    <cfRule type="expression" dxfId="35" priority="13">
       <formula>_xlfn.ISFORMULA(C82)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="expression" dxfId="18" priority="11">
+    <cfRule type="expression" dxfId="34" priority="11">
       <formula>_xlfn.ISFORMULA(D7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="expression" dxfId="17" priority="12">
+    <cfRule type="expression" dxfId="33" priority="12">
       <formula>_xlfn.ISFORMULA(D6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9:D13">
-    <cfRule type="expression" dxfId="16" priority="10">
+    <cfRule type="expression" dxfId="32" priority="10">
       <formula>_xlfn.ISFORMULA(D9)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32">
-    <cfRule type="expression" dxfId="15" priority="9">
+    <cfRule type="expression" dxfId="31" priority="9">
       <formula>_xlfn.ISFORMULA(D32)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D28 D32">
-    <cfRule type="expression" dxfId="14" priority="8">
+    <cfRule type="expression" dxfId="30" priority="8">
       <formula>_xlfn.ISFORMULA(D28)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30">
-    <cfRule type="expression" dxfId="13" priority="7">
+    <cfRule type="expression" dxfId="29" priority="7">
       <formula>_xlfn.ISFORMULA(D30)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9:C10">
-    <cfRule type="expression" dxfId="12" priority="4">
+    <cfRule type="expression" dxfId="28" priority="4">
       <formula>_xlfn.ISFORMULA(C9)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D45 D48:D49">
-    <cfRule type="expression" dxfId="11" priority="3">
+    <cfRule type="expression" dxfId="27" priority="3">
       <formula>_xlfn.ISFORMULA(D45)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23">
-    <cfRule type="expression" dxfId="10" priority="2">
+    <cfRule type="expression" dxfId="26" priority="2">
       <formula>_xlfn.ISFORMULA(C23)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B82:B84">
-    <cfRule type="expression" dxfId="9" priority="1">
+    <cfRule type="expression" dxfId="25" priority="1">
       <formula>_xlfn.ISFORMULA(B82)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9268,12 +9504,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9947295B-8D1F-FB48-972A-B6AD7BBC4112}">
   <dimension ref="A1:Y153"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B113" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B10" sqref="B10"/>
       <selection pane="topRight" activeCell="B10" sqref="B10"/>
       <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
-      <selection pane="bottomRight" activeCell="B128" sqref="B128"/>
+      <selection pane="bottomRight" activeCell="D106" sqref="D106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="46.83203125" defaultRowHeight="13" customHeight="1"/>
@@ -15371,17 +15607,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1 A3:XFD1048576 A2:N2 P2:XFD2">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="24" priority="1">
       <formula>_xlfn.ISFORMULA(A1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:XFD1048576 A2:N2 P2:XFD2">
-    <cfRule type="expression" dxfId="7" priority="168">
+    <cfRule type="expression" dxfId="23" priority="168">
       <formula>AND(COUNTA($A2:$AA2)=0, NOT(ISBLANK($A3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1048576:XFD1048576">
-    <cfRule type="expression" dxfId="6" priority="181">
+    <cfRule type="expression" dxfId="22" priority="181">
       <formula>AND(COUNTA(#REF!)=0, NOT(ISBLANK($A1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15390,6 +15626,1477 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E388B376-25CD-114A-9979-B5C580A31165}">
+  <dimension ref="A1:Y155"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="B10" sqref="B10"/>
+      <selection pane="topRight" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomRight" activeCell="F21" sqref="F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="46.83203125" defaultRowHeight="13" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="14.83203125" style="36" customWidth="1"/>
+    <col min="2" max="15" width="46.83203125" style="36"/>
+    <col min="16" max="16" width="46.83203125" style="32"/>
+    <col min="17" max="16384" width="46.83203125" style="36"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" s="34" customFormat="1" ht="13" customHeight="1">
+      <c r="B1" s="34" t="s">
+        <v>1147</v>
+      </c>
+      <c r="C1" s="34" t="s">
+        <v>221</v>
+      </c>
+      <c r="D1" s="34" t="s">
+        <v>356</v>
+      </c>
+      <c r="E1" s="34" t="s">
+        <v>224</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>1148</v>
+      </c>
+      <c r="P1" s="35"/>
+    </row>
+    <row r="2" spans="1:25" ht="13" customHeight="1">
+      <c r="A2" s="36" t="s">
+        <v>1112</v>
+      </c>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
+    </row>
+    <row r="3" spans="1:25" ht="13" customHeight="1">
+      <c r="A3" s="36" t="s">
+        <v>795</v>
+      </c>
+      <c r="Q3" s="32"/>
+      <c r="R3" s="32"/>
+      <c r="S3" s="32"/>
+      <c r="T3" s="32"/>
+    </row>
+    <row r="4" spans="1:25" ht="13" customHeight="1">
+      <c r="A4" s="36" t="s">
+        <v>796</v>
+      </c>
+      <c r="Q4" s="32"/>
+      <c r="R4" s="32"/>
+      <c r="S4" s="32"/>
+      <c r="T4" s="32"/>
+    </row>
+    <row r="5" spans="1:25" ht="13" customHeight="1">
+      <c r="A5" s="36" t="s">
+        <v>1088</v>
+      </c>
+      <c r="Q5" s="32"/>
+      <c r="R5" s="32"/>
+      <c r="S5" s="32"/>
+      <c r="T5" s="32"/>
+    </row>
+    <row r="6" spans="1:25" ht="13" customHeight="1">
+      <c r="A6" s="36" t="s">
+        <v>1097</v>
+      </c>
+      <c r="Q6" s="32"/>
+      <c r="R6" s="32"/>
+      <c r="S6" s="32"/>
+      <c r="T6" s="32"/>
+    </row>
+    <row r="7" spans="1:25" ht="13" customHeight="1">
+      <c r="A7" s="36" t="s">
+        <v>801</v>
+      </c>
+      <c r="B7" s="33" t="s">
+        <v>396</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>396</v>
+      </c>
+      <c r="D7" s="33" t="s">
+        <v>396</v>
+      </c>
+      <c r="E7" s="33" t="s">
+        <v>396</v>
+      </c>
+      <c r="F7" s="33" t="s">
+        <v>396</v>
+      </c>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="33"/>
+      <c r="K7" s="33"/>
+      <c r="L7" s="33"/>
+      <c r="M7" s="33"/>
+      <c r="N7" s="33"/>
+      <c r="O7" s="33"/>
+      <c r="Q7" s="33"/>
+      <c r="R7" s="33"/>
+      <c r="S7" s="33"/>
+      <c r="T7" s="33"/>
+      <c r="U7" s="33"/>
+      <c r="V7" s="33"/>
+      <c r="W7" s="33"/>
+      <c r="X7" s="33"/>
+      <c r="Y7" s="33"/>
+    </row>
+    <row r="8" spans="1:25" ht="13" customHeight="1">
+      <c r="A8" s="36" t="s">
+        <v>970</v>
+      </c>
+      <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
+      <c r="L8" s="33"/>
+      <c r="M8" s="33"/>
+      <c r="N8" s="33"/>
+      <c r="O8" s="33"/>
+      <c r="P8" s="33"/>
+      <c r="Q8" s="33"/>
+      <c r="R8" s="33"/>
+      <c r="S8" s="33"/>
+      <c r="T8" s="33"/>
+      <c r="U8" s="33"/>
+      <c r="V8" s="33"/>
+      <c r="W8" s="33"/>
+      <c r="X8" s="33"/>
+      <c r="Y8" s="33"/>
+    </row>
+    <row r="10" spans="1:25" ht="13" customHeight="1">
+      <c r="A10" s="36" t="s">
+        <v>819</v>
+      </c>
+      <c r="B10" s="36" t="s">
+        <v>838</v>
+      </c>
+      <c r="C10" s="36" t="str">
+        <f>B10</f>
+        <v>PathIn:  [data, output]</v>
+      </c>
+      <c r="D10" s="36" t="str">
+        <f>C10</f>
+        <v>PathIn:  [data, output]</v>
+      </c>
+      <c r="E10" s="36" t="str">
+        <f>D10</f>
+        <v>PathIn:  [data, output]</v>
+      </c>
+      <c r="F10" s="36" t="str">
+        <f>E10</f>
+        <v>PathIn:  [data, output]</v>
+      </c>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="33"/>
+      <c r="N10" s="33"/>
+      <c r="O10" s="33"/>
+      <c r="Q10" s="32"/>
+      <c r="R10" s="32"/>
+      <c r="S10" s="32"/>
+      <c r="V10" s="33"/>
+      <c r="W10" s="33"/>
+      <c r="X10" s="33"/>
+      <c r="Y10" s="33"/>
+    </row>
+    <row r="11" spans="1:25" ht="13" customHeight="1">
+      <c r="A11" s="36" t="s">
+        <v>169</v>
+      </c>
+      <c r="B11" s="36" t="s">
+        <v>1168</v>
+      </c>
+      <c r="C11" s="36" t="s">
+        <v>1170</v>
+      </c>
+      <c r="D11" s="36" t="s">
+        <v>1169</v>
+      </c>
+      <c r="E11" s="36" t="s">
+        <v>1171</v>
+      </c>
+      <c r="F11" s="36" t="s">
+        <v>1172</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" ht="13" customHeight="1">
+      <c r="A13" s="36" t="s">
+        <v>170</v>
+      </c>
+      <c r="B13" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="N13" s="37"/>
+      <c r="X13" s="33"/>
+    </row>
+    <row r="14" spans="1:25" ht="13" customHeight="1">
+      <c r="B14" s="36" t="s">
+        <v>1142</v>
+      </c>
+      <c r="C14" s="36" t="s">
+        <v>1143</v>
+      </c>
+      <c r="D14" s="36" t="s">
+        <v>1144</v>
+      </c>
+      <c r="E14" s="36" t="s">
+        <v>1145</v>
+      </c>
+      <c r="F14" s="36" t="s">
+        <v>1146</v>
+      </c>
+      <c r="N14" s="37"/>
+    </row>
+    <row r="15" spans="1:25" ht="13" customHeight="1">
+      <c r="B15" s="36" t="s">
+        <v>510</v>
+      </c>
+      <c r="C15" s="36" t="s">
+        <v>510</v>
+      </c>
+      <c r="D15" s="36" t="s">
+        <v>510</v>
+      </c>
+      <c r="E15" s="36" t="s">
+        <v>510</v>
+      </c>
+      <c r="F15" s="36" t="s">
+        <v>510</v>
+      </c>
+      <c r="N15" s="37"/>
+    </row>
+    <row r="17" spans="1:24" ht="13" customHeight="1">
+      <c r="A17" s="36" t="s">
+        <v>172</v>
+      </c>
+      <c r="D17" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="36" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" ht="13" customHeight="1">
+      <c r="D18" s="36" t="s">
+        <v>595</v>
+      </c>
+      <c r="F18" s="36" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" ht="13" customHeight="1">
+      <c r="D19" s="36" t="s">
+        <v>714</v>
+      </c>
+      <c r="F19" s="36" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" ht="13" customHeight="1">
+      <c r="D20" s="36" t="s">
+        <v>1175</v>
+      </c>
+      <c r="F20" s="36" t="s">
+        <v>1177</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" ht="13" customHeight="1">
+      <c r="D21" s="36" t="s">
+        <v>1174</v>
+      </c>
+      <c r="F21" s="36" t="s">
+        <v>1176</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" ht="13" customHeight="1">
+      <c r="F22" s="36" t="s">
+        <v>1174</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" ht="13" customHeight="1">
+      <c r="A26" s="36" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" ht="13" customHeight="1">
+      <c r="A28" s="36" t="s">
+        <v>174</v>
+      </c>
+      <c r="O28" s="33"/>
+      <c r="Q28" s="32"/>
+      <c r="R28" s="32"/>
+      <c r="S28" s="33"/>
+      <c r="U28" s="33"/>
+    </row>
+    <row r="29" spans="1:24" ht="13" customHeight="1">
+      <c r="O29" s="33"/>
+      <c r="Q29" s="32"/>
+      <c r="R29" s="32"/>
+      <c r="S29" s="33"/>
+      <c r="U29" s="33"/>
+    </row>
+    <row r="30" spans="1:24" ht="13" customHeight="1">
+      <c r="A30" s="36" t="s">
+        <v>175</v>
+      </c>
+      <c r="O30" s="33"/>
+      <c r="Q30" s="33"/>
+    </row>
+    <row r="31" spans="1:24" ht="13" customHeight="1">
+      <c r="B31" s="33"/>
+      <c r="K31" s="33"/>
+      <c r="L31" s="33"/>
+      <c r="M31" s="33"/>
+      <c r="N31" s="33"/>
+      <c r="O31" s="33"/>
+      <c r="Q31" s="32"/>
+      <c r="R31" s="32"/>
+      <c r="S31" s="32"/>
+      <c r="T31" s="32"/>
+      <c r="U31" s="33"/>
+      <c r="V31" s="33"/>
+      <c r="W31" s="33"/>
+      <c r="X31" s="33"/>
+    </row>
+    <row r="32" spans="1:24" ht="13" customHeight="1">
+      <c r="A32" s="36" t="s">
+        <v>176</v>
+      </c>
+      <c r="B32" s="33"/>
+      <c r="K32" s="33"/>
+      <c r="N32" s="33"/>
+      <c r="O32" s="33"/>
+      <c r="Q32" s="32"/>
+      <c r="R32" s="32"/>
+      <c r="S32" s="32"/>
+      <c r="T32" s="32"/>
+      <c r="U32" s="33"/>
+      <c r="V32" s="33"/>
+      <c r="W32" s="33"/>
+      <c r="X32" s="33"/>
+    </row>
+    <row r="33" spans="1:25" ht="13" customHeight="1">
+      <c r="B33" s="33"/>
+      <c r="K33" s="33"/>
+      <c r="L33" s="33"/>
+      <c r="M33" s="33"/>
+      <c r="N33" s="33"/>
+      <c r="O33" s="33"/>
+      <c r="Q33" s="32"/>
+      <c r="R33" s="32"/>
+      <c r="S33" s="32"/>
+      <c r="T33" s="32"/>
+      <c r="U33" s="33"/>
+      <c r="V33" s="33"/>
+      <c r="W33" s="33"/>
+      <c r="X33" s="33"/>
+      <c r="Y33" s="33"/>
+    </row>
+    <row r="34" spans="1:25" ht="13" customHeight="1">
+      <c r="A34" s="36" t="s">
+        <v>177</v>
+      </c>
+      <c r="B34" s="33"/>
+      <c r="F34" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="K34" s="33"/>
+      <c r="L34" s="33"/>
+      <c r="M34" s="33"/>
+      <c r="N34" s="33"/>
+      <c r="Q34" s="32"/>
+      <c r="R34" s="32"/>
+      <c r="S34" s="32"/>
+      <c r="T34" s="32"/>
+      <c r="U34" s="33"/>
+      <c r="V34" s="33"/>
+      <c r="W34" s="33"/>
+      <c r="X34" s="33"/>
+      <c r="Y34" s="33"/>
+    </row>
+    <row r="35" spans="1:25" ht="13" customHeight="1">
+      <c r="B35" s="33"/>
+      <c r="F35" s="36" t="s">
+        <v>1166</v>
+      </c>
+      <c r="K35" s="33"/>
+      <c r="L35" s="33"/>
+      <c r="M35" s="33"/>
+      <c r="N35" s="33"/>
+      <c r="Q35" s="32"/>
+      <c r="R35" s="32"/>
+      <c r="S35" s="32"/>
+      <c r="T35" s="32"/>
+      <c r="U35" s="33"/>
+      <c r="V35" s="33"/>
+      <c r="W35" s="33"/>
+      <c r="X35" s="33"/>
+      <c r="Y35" s="33"/>
+    </row>
+    <row r="36" spans="1:25" ht="13" customHeight="1">
+      <c r="B36" s="33"/>
+      <c r="F36" s="36" t="s">
+        <v>1167</v>
+      </c>
+      <c r="K36" s="33"/>
+      <c r="L36" s="33"/>
+      <c r="M36" s="33"/>
+      <c r="N36" s="33"/>
+      <c r="Q36" s="32"/>
+      <c r="R36" s="32"/>
+      <c r="S36" s="32"/>
+      <c r="T36" s="32"/>
+      <c r="U36" s="33"/>
+      <c r="V36" s="33"/>
+      <c r="W36" s="33"/>
+      <c r="X36" s="33"/>
+      <c r="Y36" s="33"/>
+    </row>
+    <row r="37" spans="1:25" ht="13" customHeight="1">
+      <c r="B37" s="33"/>
+      <c r="K37" s="33"/>
+      <c r="L37" s="33"/>
+      <c r="M37" s="33"/>
+      <c r="O37" s="33"/>
+      <c r="Q37" s="32"/>
+      <c r="R37" s="32"/>
+      <c r="S37" s="32"/>
+      <c r="T37" s="32"/>
+      <c r="U37" s="33"/>
+      <c r="W37" s="33"/>
+      <c r="X37" s="33"/>
+    </row>
+    <row r="38" spans="1:25" ht="13" customHeight="1">
+      <c r="A38" s="38" t="s">
+        <v>178</v>
+      </c>
+      <c r="B38" s="36" t="s">
+        <v>398</v>
+      </c>
+      <c r="C38" s="36" t="s">
+        <v>398</v>
+      </c>
+      <c r="D38" s="36" t="s">
+        <v>398</v>
+      </c>
+      <c r="F38" s="36" t="s">
+        <v>398</v>
+      </c>
+      <c r="K38" s="33"/>
+      <c r="O38" s="33"/>
+      <c r="Q38" s="32"/>
+      <c r="R38" s="32"/>
+      <c r="S38" s="32"/>
+      <c r="T38" s="32"/>
+      <c r="U38" s="33"/>
+      <c r="W38" s="33"/>
+      <c r="X38" s="33"/>
+    </row>
+    <row r="39" spans="1:25" ht="13" customHeight="1">
+      <c r="A39" s="38"/>
+      <c r="B39" s="36" t="s">
+        <v>1055</v>
+      </c>
+      <c r="C39" s="36" t="s">
+        <v>1053</v>
+      </c>
+      <c r="D39" s="36" t="s">
+        <v>1159</v>
+      </c>
+      <c r="F39" s="36" t="s">
+        <v>1164</v>
+      </c>
+      <c r="K39" s="33"/>
+      <c r="L39" s="33"/>
+      <c r="M39" s="33"/>
+      <c r="O39" s="33"/>
+      <c r="Q39" s="32"/>
+      <c r="R39" s="32"/>
+      <c r="S39" s="32"/>
+      <c r="T39" s="32"/>
+      <c r="U39" s="33"/>
+    </row>
+    <row r="40" spans="1:25" ht="13" customHeight="1">
+      <c r="A40" s="38"/>
+      <c r="B40" s="36" t="s">
+        <v>932</v>
+      </c>
+      <c r="C40" s="36" t="s">
+        <v>1149</v>
+      </c>
+      <c r="D40" s="36" t="s">
+        <v>1160</v>
+      </c>
+      <c r="F40" s="36" t="s">
+        <v>936</v>
+      </c>
+      <c r="K40" s="33"/>
+      <c r="L40" s="33"/>
+      <c r="M40" s="33"/>
+      <c r="O40" s="33"/>
+      <c r="Q40" s="32"/>
+      <c r="R40" s="32"/>
+      <c r="S40" s="32"/>
+      <c r="T40" s="32"/>
+      <c r="U40" s="33"/>
+    </row>
+    <row r="41" spans="1:25" ht="13" customHeight="1">
+      <c r="A41" s="38"/>
+      <c r="B41" s="36" t="s">
+        <v>984</v>
+      </c>
+      <c r="C41" s="36" t="s">
+        <v>984</v>
+      </c>
+      <c r="D41" s="36" t="s">
+        <v>1161</v>
+      </c>
+      <c r="F41" s="36" t="s">
+        <v>984</v>
+      </c>
+      <c r="K41" s="33"/>
+      <c r="L41" s="33"/>
+      <c r="M41" s="33"/>
+      <c r="O41" s="33"/>
+      <c r="Q41" s="32"/>
+      <c r="R41" s="32"/>
+      <c r="S41" s="32"/>
+      <c r="T41" s="32"/>
+    </row>
+    <row r="42" spans="1:25" ht="13" customHeight="1">
+      <c r="A42" s="38"/>
+      <c r="B42" s="36" t="s">
+        <v>1154</v>
+      </c>
+      <c r="C42" s="36" t="s">
+        <v>1150</v>
+      </c>
+      <c r="D42" s="36" t="s">
+        <v>1162</v>
+      </c>
+      <c r="F42" s="36" t="s">
+        <v>1165</v>
+      </c>
+      <c r="K42" s="33"/>
+      <c r="L42" s="33"/>
+      <c r="M42" s="33"/>
+      <c r="N42" s="33"/>
+      <c r="O42" s="33"/>
+      <c r="Q42" s="32"/>
+      <c r="R42" s="32"/>
+      <c r="S42" s="32"/>
+      <c r="T42" s="32"/>
+      <c r="U42" s="33"/>
+    </row>
+    <row r="43" spans="1:25" ht="13" customHeight="1">
+      <c r="A43" s="38"/>
+      <c r="B43" s="36" t="s">
+        <v>1155</v>
+      </c>
+      <c r="C43" s="36" t="s">
+        <v>1151</v>
+      </c>
+      <c r="D43" s="36" t="s">
+        <v>1155</v>
+      </c>
+      <c r="F43" s="36" t="s">
+        <v>1151</v>
+      </c>
+      <c r="L43" s="33"/>
+      <c r="N43" s="33"/>
+      <c r="O43" s="33"/>
+      <c r="Q43" s="32"/>
+      <c r="R43" s="32"/>
+      <c r="S43" s="32"/>
+      <c r="T43" s="32"/>
+      <c r="U43" s="33"/>
+      <c r="Y43" s="33"/>
+    </row>
+    <row r="44" spans="1:25" ht="13" customHeight="1">
+      <c r="A44" s="38"/>
+      <c r="B44" s="36" t="s">
+        <v>1152</v>
+      </c>
+      <c r="C44" s="36" t="str">
+        <f>$B$44</f>
+        <v xml:space="preserve">    kind:   inner</v>
+      </c>
+      <c r="D44" s="36" t="str">
+        <f>$B$44</f>
+        <v xml:space="preserve">    kind:   inner</v>
+      </c>
+      <c r="F44" s="36" t="str">
+        <f>$B$44</f>
+        <v xml:space="preserve">    kind:   inner</v>
+      </c>
+      <c r="K44" s="33"/>
+      <c r="L44" s="33"/>
+      <c r="M44" s="33"/>
+      <c r="Q44" s="32"/>
+      <c r="R44" s="32"/>
+      <c r="S44" s="32"/>
+      <c r="T44" s="32"/>
+      <c r="Y44" s="33"/>
+    </row>
+    <row r="45" spans="1:25" ht="13" customHeight="1">
+      <c r="A45" s="38"/>
+      <c r="F45" s="33"/>
+      <c r="K45" s="33"/>
+      <c r="L45" s="33"/>
+      <c r="M45" s="33"/>
+      <c r="O45" s="33"/>
+      <c r="Q45" s="32"/>
+      <c r="R45" s="32"/>
+      <c r="S45" s="32"/>
+      <c r="T45" s="32"/>
+    </row>
+    <row r="46" spans="1:25" ht="13" customHeight="1">
+      <c r="A46" s="38" t="s">
+        <v>179</v>
+      </c>
+      <c r="K46" s="33"/>
+      <c r="L46" s="33"/>
+      <c r="M46" s="33"/>
+      <c r="O46" s="33"/>
+      <c r="Q46" s="32"/>
+      <c r="R46" s="32"/>
+      <c r="S46" s="32"/>
+      <c r="T46" s="32"/>
+      <c r="U46" s="33"/>
+    </row>
+    <row r="47" spans="1:25" ht="13" customHeight="1">
+      <c r="A47" s="38"/>
+      <c r="K47" s="33"/>
+      <c r="L47" s="33"/>
+      <c r="M47" s="33"/>
+      <c r="O47" s="33"/>
+      <c r="Q47" s="32"/>
+      <c r="R47" s="32"/>
+      <c r="S47" s="32"/>
+      <c r="T47" s="32"/>
+      <c r="U47" s="33"/>
+    </row>
+    <row r="48" spans="1:25" ht="13" customHeight="1">
+      <c r="A48" s="38" t="s">
+        <v>180</v>
+      </c>
+      <c r="B48" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="K48" s="33"/>
+      <c r="L48" s="33"/>
+      <c r="M48" s="33"/>
+      <c r="O48" s="33"/>
+      <c r="Q48" s="32"/>
+      <c r="R48" s="32"/>
+      <c r="S48" s="32"/>
+      <c r="T48" s="32"/>
+      <c r="U48" s="33"/>
+    </row>
+    <row r="49" spans="1:22" ht="13" customHeight="1">
+      <c r="A49" s="38"/>
+      <c r="B49" s="36" t="s">
+        <v>1157</v>
+      </c>
+      <c r="K49" s="33"/>
+      <c r="L49" s="33"/>
+      <c r="M49" s="33"/>
+      <c r="O49" s="33"/>
+      <c r="Q49" s="32"/>
+      <c r="R49" s="32"/>
+      <c r="S49" s="32"/>
+      <c r="T49" s="32"/>
+      <c r="U49" s="33"/>
+    </row>
+    <row r="50" spans="1:22" ht="13" customHeight="1">
+      <c r="A50" s="38"/>
+      <c r="B50" s="36" t="s">
+        <v>1158</v>
+      </c>
+      <c r="K50" s="33"/>
+      <c r="L50" s="33"/>
+      <c r="M50" s="33"/>
+      <c r="O50" s="33"/>
+      <c r="Q50" s="32"/>
+      <c r="R50" s="32"/>
+      <c r="S50" s="32"/>
+      <c r="T50" s="32"/>
+      <c r="U50" s="33"/>
+    </row>
+    <row r="51" spans="1:22" ht="13" customHeight="1">
+      <c r="A51" s="38"/>
+      <c r="B51" s="36" t="s">
+        <v>101</v>
+      </c>
+      <c r="L51" s="33"/>
+      <c r="O51" s="33"/>
+      <c r="Q51" s="32"/>
+      <c r="R51" s="32"/>
+      <c r="S51" s="32"/>
+      <c r="T51" s="32"/>
+      <c r="U51" s="33"/>
+    </row>
+    <row r="52" spans="1:22" ht="13" customHeight="1">
+      <c r="A52" s="38"/>
+      <c r="K52" s="33"/>
+      <c r="L52" s="33"/>
+      <c r="M52" s="33"/>
+      <c r="O52" s="33"/>
+      <c r="Q52" s="32"/>
+      <c r="R52" s="32"/>
+      <c r="S52" s="32"/>
+      <c r="T52" s="32"/>
+      <c r="U52" s="33"/>
+    </row>
+    <row r="53" spans="1:22" ht="13" customHeight="1">
+      <c r="A53" s="38" t="s">
+        <v>427</v>
+      </c>
+      <c r="B53" s="36" t="s">
+        <v>436</v>
+      </c>
+      <c r="C53" s="36" t="s">
+        <v>436</v>
+      </c>
+      <c r="D53" s="36" t="s">
+        <v>436</v>
+      </c>
+      <c r="F53" s="36" t="s">
+        <v>436</v>
+      </c>
+      <c r="L53" s="33"/>
+      <c r="O53" s="33"/>
+      <c r="Q53" s="32"/>
+      <c r="R53" s="32"/>
+      <c r="S53" s="32"/>
+      <c r="T53" s="32"/>
+      <c r="U53" s="33"/>
+    </row>
+    <row r="54" spans="1:22" ht="13" customHeight="1">
+      <c r="A54" s="38"/>
+      <c r="B54" s="36" t="s">
+        <v>522</v>
+      </c>
+      <c r="C54" s="36" t="str">
+        <f>$B54</f>
+        <v xml:space="preserve">  operation: sum</v>
+      </c>
+      <c r="D54" s="36" t="str">
+        <f>$B54</f>
+        <v xml:space="preserve">  operation: sum</v>
+      </c>
+      <c r="F54" s="36" t="str">
+        <f>$B54</f>
+        <v xml:space="preserve">  operation: sum</v>
+      </c>
+      <c r="K54" s="33"/>
+      <c r="L54" s="33"/>
+      <c r="M54" s="33"/>
+      <c r="O54" s="33"/>
+      <c r="Q54" s="32"/>
+      <c r="R54" s="32"/>
+      <c r="S54" s="32"/>
+      <c r="T54" s="32"/>
+      <c r="U54" s="33"/>
+    </row>
+    <row r="55" spans="1:22" ht="13" customHeight="1">
+      <c r="A55" s="38"/>
+      <c r="B55" s="36" t="s">
+        <v>523</v>
+      </c>
+      <c r="C55" s="36" t="str">
+        <f t="shared" ref="C55:F57" si="0">$B55</f>
+        <v xml:space="preserve">  axis:   row</v>
+      </c>
+      <c r="D55" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  axis:   row</v>
+      </c>
+      <c r="F55" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  axis:   row</v>
+      </c>
+      <c r="K55" s="33"/>
+      <c r="L55" s="33"/>
+      <c r="M55" s="33"/>
+      <c r="O55" s="33"/>
+      <c r="Q55" s="32"/>
+      <c r="R55" s="32"/>
+      <c r="S55" s="32"/>
+      <c r="T55" s="32"/>
+      <c r="U55" s="33"/>
+    </row>
+    <row r="56" spans="1:22" ht="13" customHeight="1">
+      <c r="A56" s="38"/>
+      <c r="B56" s="36" t="s">
+        <v>525</v>
+      </c>
+      <c r="C56" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  from:   nothing</v>
+      </c>
+      <c r="D56" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  from:   nothing</v>
+      </c>
+      <c r="F56" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  from:   nothing</v>
+      </c>
+      <c r="K56" s="33"/>
+      <c r="L56" s="33"/>
+      <c r="M56" s="33"/>
+      <c r="O56" s="33"/>
+      <c r="Q56" s="32"/>
+      <c r="R56" s="32"/>
+      <c r="S56" s="32"/>
+      <c r="T56" s="32"/>
+      <c r="U56" s="33"/>
+    </row>
+    <row r="57" spans="1:22" ht="13" customHeight="1">
+      <c r="B57" s="36" t="s">
+        <v>524</v>
+      </c>
+      <c r="C57" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  to:     nothing</v>
+      </c>
+      <c r="D57" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  to:     nothing</v>
+      </c>
+      <c r="F57" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  to:     nothing</v>
+      </c>
+      <c r="K57" s="33"/>
+      <c r="L57" s="33"/>
+      <c r="M57" s="33"/>
+      <c r="O57" s="33"/>
+      <c r="Q57" s="32"/>
+      <c r="R57" s="32"/>
+      <c r="S57" s="32"/>
+      <c r="T57" s="32"/>
+      <c r="U57" s="33"/>
+    </row>
+    <row r="58" spans="1:22" ht="13" customHeight="1">
+      <c r="B58" s="36" t="s">
+        <v>1156</v>
+      </c>
+      <c r="C58" s="36" t="s">
+        <v>1153</v>
+      </c>
+      <c r="D58" s="36" t="s">
+        <v>1163</v>
+      </c>
+      <c r="F58" s="36" t="s">
+        <v>1173</v>
+      </c>
+      <c r="K58" s="33"/>
+      <c r="L58" s="33"/>
+      <c r="M58" s="33"/>
+      <c r="O58" s="33"/>
+      <c r="Q58" s="32"/>
+      <c r="R58" s="32"/>
+      <c r="S58" s="32"/>
+      <c r="T58" s="32"/>
+      <c r="U58" s="33"/>
+    </row>
+    <row r="59" spans="1:22" ht="13" customHeight="1">
+      <c r="B59" s="36" t="s">
+        <v>440</v>
+      </c>
+      <c r="C59" s="36" t="str">
+        <f>$B59</f>
+        <v xml:space="preserve">  output: value</v>
+      </c>
+      <c r="D59" s="36" t="str">
+        <f>$B59</f>
+        <v xml:space="preserve">  output: value</v>
+      </c>
+      <c r="F59" s="36" t="str">
+        <f>$B59</f>
+        <v xml:space="preserve">  output: value</v>
+      </c>
+      <c r="K59" s="33"/>
+      <c r="L59" s="33"/>
+      <c r="M59" s="33"/>
+      <c r="O59" s="33"/>
+      <c r="Q59" s="32"/>
+      <c r="R59" s="32"/>
+      <c r="S59" s="32"/>
+      <c r="T59" s="32"/>
+      <c r="U59" s="33"/>
+    </row>
+    <row r="60" spans="1:22" ht="13" customHeight="1">
+      <c r="K60" s="33"/>
+      <c r="L60" s="33"/>
+      <c r="M60" s="33"/>
+      <c r="O60" s="33"/>
+      <c r="Q60" s="32"/>
+      <c r="R60" s="32"/>
+      <c r="S60" s="32"/>
+      <c r="T60" s="32"/>
+      <c r="U60" s="33"/>
+    </row>
+    <row r="61" spans="1:22" ht="13" customHeight="1">
+      <c r="K61" s="33"/>
+      <c r="L61" s="33"/>
+      <c r="M61" s="33"/>
+      <c r="O61" s="33"/>
+      <c r="Q61" s="32"/>
+      <c r="R61" s="32"/>
+      <c r="S61" s="32"/>
+      <c r="T61" s="32"/>
+      <c r="U61" s="33"/>
+    </row>
+    <row r="62" spans="1:22" ht="13" customHeight="1">
+      <c r="O62" s="33"/>
+      <c r="Q62" s="33"/>
+      <c r="R62" s="33"/>
+      <c r="S62" s="33"/>
+      <c r="T62" s="33"/>
+      <c r="U62" s="33"/>
+    </row>
+    <row r="63" spans="1:22" ht="13" customHeight="1">
+      <c r="K63" s="33"/>
+      <c r="L63" s="33"/>
+      <c r="M63" s="33"/>
+      <c r="V63" s="33"/>
+    </row>
+    <row r="64" spans="1:22" ht="13" customHeight="1">
+      <c r="K64" s="33"/>
+      <c r="L64" s="33"/>
+      <c r="M64" s="33"/>
+      <c r="V64" s="33"/>
+    </row>
+    <row r="65" spans="6:22" ht="13" customHeight="1">
+      <c r="K65" s="33"/>
+      <c r="L65" s="33"/>
+      <c r="M65" s="33"/>
+      <c r="V65" s="33"/>
+    </row>
+    <row r="67" spans="6:22" ht="13" customHeight="1">
+      <c r="V67" s="33"/>
+    </row>
+    <row r="79" spans="6:22" ht="13" customHeight="1">
+      <c r="F79" s="33"/>
+      <c r="G79" s="33"/>
+      <c r="J79" s="33"/>
+      <c r="N79" s="33"/>
+    </row>
+    <row r="80" spans="6:22" ht="13" customHeight="1">
+      <c r="F80" s="33"/>
+      <c r="G80" s="33"/>
+      <c r="J80" s="33"/>
+      <c r="N80" s="33"/>
+    </row>
+    <row r="81" spans="6:24" ht="13" customHeight="1">
+      <c r="F81" s="33"/>
+      <c r="G81" s="33"/>
+      <c r="J81" s="33"/>
+      <c r="N81" s="33"/>
+    </row>
+    <row r="82" spans="6:24" ht="13" customHeight="1">
+      <c r="F82" s="33"/>
+      <c r="G82" s="33"/>
+      <c r="J82" s="33"/>
+      <c r="N82" s="33"/>
+    </row>
+    <row r="83" spans="6:24" ht="13" customHeight="1">
+      <c r="F83" s="33"/>
+      <c r="J83" s="33"/>
+      <c r="N83" s="33"/>
+    </row>
+    <row r="84" spans="6:24" ht="13" customHeight="1">
+      <c r="F84" s="33"/>
+      <c r="J84" s="33"/>
+      <c r="N84" s="33"/>
+    </row>
+    <row r="85" spans="6:24" ht="13" customHeight="1">
+      <c r="F85" s="33"/>
+      <c r="J85" s="33"/>
+      <c r="N85" s="33"/>
+    </row>
+    <row r="86" spans="6:24" customFormat="1" ht="13" customHeight="1">
+      <c r="H86" s="33"/>
+    </row>
+    <row r="87" spans="6:24" ht="13" customHeight="1">
+      <c r="F87" s="33"/>
+      <c r="H87" s="33"/>
+      <c r="J87" s="33"/>
+      <c r="N87" s="33"/>
+    </row>
+    <row r="88" spans="6:24" ht="13" customHeight="1">
+      <c r="F88" s="33"/>
+      <c r="H88" s="33"/>
+      <c r="J88" s="33"/>
+      <c r="N88" s="33"/>
+    </row>
+    <row r="90" spans="6:24" ht="13" customHeight="1">
+      <c r="Q90" s="32"/>
+      <c r="W90" s="33"/>
+      <c r="X90" s="33"/>
+    </row>
+    <row r="91" spans="6:24" ht="13" customHeight="1">
+      <c r="Q91" s="32"/>
+      <c r="W91" s="33"/>
+      <c r="X91" s="33"/>
+    </row>
+    <row r="92" spans="6:24" ht="13" customHeight="1">
+      <c r="Q92" s="32"/>
+      <c r="W92" s="33"/>
+      <c r="X92" s="33"/>
+    </row>
+    <row r="93" spans="6:24" ht="13" customHeight="1">
+      <c r="Q93" s="32"/>
+      <c r="W93" s="33"/>
+      <c r="X93" s="33"/>
+    </row>
+    <row r="95" spans="6:24" ht="13" customHeight="1">
+      <c r="W95" s="33"/>
+    </row>
+    <row r="96" spans="6:24" ht="13" customHeight="1">
+      <c r="W96" s="33"/>
+    </row>
+    <row r="97" spans="11:24" ht="13" customHeight="1">
+      <c r="W97" s="33"/>
+    </row>
+    <row r="98" spans="11:24" ht="13" customHeight="1">
+      <c r="W98" s="33"/>
+    </row>
+    <row r="99" spans="11:24" ht="13" customHeight="1">
+      <c r="W99" s="33"/>
+    </row>
+    <row r="101" spans="11:24" ht="13" customHeight="1">
+      <c r="K101" s="33"/>
+      <c r="L101" s="33"/>
+      <c r="Q101" s="32"/>
+      <c r="R101" s="32"/>
+      <c r="S101" s="32"/>
+      <c r="X101" s="33"/>
+    </row>
+    <row r="102" spans="11:24" ht="13" customHeight="1">
+      <c r="L102" s="33"/>
+      <c r="N102" s="37"/>
+      <c r="Q102" s="32"/>
+      <c r="R102" s="32"/>
+      <c r="S102" s="32"/>
+      <c r="U102" s="37"/>
+      <c r="X102" s="33"/>
+    </row>
+    <row r="103" spans="11:24" ht="13" customHeight="1">
+      <c r="L103" s="33"/>
+      <c r="N103" s="37"/>
+      <c r="Q103" s="32"/>
+      <c r="R103" s="32"/>
+      <c r="S103" s="32"/>
+      <c r="U103" s="37"/>
+      <c r="X103" s="33"/>
+    </row>
+    <row r="104" spans="11:24" ht="13" customHeight="1">
+      <c r="L104" s="33"/>
+      <c r="N104" s="37"/>
+      <c r="Q104" s="32"/>
+      <c r="R104" s="32"/>
+      <c r="S104" s="32"/>
+      <c r="U104" s="37"/>
+      <c r="X104" s="33"/>
+    </row>
+    <row r="105" spans="11:24" ht="13" customHeight="1">
+      <c r="L105" s="33"/>
+      <c r="N105" s="37"/>
+      <c r="Q105" s="32"/>
+      <c r="R105" s="32"/>
+      <c r="S105" s="32"/>
+      <c r="U105" s="37"/>
+      <c r="X105" s="33"/>
+    </row>
+    <row r="106" spans="11:24" ht="13" customHeight="1">
+      <c r="L106" s="33"/>
+      <c r="N106" s="37"/>
+      <c r="Q106" s="32"/>
+      <c r="R106" s="32"/>
+      <c r="S106" s="32"/>
+      <c r="U106" s="37"/>
+      <c r="X106" s="33"/>
+    </row>
+    <row r="107" spans="11:24" ht="13" customHeight="1">
+      <c r="L107" s="33"/>
+      <c r="N107" s="37"/>
+      <c r="Q107" s="32"/>
+      <c r="R107" s="32"/>
+      <c r="S107" s="32"/>
+    </row>
+    <row r="108" spans="11:24" ht="13" customHeight="1">
+      <c r="L108" s="33"/>
+      <c r="N108" s="37"/>
+      <c r="Q108" s="32"/>
+      <c r="R108" s="32"/>
+      <c r="S108" s="32"/>
+    </row>
+    <row r="109" spans="11:24" ht="13" customHeight="1">
+      <c r="L109" s="33"/>
+      <c r="N109" s="37"/>
+      <c r="Q109" s="32"/>
+      <c r="R109" s="32"/>
+      <c r="S109" s="32"/>
+    </row>
+    <row r="110" spans="11:24" ht="13" customHeight="1">
+      <c r="L110" s="33"/>
+      <c r="N110" s="37"/>
+      <c r="Q110" s="32"/>
+      <c r="R110" s="32"/>
+      <c r="S110" s="32"/>
+    </row>
+    <row r="111" spans="11:24" ht="13" customHeight="1">
+      <c r="L111" s="33"/>
+      <c r="N111" s="37"/>
+      <c r="Q111" s="32"/>
+      <c r="R111" s="32"/>
+      <c r="S111" s="32"/>
+    </row>
+    <row r="112" spans="11:24" ht="13" customHeight="1">
+      <c r="L112" s="33"/>
+      <c r="N112" s="37"/>
+      <c r="Q112" s="32"/>
+      <c r="R112" s="32"/>
+      <c r="S112" s="32"/>
+    </row>
+    <row r="113" spans="6:19" ht="13" customHeight="1">
+      <c r="L113" s="33"/>
+      <c r="P113" s="36"/>
+      <c r="Q113" s="32"/>
+      <c r="R113" s="32"/>
+      <c r="S113" s="32"/>
+    </row>
+    <row r="114" spans="6:19" ht="13" customHeight="1">
+      <c r="L114" s="33"/>
+      <c r="Q114" s="32"/>
+      <c r="R114" s="32"/>
+      <c r="S114" s="32"/>
+    </row>
+    <row r="115" spans="6:19" ht="13" customHeight="1">
+      <c r="L115" s="33"/>
+    </row>
+    <row r="116" spans="6:19" ht="13" customHeight="1">
+      <c r="L116" s="33"/>
+    </row>
+    <row r="117" spans="6:19" ht="13" customHeight="1">
+      <c r="L117" s="33"/>
+    </row>
+    <row r="118" spans="6:19" ht="13" customHeight="1">
+      <c r="L118" s="33"/>
+    </row>
+    <row r="119" spans="6:19" ht="13" customHeight="1">
+      <c r="L119" s="33"/>
+    </row>
+    <row r="120" spans="6:19" ht="13" customHeight="1">
+      <c r="L120" s="33"/>
+      <c r="Q120" s="32"/>
+      <c r="R120" s="32"/>
+      <c r="S120" s="32"/>
+    </row>
+    <row r="121" spans="6:19" ht="13" customHeight="1">
+      <c r="L121" s="33"/>
+      <c r="Q121" s="32"/>
+      <c r="R121" s="32"/>
+      <c r="S121" s="32"/>
+    </row>
+    <row r="122" spans="6:19" ht="13" customHeight="1">
+      <c r="L122" s="33"/>
+      <c r="Q122" s="32"/>
+      <c r="R122" s="32"/>
+      <c r="S122" s="32"/>
+    </row>
+    <row r="123" spans="6:19" ht="13" customHeight="1">
+      <c r="L123" s="33"/>
+      <c r="Q123" s="32"/>
+      <c r="R123" s="32"/>
+      <c r="S123" s="32"/>
+    </row>
+    <row r="124" spans="6:19" ht="13" customHeight="1">
+      <c r="L124" s="33"/>
+      <c r="Q124" s="32"/>
+      <c r="R124" s="32"/>
+      <c r="S124" s="32"/>
+    </row>
+    <row r="125" spans="6:19" ht="13" customHeight="1">
+      <c r="L125" s="33"/>
+      <c r="Q125" s="32"/>
+      <c r="R125" s="32"/>
+      <c r="S125" s="32"/>
+    </row>
+    <row r="127" spans="6:19" ht="13" customHeight="1">
+      <c r="F127" s="33"/>
+      <c r="J127" s="33"/>
+      <c r="N127" s="33"/>
+    </row>
+    <row r="128" spans="6:19" ht="13" customHeight="1">
+      <c r="F128" s="33"/>
+      <c r="J128" s="33"/>
+      <c r="N128" s="33"/>
+    </row>
+    <row r="129" spans="6:19" ht="13" customHeight="1">
+      <c r="F129" s="33"/>
+      <c r="J129" s="33"/>
+      <c r="N129" s="33"/>
+    </row>
+    <row r="130" spans="6:19" ht="13" customHeight="1">
+      <c r="F130" s="33"/>
+      <c r="J130" s="33"/>
+      <c r="N130" s="33"/>
+    </row>
+    <row r="131" spans="6:19" ht="13" customHeight="1">
+      <c r="F131" s="33"/>
+      <c r="G131" s="33"/>
+      <c r="H131" s="33"/>
+      <c r="J131" s="33"/>
+      <c r="N131" s="33"/>
+    </row>
+    <row r="132" spans="6:19" ht="13" customHeight="1">
+      <c r="F132" s="33"/>
+      <c r="G132" s="33"/>
+      <c r="H132" s="33"/>
+      <c r="J132" s="33"/>
+      <c r="N132" s="33"/>
+    </row>
+    <row r="133" spans="6:19" ht="13" customHeight="1">
+      <c r="F133" s="33"/>
+      <c r="G133" s="33"/>
+      <c r="H133" s="33"/>
+      <c r="J133" s="33"/>
+      <c r="N133" s="33"/>
+    </row>
+    <row r="134" spans="6:19" ht="13" customHeight="1">
+      <c r="F134" s="33"/>
+      <c r="G134" s="33"/>
+      <c r="H134" s="33"/>
+      <c r="I134" s="33"/>
+      <c r="J134" s="33"/>
+      <c r="N134" s="33"/>
+    </row>
+    <row r="135" spans="6:19" ht="13" customHeight="1">
+      <c r="F135" s="33"/>
+      <c r="G135" s="33"/>
+      <c r="H135" s="33"/>
+      <c r="I135" s="33"/>
+      <c r="J135" s="33"/>
+      <c r="N135" s="33"/>
+    </row>
+    <row r="136" spans="6:19" ht="13" customHeight="1">
+      <c r="F136" s="33"/>
+      <c r="G136" s="33"/>
+      <c r="H136" s="33"/>
+      <c r="I136" s="33"/>
+      <c r="J136" s="33"/>
+      <c r="N136" s="33"/>
+    </row>
+    <row r="138" spans="6:19" ht="13" customHeight="1">
+      <c r="O138" s="33"/>
+      <c r="Q138" s="33"/>
+    </row>
+    <row r="139" spans="6:19" ht="13" customHeight="1">
+      <c r="O139" s="33"/>
+      <c r="Q139" s="33"/>
+    </row>
+    <row r="140" spans="6:19" ht="13" customHeight="1">
+      <c r="O140" s="33"/>
+      <c r="Q140" s="33"/>
+    </row>
+    <row r="141" spans="6:19" ht="13" customHeight="1">
+      <c r="O141" s="33"/>
+      <c r="Q141" s="33"/>
+      <c r="R141" s="33"/>
+      <c r="S141" s="33"/>
+    </row>
+    <row r="142" spans="6:19" ht="13" customHeight="1">
+      <c r="N142" s="37"/>
+      <c r="Q142" s="32"/>
+      <c r="R142" s="32"/>
+      <c r="S142" s="32"/>
+    </row>
+    <row r="143" spans="6:19" ht="13" customHeight="1">
+      <c r="N143" s="37"/>
+      <c r="Q143" s="32"/>
+      <c r="R143" s="32"/>
+      <c r="S143" s="32"/>
+    </row>
+    <row r="144" spans="6:19" ht="13" customHeight="1">
+      <c r="Q144" s="32"/>
+      <c r="R144" s="32"/>
+      <c r="S144" s="32"/>
+    </row>
+    <row r="145" spans="1:20" ht="13" customHeight="1">
+      <c r="O145" s="33"/>
+      <c r="Q145" s="32"/>
+      <c r="R145" s="32"/>
+      <c r="S145" s="32"/>
+      <c r="T145" s="33"/>
+    </row>
+    <row r="146" spans="1:20" ht="13" customHeight="1">
+      <c r="O146" s="33"/>
+      <c r="Q146" s="32"/>
+      <c r="R146" s="32"/>
+      <c r="S146" s="32"/>
+      <c r="T146" s="33"/>
+    </row>
+    <row r="147" spans="1:20" ht="13" customHeight="1">
+      <c r="O147" s="33"/>
+      <c r="Q147" s="32"/>
+      <c r="R147" s="32"/>
+      <c r="S147" s="32"/>
+      <c r="T147" s="33"/>
+    </row>
+    <row r="149" spans="1:20" ht="13" customHeight="1">
+      <c r="Q149" s="32"/>
+      <c r="R149" s="32"/>
+      <c r="S149" s="32"/>
+    </row>
+    <row r="150" spans="1:20" ht="13" customHeight="1">
+      <c r="Q150" s="32"/>
+      <c r="R150" s="32"/>
+      <c r="S150" s="32"/>
+    </row>
+    <row r="151" spans="1:20" ht="13" customHeight="1">
+      <c r="Q151" s="32"/>
+      <c r="R151" s="32"/>
+      <c r="S151" s="32"/>
+    </row>
+    <row r="152" spans="1:20" ht="13" customHeight="1">
+      <c r="A152" s="38"/>
+      <c r="Q152" s="32"/>
+      <c r="R152" s="32"/>
+      <c r="S152" s="32"/>
+    </row>
+    <row r="153" spans="1:20" ht="13" customHeight="1">
+      <c r="A153" s="38"/>
+      <c r="Q153" s="32"/>
+      <c r="R153" s="32"/>
+      <c r="S153" s="32"/>
+    </row>
+    <row r="154" spans="1:20" ht="13" customHeight="1">
+      <c r="A154" s="38"/>
+      <c r="Q154" s="32"/>
+      <c r="R154" s="32"/>
+      <c r="S154" s="32"/>
+    </row>
+    <row r="155" spans="1:20" ht="13" customHeight="1">
+      <c r="A155" s="38"/>
+      <c r="Q155" s="32"/>
+      <c r="R155" s="32"/>
+      <c r="S155" s="32"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:XFD1 A2:N2 P2:XFD2 C17:E17 A79:B80 D79:XFD80 A81:XFD1048576 A17 A12:XFD16 E11:XFD11 A11:C11 A3:XFD10 A23:XFD78 A18:E22 G17:XFD22">
+    <cfRule type="expression" dxfId="21" priority="11">
+      <formula>_xlfn.ISFORMULA(A1)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:N2 P2:XFD2 C17:E17 A79:B80 D79:XFD80 A17 A23:XFD33 A81:XFD1048576 A12:XFD16 B11:C11 E11:XFD11 A3:XFD10 A37:XFD78 A18:E22 G17:XFD22">
+    <cfRule type="expression" dxfId="20" priority="12">
+      <formula>AND(COUNTA($A2:$AA2)=0, NOT(ISBLANK($A3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B15">
+    <cfRule type="expression" dxfId="19" priority="197">
+      <formula>AND(COUNTA($A17:$AA17)=0, NOT(ISBLANK($A18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C15">
+    <cfRule type="expression" dxfId="18" priority="10">
+      <formula>AND(COUNTA($A17:$AA17)=0, NOT(ISBLANK($A18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D15:F15">
+    <cfRule type="expression" dxfId="17" priority="9">
+      <formula>AND(COUNTA($A17:$AA17)=0, NOT(ISBLANK($A18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C79:C80">
+    <cfRule type="expression" dxfId="16" priority="7">
+      <formula>_xlfn.ISFORMULA(C79)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C79:C80">
+    <cfRule type="expression" dxfId="15" priority="8">
+      <formula>AND(COUNTA($A79:$AA79)=0, NOT(ISBLANK($A80)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1048576:XFD1048576">
+    <cfRule type="expression" dxfId="14" priority="198">
+      <formula>AND(COUNTA(#REF!)=0, NOT(ISBLANK($A1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A36:XFD36">
+    <cfRule type="expression" dxfId="13" priority="202">
+      <formula>AND(COUNTA($A36:$AA36)=0, NOT(ISBLANK($A38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A34:XFD35">
+    <cfRule type="expression" dxfId="12" priority="205">
+      <formula>AND(COUNTA($A34:$AA34)=0, NOT(ISBLANK($A37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D11">
+    <cfRule type="expression" dxfId="5" priority="5">
+      <formula>_xlfn.ISFORMULA(D11)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D11">
+    <cfRule type="expression" dxfId="4" priority="6">
+      <formula>AND(COUNTA($A11:$AA11)=0, NOT(ISBLANK($A12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F17:F21">
+    <cfRule type="expression" dxfId="3" priority="3">
+      <formula>_xlfn.ISFORMULA(F17)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F17:F21">
+    <cfRule type="expression" dxfId="2" priority="4">
+      <formula>AND(COUNTA($A17:$AA17)=0, NOT(ISBLANK($A18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F22">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>_xlfn.ISFORMULA(F22)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F22">
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>AND(COUNTA($A22:$AA22)=0, NOT(ISBLANK($A23)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BE5A693-F7F5-4E49-9BB0-AEC7C8F410F3}">
   <dimension ref="A1:X145"/>
   <sheetViews>
@@ -20797,32 +22504,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="11" priority="6">
       <formula>_xlfn.ISFORMULA(A1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G63:G67">
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="10" priority="5">
       <formula>_xlfn.ISFORMULA(G63)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G30:G31">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="9" priority="4">
       <formula>_xlfn.ISFORMULA(G30)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G26:G27">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="8" priority="2">
       <formula>_xlfn.ISFORMULA(G26)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G33:G58">
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="7" priority="3">
       <formula>_xlfn.ISFORMULA(G33)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M32">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="6" priority="1">
       <formula>_xlfn.ISFORMULA(M32)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Sharing complete: CFS, GSP, PCE, SGF, UTD
</commit_message>
<xml_diff>
--- a/data/readfiles/generate_yaml.xlsx
+++ b/data/readfiles/generate_yaml.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chughes/Documents/Git/SLiDE/data/readfiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C2BF313-1118-204F-9E30-84D6C8301A13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0179C0C-8FE2-6846-91FE-EE503E873E86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18900" activeTab="6" xr2:uid="{ECEEE8D6-CC61-454D-945D-45D0FFF64D45}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3080" uniqueCount="1178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3110" uniqueCount="1183">
   <si>
     <t>bea_supply</t>
   </si>
@@ -3501,9 +3501,6 @@
     <t xml:space="preserve">    kind:   inner</t>
   </si>
   <si>
-    <t xml:space="preserve">  input:  [yr, r, gdpcat, s, units]</t>
-  </si>
-  <si>
     <t xml:space="preserve">    input:  sg</t>
   </si>
   <si>
@@ -3555,25 +3552,43 @@
     <t>PathOut: [data, share, gsp.csv]</t>
   </si>
   <si>
+    <t>PathOut: [data, share, utd.csv]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  input:  [yr, r, s, t, units]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - {col: g,     type: String}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - {col: t,     type: String}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - {col: s,     type: String}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - file:   [crosswalk, sgf.csv]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    input:  ec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  input:  [yr, r, s, gdpcat, units]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - {col: s,      type: String}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - {col: g,          type: String}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - {col: share, type: Float64}</t>
+  </si>
+  <si>
+    <t># - {col: units, type: String}</t>
+  </si>
+  <si>
     <t>PathOut: [data, share, sgf.csv]</t>
-  </si>
-  <si>
-    <t>PathOut: [data, share, utd.csv]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  input:  [yr, r, s, t, units]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  - {col: value, type: String}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  - {col: g,     type: String}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  - {col: t,     type: String}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  - {col: s,     type: String}</t>
   </si>
 </sst>
 </file>
@@ -3827,21 +3842,11 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="49">
+  <dxfs count="47">
     <dxf>
       <fill>
         <patternFill>
           <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3853,12 +3858,16 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color theme="9"/>
-      </font>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3940,30 +3949,42 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3985,23 +4006,12 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -6266,15 +6276,15 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="48" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="1" operator="equal">
       <formula>" "</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="3">
+    <cfRule type="expression" dxfId="45" priority="3">
       <formula>_xlfn.ISFORMULA(A1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:XFD1048576">
-    <cfRule type="expression" dxfId="46" priority="2">
+    <cfRule type="expression" dxfId="44" priority="2">
       <formula>AND(ISBLANK($A2), NOT(ISBLANK($A3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7654,15 +7664,15 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="45" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="2" operator="equal">
       <formula>" "</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="56">
+    <cfRule type="expression" dxfId="42" priority="56">
       <formula>_xlfn.ISFORMULA(A1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:XFD1048576">
-    <cfRule type="expression" dxfId="43" priority="3">
+    <cfRule type="expression" dxfId="41" priority="3">
       <formula>AND(ISBLANK($A2), NOT(ISBLANK($A3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8707,15 +8717,15 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="42" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="1" operator="equal">
       <formula>" "</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="36">
+    <cfRule type="expression" dxfId="39" priority="36">
       <formula>_xlfn.ISFORMULA(A1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:XFD1048576">
-    <cfRule type="expression" dxfId="40" priority="2">
+    <cfRule type="expression" dxfId="38" priority="2">
       <formula>AND(ISBLANK($A3), NOT(ISBLANK($A4)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9422,77 +9432,77 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D81:D83">
-    <cfRule type="expression" dxfId="39" priority="5">
+    <cfRule type="expression" dxfId="37" priority="5">
       <formula>_xlfn.ISFORMULA(D81)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:C7">
-    <cfRule type="expression" dxfId="38" priority="16">
+    <cfRule type="expression" dxfId="36" priority="16">
       <formula>_xlfn.ISFORMULA(C6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18:E22">
-    <cfRule type="expression" dxfId="37" priority="15">
+    <cfRule type="expression" dxfId="35" priority="15">
       <formula>_xlfn.ISFORMULA(E18)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:C31">
-    <cfRule type="expression" dxfId="36" priority="14">
+    <cfRule type="expression" dxfId="34" priority="14">
       <formula>_xlfn.ISFORMULA(C28)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C82:C84">
-    <cfRule type="expression" dxfId="35" priority="13">
+    <cfRule type="expression" dxfId="33" priority="13">
       <formula>_xlfn.ISFORMULA(C82)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="expression" dxfId="34" priority="11">
+    <cfRule type="expression" dxfId="32" priority="11">
       <formula>_xlfn.ISFORMULA(D7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="expression" dxfId="33" priority="12">
+    <cfRule type="expression" dxfId="31" priority="12">
       <formula>_xlfn.ISFORMULA(D6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9:D13">
-    <cfRule type="expression" dxfId="32" priority="10">
+    <cfRule type="expression" dxfId="30" priority="10">
       <formula>_xlfn.ISFORMULA(D9)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32">
-    <cfRule type="expression" dxfId="31" priority="9">
+    <cfRule type="expression" dxfId="29" priority="9">
       <formula>_xlfn.ISFORMULA(D32)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D28 D32">
-    <cfRule type="expression" dxfId="30" priority="8">
+    <cfRule type="expression" dxfId="28" priority="8">
       <formula>_xlfn.ISFORMULA(D28)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30">
-    <cfRule type="expression" dxfId="29" priority="7">
+    <cfRule type="expression" dxfId="27" priority="7">
       <formula>_xlfn.ISFORMULA(D30)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9:C10">
-    <cfRule type="expression" dxfId="28" priority="4">
+    <cfRule type="expression" dxfId="26" priority="4">
       <formula>_xlfn.ISFORMULA(C9)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D45 D48:D49">
-    <cfRule type="expression" dxfId="27" priority="3">
+    <cfRule type="expression" dxfId="25" priority="3">
       <formula>_xlfn.ISFORMULA(D45)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23">
-    <cfRule type="expression" dxfId="26" priority="2">
+    <cfRule type="expression" dxfId="24" priority="2">
       <formula>_xlfn.ISFORMULA(C23)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B82:B84">
-    <cfRule type="expression" dxfId="25" priority="1">
+    <cfRule type="expression" dxfId="23" priority="1">
       <formula>_xlfn.ISFORMULA(B82)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9505,11 +9515,11 @@
   <dimension ref="A1:Y153"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B10" sqref="B10"/>
       <selection pane="topRight" activeCell="B10" sqref="B10"/>
       <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
-      <selection pane="bottomRight" activeCell="D106" sqref="D106"/>
+      <selection pane="bottomRight" activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="46.83203125" defaultRowHeight="13" customHeight="1"/>
@@ -15607,17 +15617,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1 A3:XFD1048576 A2:N2 P2:XFD2">
-    <cfRule type="expression" dxfId="24" priority="1">
+    <cfRule type="expression" dxfId="22" priority="1">
       <formula>_xlfn.ISFORMULA(A1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:XFD1048576 A2:N2 P2:XFD2">
-    <cfRule type="expression" dxfId="23" priority="168">
+    <cfRule type="expression" dxfId="21" priority="168">
       <formula>AND(COUNTA($A2:$AA2)=0, NOT(ISBLANK($A3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1048576:XFD1048576">
-    <cfRule type="expression" dxfId="22" priority="181">
+    <cfRule type="expression" dxfId="20" priority="181">
       <formula>AND(COUNTA(#REF!)=0, NOT(ISBLANK($A1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15630,11 +15640,11 @@
   <dimension ref="A1:Y155"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B10" sqref="B10"/>
       <selection pane="topRight" activeCell="B10" sqref="B10"/>
       <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
-      <selection pane="bottomRight" activeCell="F21" sqref="F21"/>
+      <selection pane="bottomRight" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="46.83203125" defaultRowHeight="13" customHeight="1"/>
@@ -15816,19 +15826,19 @@
         <v>169</v>
       </c>
       <c r="B11" s="36" t="s">
+        <v>1167</v>
+      </c>
+      <c r="C11" s="36" t="s">
+        <v>1169</v>
+      </c>
+      <c r="D11" s="36" t="s">
         <v>1168</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="E11" s="36" t="s">
+        <v>1182</v>
+      </c>
+      <c r="F11" s="36" t="s">
         <v>1170</v>
-      </c>
-      <c r="D11" s="36" t="s">
-        <v>1169</v>
-      </c>
-      <c r="E11" s="36" t="s">
-        <v>1171</v>
-      </c>
-      <c r="F11" s="36" t="s">
-        <v>1172</v>
       </c>
     </row>
     <row r="13" spans="1:25" ht="13" customHeight="1">
@@ -15893,48 +15903,115 @@
       <c r="A17" s="36" t="s">
         <v>172</v>
       </c>
+      <c r="B17" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="D17" s="36" t="s">
         <v>9</v>
       </c>
+      <c r="E17" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="F17" s="36" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:24" ht="13" customHeight="1">
+      <c r="B18" s="36" t="s">
+        <v>514</v>
+      </c>
+      <c r="C18" s="36" t="s">
+        <v>585</v>
+      </c>
       <c r="D18" s="36" t="s">
         <v>595</v>
       </c>
+      <c r="E18" s="36" t="s">
+        <v>595</v>
+      </c>
       <c r="F18" s="36" t="s">
         <v>595</v>
       </c>
     </row>
     <row r="19" spans="1:24" ht="13" customHeight="1">
+      <c r="B19" s="36" t="s">
+        <v>513</v>
+      </c>
+      <c r="C19" s="36" t="s">
+        <v>614</v>
+      </c>
       <c r="D19" s="36" t="s">
         <v>714</v>
       </c>
+      <c r="E19" s="36" t="s">
+        <v>714</v>
+      </c>
       <c r="F19" s="36" t="s">
         <v>714</v>
       </c>
     </row>
     <row r="20" spans="1:24" ht="13" customHeight="1">
+      <c r="B20" s="36" t="s">
+        <v>1179</v>
+      </c>
+      <c r="C20" s="36" t="s">
+        <v>1178</v>
+      </c>
       <c r="D20" s="36" t="s">
-        <v>1175</v>
+        <v>1172</v>
+      </c>
+      <c r="E20" s="36" t="s">
+        <v>1172</v>
       </c>
       <c r="F20" s="36" t="s">
-        <v>1177</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="21" spans="1:24" ht="13" customHeight="1">
+      <c r="B21" s="36" t="s">
+        <v>515</v>
+      </c>
+      <c r="C21" s="36" t="s">
+        <v>612</v>
+      </c>
       <c r="D21" s="36" t="s">
-        <v>1174</v>
+        <v>147</v>
+      </c>
+      <c r="E21" s="36" t="s">
+        <v>1181</v>
       </c>
       <c r="F21" s="36" t="s">
-        <v>1176</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="22" spans="1:24" ht="13" customHeight="1">
+      <c r="B22" s="36" t="s">
+        <v>516</v>
+      </c>
+      <c r="C22" s="36" t="s">
+        <v>148</v>
+      </c>
+      <c r="E22" s="36" t="s">
+        <v>147</v>
+      </c>
       <c r="F22" s="36" t="s">
-        <v>1174</v>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" ht="13" customHeight="1">
+      <c r="C23" s="36" t="s">
+        <v>149</v>
+      </c>
+      <c r="F23" s="36" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" ht="13" customHeight="1">
+      <c r="F24" s="36" t="s">
+        <v>1180</v>
       </c>
     </row>
     <row r="26" spans="1:24" ht="13" customHeight="1">
@@ -16041,7 +16118,7 @@
     <row r="35" spans="1:25" ht="13" customHeight="1">
       <c r="B35" s="33"/>
       <c r="F35" s="36" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="K35" s="33"/>
       <c r="L35" s="33"/>
@@ -16060,7 +16137,7 @@
     <row r="36" spans="1:25" ht="13" customHeight="1">
       <c r="B36" s="33"/>
       <c r="F36" s="36" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="K36" s="33"/>
       <c r="L36" s="33"/>
@@ -16103,6 +16180,9 @@
       <c r="D38" s="36" t="s">
         <v>398</v>
       </c>
+      <c r="E38" s="36" t="s">
+        <v>398</v>
+      </c>
       <c r="F38" s="36" t="s">
         <v>398</v>
       </c>
@@ -16125,10 +16205,13 @@
         <v>1053</v>
       </c>
       <c r="D39" s="36" t="s">
-        <v>1159</v>
+        <v>1158</v>
+      </c>
+      <c r="E39" s="36" t="s">
+        <v>1175</v>
       </c>
       <c r="F39" s="36" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="K39" s="33"/>
       <c r="L39" s="33"/>
@@ -16149,7 +16232,10 @@
         <v>1149</v>
       </c>
       <c r="D40" s="36" t="s">
-        <v>1160</v>
+        <v>1159</v>
+      </c>
+      <c r="E40" s="36" t="s">
+        <v>957</v>
       </c>
       <c r="F40" s="36" t="s">
         <v>936</v>
@@ -16173,7 +16259,10 @@
         <v>984</v>
       </c>
       <c r="D41" s="36" t="s">
-        <v>1161</v>
+        <v>1160</v>
+      </c>
+      <c r="E41" s="36" t="s">
+        <v>984</v>
       </c>
       <c r="F41" s="36" t="s">
         <v>984</v>
@@ -16190,16 +16279,19 @@
     <row r="42" spans="1:25" ht="13" customHeight="1">
       <c r="A42" s="38"/>
       <c r="B42" s="36" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="C42" s="36" t="s">
         <v>1150</v>
       </c>
       <c r="D42" s="36" t="s">
-        <v>1162</v>
+        <v>1161</v>
+      </c>
+      <c r="E42" s="36" t="s">
+        <v>1176</v>
       </c>
       <c r="F42" s="36" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="K42" s="33"/>
       <c r="L42" s="33"/>
@@ -16215,13 +16307,16 @@
     <row r="43" spans="1:25" ht="13" customHeight="1">
       <c r="A43" s="38"/>
       <c r="B43" s="36" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="C43" s="36" t="s">
         <v>1151</v>
       </c>
       <c r="D43" s="36" t="s">
-        <v>1155</v>
+        <v>1154</v>
+      </c>
+      <c r="E43" s="36" t="s">
+        <v>1154</v>
       </c>
       <c r="F43" s="36" t="s">
         <v>1151</v>
@@ -16246,6 +16341,10 @@
         <v xml:space="preserve">    kind:   inner</v>
       </c>
       <c r="D44" s="36" t="str">
+        <f>$B$44</f>
+        <v xml:space="preserve">    kind:   inner</v>
+      </c>
+      <c r="E44" s="36" t="str">
         <f>$B$44</f>
         <v xml:space="preserve">    kind:   inner</v>
       </c>
@@ -16307,6 +16406,9 @@
       <c r="B48" s="36" t="s">
         <v>18</v>
       </c>
+      <c r="E48" s="36" t="s">
+        <v>18</v>
+      </c>
       <c r="K48" s="33"/>
       <c r="L48" s="33"/>
       <c r="M48" s="33"/>
@@ -16320,7 +16422,11 @@
     <row r="49" spans="1:22" ht="13" customHeight="1">
       <c r="A49" s="38"/>
       <c r="B49" s="36" t="s">
-        <v>1157</v>
+        <v>1156</v>
+      </c>
+      <c r="E49" s="36" t="str">
+        <f>$B49</f>
+        <v xml:space="preserve">  col: g</v>
       </c>
       <c r="K49" s="33"/>
       <c r="L49" s="33"/>
@@ -16335,7 +16441,11 @@
     <row r="50" spans="1:22" ht="13" customHeight="1">
       <c r="A50" s="38"/>
       <c r="B50" s="36" t="s">
-        <v>1158</v>
+        <v>1157</v>
+      </c>
+      <c r="E50" s="36" t="str">
+        <f t="shared" ref="E50:E51" si="0">$B50</f>
+        <v xml:space="preserve">  val: missing</v>
       </c>
       <c r="K50" s="33"/>
       <c r="L50" s="33"/>
@@ -16351,6 +16461,10 @@
       <c r="A51" s="38"/>
       <c r="B51" s="36" t="s">
         <v>101</v>
+      </c>
+      <c r="E51" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  operation: "=="</v>
       </c>
       <c r="L51" s="33"/>
       <c r="O51" s="33"/>
@@ -16385,6 +16499,9 @@
       <c r="D53" s="36" t="s">
         <v>436</v>
       </c>
+      <c r="E53" s="36" t="s">
+        <v>436</v>
+      </c>
       <c r="F53" s="36" t="s">
         <v>436</v>
       </c>
@@ -16406,6 +16523,10 @@
         <v xml:space="preserve">  operation: sum</v>
       </c>
       <c r="D54" s="36" t="str">
+        <f>$B54</f>
+        <v xml:space="preserve">  operation: sum</v>
+      </c>
+      <c r="E54" s="36" t="str">
         <f>$B54</f>
         <v xml:space="preserve">  operation: sum</v>
       </c>
@@ -16429,15 +16550,19 @@
         <v>523</v>
       </c>
       <c r="C55" s="36" t="str">
-        <f t="shared" ref="C55:F57" si="0">$B55</f>
+        <f t="shared" ref="C55:F57" si="1">$B55</f>
         <v xml:space="preserve">  axis:   row</v>
       </c>
       <c r="D55" s="36" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">  axis:   row</v>
       </c>
+      <c r="E55" s="36" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  axis:   row</v>
+      </c>
       <c r="F55" s="36" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">  axis:   row</v>
       </c>
       <c r="K55" s="33"/>
@@ -16456,15 +16581,19 @@
         <v>525</v>
       </c>
       <c r="C56" s="36" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">  from:   nothing</v>
       </c>
       <c r="D56" s="36" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">  from:   nothing</v>
       </c>
+      <c r="E56" s="36" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  from:   nothing</v>
+      </c>
       <c r="F56" s="36" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">  from:   nothing</v>
       </c>
       <c r="K56" s="33"/>
@@ -16482,15 +16611,19 @@
         <v>524</v>
       </c>
       <c r="C57" s="36" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">  to:     nothing</v>
       </c>
       <c r="D57" s="36" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">  to:     nothing</v>
       </c>
+      <c r="E57" s="36" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  to:     nothing</v>
+      </c>
       <c r="F57" s="36" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">  to:     nothing</v>
       </c>
       <c r="K57" s="33"/>
@@ -16505,16 +16638,19 @@
     </row>
     <row r="58" spans="1:22" ht="13" customHeight="1">
       <c r="B58" s="36" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="C58" s="36" t="s">
-        <v>1153</v>
+        <v>1177</v>
       </c>
       <c r="D58" s="36" t="s">
-        <v>1163</v>
+        <v>1162</v>
+      </c>
+      <c r="E58" s="36" t="s">
+        <v>1162</v>
       </c>
       <c r="F58" s="36" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
       <c r="K58" s="33"/>
       <c r="L58" s="33"/>
@@ -16535,6 +16671,10 @@
         <v xml:space="preserve">  output: value</v>
       </c>
       <c r="D59" s="36" t="str">
+        <f>$B59</f>
+        <v xml:space="preserve">  output: value</v>
+      </c>
+      <c r="E59" s="36" t="str">
         <f>$B59</f>
         <v xml:space="preserve">  output: value</v>
       </c>
@@ -17012,84 +17152,74 @@
       <c r="S155" s="32"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:XFD1 A2:N2 P2:XFD2 C17:E17 A79:B80 D79:XFD80 A81:XFD1048576 A17 A12:XFD16 E11:XFD11 A11:C11 A3:XFD10 A23:XFD78 A18:E22 G17:XFD22">
-    <cfRule type="expression" dxfId="21" priority="11">
+  <conditionalFormatting sqref="P2:XFD2 C17 A79:B80 A17 A11:C11 G24:XFD24 A18:C21 H17:XFD23 A22:D23 A7:D10 A12:D15 E7:XFD15 A1:XFD1 A2:N2 D79:XFD80 A81:XFD1048576 A16:XFD16 A3:XFD6 A24:E24 A25:XFD78 E17:E22">
+    <cfRule type="expression" dxfId="19" priority="26">
       <formula>_xlfn.ISFORMULA(A1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:N2 P2:XFD2 C17:E17 A79:B80 D79:XFD80 A17 A23:XFD33 A81:XFD1048576 A12:XFD16 B11:C11 E11:XFD11 A3:XFD10 A37:XFD78 A18:E22 G17:XFD22">
-    <cfRule type="expression" dxfId="20" priority="12">
+  <conditionalFormatting sqref="C79:C80">
+    <cfRule type="expression" dxfId="18" priority="22">
+      <formula>_xlfn.ISFORMULA(C79)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1048576:XFD1048576">
+    <cfRule type="expression" dxfId="17" priority="213">
+      <formula>AND(COUNTA(#REF!)=0, NOT(ISBLANK($A1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D11">
+    <cfRule type="expression" dxfId="16" priority="20">
+      <formula>_xlfn.ISFORMULA(D11)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F17:F21">
+    <cfRule type="expression" dxfId="15" priority="18">
+      <formula>_xlfn.ISFORMULA(F17)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F22">
+    <cfRule type="expression" dxfId="14" priority="16">
+      <formula>_xlfn.ISFORMULA(F22)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F23:F24">
+    <cfRule type="expression" dxfId="13" priority="14">
+      <formula>_xlfn.ISFORMULA(F23)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G17:G23">
+    <cfRule type="expression" dxfId="12" priority="10">
+      <formula>_xlfn.ISFORMULA(G17)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D17:D21">
+    <cfRule type="expression" dxfId="11" priority="8">
+      <formula>_xlfn.ISFORMULA(D17)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:N2 P2:XFD2 C17 A17 E3:XFD16 E25:XFD33 E24 A2:D10 A12:D16 A37:XFD1048576 A18:C19 D17:XFD19 F20:XFD24 A20:D33 B11:D11">
+    <cfRule type="expression" dxfId="4" priority="273">
       <formula>AND(COUNTA($A2:$AA2)=0, NOT(ISBLANK($A3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B15">
-    <cfRule type="expression" dxfId="19" priority="197">
+  <conditionalFormatting sqref="B15:F15">
+    <cfRule type="expression" dxfId="3" priority="353">
       <formula>AND(COUNTA($A17:$AA17)=0, NOT(ISBLANK($A18)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C15">
-    <cfRule type="expression" dxfId="18" priority="10">
-      <formula>AND(COUNTA($A17:$AA17)=0, NOT(ISBLANK($A18)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D15:F15">
-    <cfRule type="expression" dxfId="17" priority="9">
-      <formula>AND(COUNTA($A17:$AA17)=0, NOT(ISBLANK($A18)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C79:C80">
-    <cfRule type="expression" dxfId="16" priority="7">
-      <formula>_xlfn.ISFORMULA(C79)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C79:C80">
-    <cfRule type="expression" dxfId="15" priority="8">
-      <formula>AND(COUNTA($A79:$AA79)=0, NOT(ISBLANK($A80)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1048576:XFD1048576">
-    <cfRule type="expression" dxfId="14" priority="198">
-      <formula>AND(COUNTA(#REF!)=0, NOT(ISBLANK($A1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A36:XFD36">
-    <cfRule type="expression" dxfId="13" priority="202">
+    <cfRule type="expression" dxfId="2" priority="361">
       <formula>AND(COUNTA($A36:$AA36)=0, NOT(ISBLANK($A38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A34:XFD35">
-    <cfRule type="expression" dxfId="12" priority="205">
+    <cfRule type="expression" dxfId="1" priority="368">
       <formula>AND(COUNTA($A34:$AA34)=0, NOT(ISBLANK($A37)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D11">
-    <cfRule type="expression" dxfId="5" priority="5">
-      <formula>_xlfn.ISFORMULA(D11)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D11">
-    <cfRule type="expression" dxfId="4" priority="6">
-      <formula>AND(COUNTA($A11:$AA11)=0, NOT(ISBLANK($A12)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F17:F21">
-    <cfRule type="expression" dxfId="3" priority="3">
-      <formula>_xlfn.ISFORMULA(F17)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F17:F21">
-    <cfRule type="expression" dxfId="2" priority="4">
-      <formula>AND(COUNTA($A17:$AA17)=0, NOT(ISBLANK($A18)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F22">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>_xlfn.ISFORMULA(F22)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F22">
-    <cfRule type="expression" dxfId="0" priority="2">
-      <formula>AND(COUNTA($A22:$AA22)=0, NOT(ISBLANK($A23)))</formula>
+  <conditionalFormatting sqref="E20:E22">
+    <cfRule type="expression" dxfId="0" priority="376">
+      <formula>AND(COUNTA($A21:$AA21)=0, NOT(ISBLANK($A22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -22504,32 +22634,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="expression" dxfId="11" priority="6">
+    <cfRule type="expression" dxfId="10" priority="6">
       <formula>_xlfn.ISFORMULA(A1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G63:G67">
-    <cfRule type="expression" dxfId="10" priority="5">
+    <cfRule type="expression" dxfId="9" priority="5">
       <formula>_xlfn.ISFORMULA(G63)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G30:G31">
-    <cfRule type="expression" dxfId="9" priority="4">
+    <cfRule type="expression" dxfId="8" priority="4">
       <formula>_xlfn.ISFORMULA(G30)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G26:G27">
-    <cfRule type="expression" dxfId="8" priority="2">
+    <cfRule type="expression" dxfId="7" priority="2">
       <formula>_xlfn.ISFORMULA(G26)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G33:G58">
-    <cfRule type="expression" dxfId="7" priority="3">
+    <cfRule type="expression" dxfId="6" priority="3">
       <formula>_xlfn.ISFORMULA(G33)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M32">
-    <cfRule type="expression" dxfId="6" priority="1">
+    <cfRule type="expression" dxfId="5" priority="1">
       <formula>_xlfn.ISFORMULA(M32)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
calibrate nat'l data over all years; extract data from JuMP dense arrays; begun disaggregation
</commit_message>
<xml_diff>
--- a/data/readfiles/generate_yaml.xlsx
+++ b/data/readfiles/generate_yaml.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chughes/Documents/Git/SLiDE/data/readfiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0179C0C-8FE2-6846-91FE-EE503E873E86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F335D12-593A-C84C-9198-54AEA6F0E186}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18900" activeTab="6" xr2:uid="{ECEEE8D6-CC61-454D-945D-45D0FFF64D45}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18900" activeTab="5" xr2:uid="{ECEEE8D6-CC61-454D-945D-45D0FFF64D45}"/>
   </bookViews>
   <sheets>
     <sheet name="map_bluenote" sheetId="5" state="hidden" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3110" uniqueCount="1183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3110" uniqueCount="1206">
   <si>
     <t>bea_supply</t>
   </si>
@@ -2556,9 +2556,6 @@
     <t>PathIn:  [data, datasources, PCE]</t>
   </si>
   <si>
-    <t>PathIn:  [data, output]</t>
-  </si>
-  <si>
     <t>PathIn:  [data, datasources, NASS]</t>
   </si>
   <si>
@@ -3589,6 +3586,78 @@
   </si>
   <si>
     <t>PathOut: [data, share, sgf.csv]</t>
+  </si>
+  <si>
+    <t>PathIn:  [data, input]</t>
+  </si>
+  <si>
+    <t>PathOut: [data, input, supply.csv]</t>
+  </si>
+  <si>
+    <t>PathOut: [data, input, use.csv]</t>
+  </si>
+  <si>
+    <t>PathOut: [data, input, supply_det.csv]</t>
+  </si>
+  <si>
+    <t>PathOut: [data, input, use_det.csv]</t>
+  </si>
+  <si>
+    <t>PathOut: [data, input, gsp_state.csv]</t>
+  </si>
+  <si>
+    <t>PathOut: [data, input, gsp_metro.csv]</t>
+  </si>
+  <si>
+    <t>PathOut: [data, input, gsp_county.csv]</t>
+  </si>
+  <si>
+    <t>PathOut: [data, input, pce.csv]</t>
+  </si>
+  <si>
+    <t>PathOut: [data, input, cfs.csv]</t>
+  </si>
+  <si>
+    <t>PathOut: [data, input, cfs_state.csv]</t>
+  </si>
+  <si>
+    <t>PathOut: [data, input, cfs_metro.csv]</t>
+  </si>
+  <si>
+    <t>PathOut: [data, input, nass.csv]</t>
+  </si>
+  <si>
+    <t>PathOut: [data, input, sgf_1997.csv]</t>
+  </si>
+  <si>
+    <t>PathOut: [data, input, sgf_1998.csv]</t>
+  </si>
+  <si>
+    <t>PathOut: [data, input, sgf_1999-2011.csv]</t>
+  </si>
+  <si>
+    <t>PathOut: [data, input, sgf_2012-2013.csv]</t>
+  </si>
+  <si>
+    <t>PathOut: [data, input, sgf_2014-2016.csv]</t>
+  </si>
+  <si>
+    <t>PathOut: [data, input, sgf.csv]</t>
+  </si>
+  <si>
+    <t>PathOut: [data, input, utd.csv]</t>
+  </si>
+  <si>
+    <t>PathOut: [data, input, crude_oil.csv]</t>
+  </si>
+  <si>
+    <t>PathOut: [data, input, emissions.csv]</t>
+  </si>
+  <si>
+    <t>PathOut: [data, input, heatrate.csv]</t>
+  </si>
+  <si>
+    <t>PathOut: [data, input, seds.csv]</t>
   </si>
 </sst>
 </file>
@@ -3844,41 +3913,6 @@
   </cellStyles>
   <dxfs count="47">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color theme="9"/>
       </font>
@@ -3935,6 +3969,41 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4801,7 +4870,7 @@
         <v>470</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="E11" s="12" t="s">
         <v>465</v>
@@ -4867,11 +4936,11 @@
     <row r="19" spans="1:8" ht="13">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="C19" s="2"/>
       <c r="H19" s="12" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="13">
@@ -4881,7 +4950,7 @@
       </c>
       <c r="C20" s="2"/>
       <c r="H20" s="12" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="13">
@@ -4891,7 +4960,7 @@
       </c>
       <c r="C21" s="2"/>
       <c r="H21" s="12" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="13">
@@ -5158,7 +5227,7 @@
     <row r="63" spans="1:3" ht="13">
       <c r="A63" s="2"/>
       <c r="B63" s="2" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="C63" s="2"/>
     </row>
@@ -5346,7 +5415,7 @@
         <v>795</v>
       </c>
       <c r="G2" s="33" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="13" customHeight="1">
@@ -5354,7 +5423,7 @@
         <v>796</v>
       </c>
       <c r="G3" s="33" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="13" customHeight="1">
@@ -5403,7 +5472,7 @@
     </row>
     <row r="5" spans="1:14" ht="13" customHeight="1">
       <c r="A5" s="49" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="13" customHeight="1">
@@ -5705,7 +5774,7 @@
         <v>496</v>
       </c>
       <c r="J19" s="33" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="K19" s="33" t="s">
         <v>394</v>
@@ -5745,13 +5814,13 @@
     </row>
     <row r="21" spans="1:14" ht="13" customHeight="1">
       <c r="B21" s="33" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="C21" s="33" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="D21" s="33" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="F21" s="33" t="s">
         <v>120</v>
@@ -5875,13 +5944,13 @@
     </row>
     <row r="31" spans="1:14" ht="13" customHeight="1">
       <c r="B31" s="33" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="C31" s="33" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="D31" s="33" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="F31" s="33" t="s">
         <v>410</v>
@@ -5902,26 +5971,26 @@
     </row>
     <row r="36" spans="1:12" ht="13" customHeight="1">
       <c r="A36" s="49" t="s">
+        <v>950</v>
+      </c>
+      <c r="K36" s="33" t="s">
         <v>951</v>
-      </c>
-      <c r="K36" s="33" t="s">
-        <v>952</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="13" customHeight="1">
       <c r="K37" s="33" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="13" customHeight="1">
       <c r="K38" s="33" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="L38" s="54"/>
     </row>
     <row r="39" spans="1:12" ht="13" customHeight="1">
       <c r="K39" s="33" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="13" customHeight="1">
@@ -5967,7 +6036,7 @@
     </row>
     <row r="50" spans="1:14" ht="13" customHeight="1">
       <c r="G50" s="55" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
     </row>
     <row r="52" spans="1:14" ht="13" customHeight="1">
@@ -6023,10 +6092,10 @@
     </row>
     <row r="58" spans="1:14" ht="13" customHeight="1">
       <c r="K58" s="33" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="N58" s="36" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="59" spans="1:14" ht="13" customHeight="1">
@@ -6056,7 +6125,7 @@
     </row>
     <row r="64" spans="1:14" ht="13" customHeight="1">
       <c r="K64" s="33" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="65" spans="1:14" ht="13" customHeight="1">
@@ -6086,7 +6155,7 @@
     </row>
     <row r="70" spans="1:14" ht="13" customHeight="1">
       <c r="K70" s="33" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="72" spans="1:14" ht="13" customHeight="1">
@@ -6117,7 +6186,7 @@
         <v>557</v>
       </c>
       <c r="G73" s="33" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="I73" s="33" t="s">
         <v>500</v>
@@ -6128,13 +6197,13 @@
     </row>
     <row r="74" spans="1:14" ht="13" customHeight="1">
       <c r="B74" s="33" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="C74" s="33" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="G74" s="33" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="I74" s="33" t="s">
         <v>498</v>
@@ -6145,7 +6214,7 @@
     </row>
     <row r="75" spans="1:14" ht="13" customHeight="1">
       <c r="G75" s="33" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="I75" s="33" t="s">
         <v>499</v>
@@ -6156,7 +6225,7 @@
     </row>
     <row r="76" spans="1:14" ht="13" customHeight="1">
       <c r="G76" s="33" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="N76" s="33" t="s">
         <v>431</v>
@@ -6164,7 +6233,7 @@
     </row>
     <row r="77" spans="1:14" ht="13" customHeight="1">
       <c r="G77" s="33" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="N77" s="33" t="s">
         <v>311</v>
@@ -6172,7 +6241,7 @@
     </row>
     <row r="78" spans="1:14" ht="13" customHeight="1">
       <c r="G78" s="33" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="N78" s="33" t="s">
         <v>432</v>
@@ -6180,27 +6249,27 @@
     </row>
     <row r="79" spans="1:14" ht="13" customHeight="1">
       <c r="G79" s="33" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="80" spans="1:14" ht="13" customHeight="1">
       <c r="G80" s="33" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="81" spans="1:14" ht="13" customHeight="1">
       <c r="G81" s="33" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="82" spans="1:14" ht="13" customHeight="1">
       <c r="G82" s="33" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="83" spans="1:14" ht="13" customHeight="1">
       <c r="G83" s="33" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="85" spans="1:14" ht="13" customHeight="1">
@@ -6219,7 +6288,7 @@
     </row>
     <row r="86" spans="1:14" ht="13" customHeight="1">
       <c r="K86" s="33" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="N86" s="33" t="s">
         <v>533</v>
@@ -6235,7 +6304,7 @@
     </row>
     <row r="88" spans="1:14" ht="13" customHeight="1">
       <c r="K88" s="33" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="N88" s="33" t="s">
         <v>20</v>
@@ -6333,22 +6402,22 @@
         <v>222</v>
       </c>
       <c r="G1" s="48" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="H1" s="48" t="s">
         <v>362</v>
       </c>
       <c r="I1" s="48" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="J1" s="48" t="s">
         <v>206</v>
       </c>
       <c r="K1" s="48" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="L1" s="48" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="13" customHeight="1">
@@ -6356,19 +6425,19 @@
         <v>795</v>
       </c>
       <c r="B2" s="33" t="s">
+        <v>847</v>
+      </c>
+      <c r="C2" s="33" t="s">
         <v>848</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="D2" s="33" t="s">
+        <v>850</v>
+      </c>
+      <c r="E2" s="33" t="s">
         <v>849</v>
       </c>
-      <c r="D2" s="33" t="s">
-        <v>851</v>
-      </c>
-      <c r="E2" s="33" t="s">
-        <v>850</v>
-      </c>
       <c r="F2" s="33" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="13" customHeight="1">
@@ -6376,7 +6445,7 @@
         <v>796</v>
       </c>
       <c r="B3" s="33" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C3" s="32" t="str">
         <f>IF(ISBLANK($B3), "", $B3)</f>
@@ -6391,7 +6460,7 @@
         <v>Source: https://www.census.gov/geographies/reference-files/time-series/demo/metro-micro/delineation-files.html</v>
       </c>
       <c r="F3" s="33" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="G3" s="36" t="s">
         <v>814</v>
@@ -6415,7 +6484,7 @@
     </row>
     <row r="4" spans="1:12" ht="13" customHeight="1">
       <c r="A4" s="49" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="C4" s="32"/>
       <c r="D4" s="32"/>
@@ -6466,19 +6535,19 @@
     </row>
     <row r="6" spans="1:12" ht="13" customHeight="1">
       <c r="A6" s="49" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="G6" s="33" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="H6" s="33" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="I6" s="33" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="J6" s="33" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="13" customHeight="1">
@@ -6513,7 +6582,7 @@
         <v>833</v>
       </c>
       <c r="K8" s="36" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="L8" s="33" t="s">
         <v>822</v>
@@ -6536,25 +6605,25 @@
         <v>732</v>
       </c>
       <c r="F9" s="33" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="G9" s="36" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="H9" s="36" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="I9" s="36" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="J9" s="36" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="K9" s="36" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="L9" s="33" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="13" customHeight="1">
@@ -6601,16 +6670,16 @@
     </row>
     <row r="12" spans="1:12" ht="13" customHeight="1">
       <c r="B12" s="33" t="s">
+        <v>1132</v>
+      </c>
+      <c r="C12" s="33" t="s">
         <v>1133</v>
       </c>
-      <c r="C12" s="33" t="s">
+      <c r="D12" s="33" t="s">
         <v>1134</v>
       </c>
-      <c r="D12" s="33" t="s">
+      <c r="E12" s="33" t="s">
         <v>1135</v>
-      </c>
-      <c r="E12" s="33" t="s">
-        <v>1136</v>
       </c>
       <c r="F12" s="33" t="s">
         <v>351</v>
@@ -6628,7 +6697,7 @@
         <v>199</v>
       </c>
       <c r="K12" s="36" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="L12" s="33" t="s">
         <v>215</v>
@@ -6636,75 +6705,75 @@
     </row>
     <row r="13" spans="1:12" ht="13" customHeight="1">
       <c r="B13" s="33" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="D13" s="33" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="E13" s="33" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="F13" s="33" t="s">
         <v>352</v>
       </c>
       <c r="G13" s="36" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="H13" s="36" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="I13" s="36" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="J13" s="36" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="K13" s="36" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="13" customHeight="1">
       <c r="B14" s="33" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="C14" s="33" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="D14" s="33" t="s">
+        <v>1129</v>
+      </c>
+      <c r="E14" s="33" t="s">
         <v>1130</v>
       </c>
-      <c r="E14" s="33" t="s">
-        <v>1131</v>
-      </c>
       <c r="G14" s="36" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="H14" s="36" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="I14" s="36" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="J14" s="36" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="K14" s="36"/>
     </row>
     <row r="15" spans="1:12" ht="13" customHeight="1">
       <c r="G15" s="36" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="H15" s="36" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="I15" s="36" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="J15" s="36" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="K15" s="36"/>
     </row>
@@ -6730,7 +6799,7 @@
     </row>
     <row r="18" spans="1:12" ht="13" customHeight="1">
       <c r="B18" s="33" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="C18" s="32" t="str">
         <f t="shared" si="0"/>
@@ -6785,7 +6854,7 @@
     </row>
     <row r="21" spans="1:12" ht="13" customHeight="1">
       <c r="B21" s="33" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C21" s="32" t="str">
         <f>IF(ISBLANK($B21), "", $B21)</f>
@@ -6806,19 +6875,19 @@
         <v>121</v>
       </c>
       <c r="H21" s="33" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="I21" s="33" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="J21" s="33" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="K21" s="36" t="s">
         <v>335</v>
       </c>
       <c r="L21" s="33" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="13" customHeight="1">
@@ -6841,19 +6910,19 @@
         <v>404</v>
       </c>
       <c r="H22" s="33" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="I22" s="33" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="J22" s="33" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="K22" s="36" t="s">
         <v>336</v>
       </c>
       <c r="L22" s="33" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="13" customHeight="1">
@@ -6873,16 +6942,16 @@
         <v>345</v>
       </c>
       <c r="H23" s="33" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="I23" s="33" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="J23" s="33" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="K23" s="36" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="13" customHeight="1">
@@ -6902,13 +6971,13 @@
         <v>346</v>
       </c>
       <c r="H24" s="33" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="I24" s="33" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="J24" s="33" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="K24" s="36"/>
     </row>
@@ -6929,10 +6998,10 @@
         <v>347</v>
       </c>
       <c r="I25" s="33" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="J25" s="33" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="K25" s="36"/>
     </row>
@@ -6950,13 +7019,13 @@
         <v>246</v>
       </c>
       <c r="F26" s="33" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="I26" s="33" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="J26" s="33" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="K26" s="36"/>
     </row>
@@ -6974,10 +7043,10 @@
         <v>250</v>
       </c>
       <c r="F27" s="33" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="J27" s="33" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="K27" s="36"/>
     </row>
@@ -6998,7 +7067,7 @@
         <v>350</v>
       </c>
       <c r="J28" s="33" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="K28" s="36"/>
     </row>
@@ -7100,20 +7169,20 @@
         <v>268</v>
       </c>
       <c r="G36" s="33" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="H36" s="33" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="I36" s="33" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="J36" s="33" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="K36" s="36"/>
       <c r="L36" s="33" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="13" customHeight="1">
@@ -7130,20 +7199,20 @@
         <v>272</v>
       </c>
       <c r="G37" s="33" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="H37" s="33" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="I37" s="33" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="J37" s="33" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="K37" s="36"/>
       <c r="L37" s="33" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="13" customHeight="1">
@@ -7160,13 +7229,13 @@
         <v>276</v>
       </c>
       <c r="H38" s="33" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="I38" s="33" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="J38" s="33" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="K38" s="36"/>
     </row>
@@ -7184,7 +7253,7 @@
         <v>280</v>
       </c>
       <c r="J39" s="33" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="K39" s="36"/>
     </row>
@@ -7286,61 +7355,61 @@
     </row>
     <row r="50" spans="1:11" ht="13" customHeight="1">
       <c r="H50" s="36" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="I50" s="36" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="J50" s="36" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="K50" s="36"/>
     </row>
     <row r="51" spans="1:11" ht="13" customHeight="1">
       <c r="H51" s="36" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="I51" s="36" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="J51" s="36" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="K51" s="36"/>
     </row>
     <row r="52" spans="1:11" ht="13" customHeight="1">
       <c r="H52" s="36" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="I52" s="36" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="J52" s="36" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="K52" s="36"/>
     </row>
     <row r="53" spans="1:11" ht="13" customHeight="1">
       <c r="H53" s="36" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="I53" s="36" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="J53" s="36" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="K53" s="36"/>
     </row>
     <row r="54" spans="1:11" ht="13" customHeight="1">
       <c r="H54" s="36" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="I54" s="36" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="J54" s="36" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="K54" s="36"/>
     </row>
@@ -7352,13 +7421,13 @@
     </row>
     <row r="56" spans="1:11" ht="13" customHeight="1">
       <c r="A56" s="49" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="H56" s="36"/>
       <c r="I56" s="36"/>
       <c r="J56" s="36"/>
       <c r="K56" s="33" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="57" spans="1:11" ht="13" customHeight="1">
@@ -7366,7 +7435,7 @@
       <c r="I57" s="36"/>
       <c r="J57" s="36"/>
       <c r="K57" s="33" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="58" spans="1:11" ht="13" customHeight="1">
@@ -7374,7 +7443,7 @@
       <c r="I58" s="36"/>
       <c r="J58" s="36"/>
       <c r="K58" s="33" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="59" spans="1:11" ht="13" customHeight="1">
@@ -7382,7 +7451,7 @@
       <c r="I59" s="36"/>
       <c r="J59" s="36"/>
       <c r="K59" s="33" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="61" spans="1:11" ht="13" customHeight="1">
@@ -7480,12 +7549,12 @@
     </row>
     <row r="74" spans="1:12" ht="13" customHeight="1">
       <c r="B74" s="36" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="C74" s="32"/>
       <c r="D74" s="32"/>
       <c r="E74" s="36" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="76" spans="1:12" ht="13" customHeight="1">
@@ -7529,10 +7598,10 @@
         <v xml:space="preserve">  - col:  nmemi</v>
       </c>
       <c r="G77" s="33" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="L77" s="33" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="78" spans="1:12" ht="13" customHeight="1">
@@ -7554,7 +7623,7 @@
         <v>706</v>
       </c>
       <c r="L78" s="33" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="79" spans="1:12" ht="13" customHeight="1">
@@ -7573,10 +7642,10 @@
         <v xml:space="preserve">    to:   [1, 2]</v>
       </c>
       <c r="G79" s="33" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="L79" s="33" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="80" spans="1:12" ht="13" customHeight="1">
@@ -7622,16 +7691,16 @@
     </row>
     <row r="85" spans="1:10" ht="13" customHeight="1">
       <c r="G85" s="33" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="H85" s="33" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="I85" s="33" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="J85" s="33" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="86" spans="1:10" ht="13" customHeight="1">
@@ -7714,7 +7783,7 @@
         <v>377</v>
       </c>
       <c r="F1" s="41" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="G1" s="40" t="s">
         <v>224</v>
@@ -7726,20 +7795,20 @@
     <row r="2" spans="1:8" s="40" customFormat="1" ht="13" customHeight="1">
       <c r="A2" s="39"/>
       <c r="B2" s="40" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="C2" s="40" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="D2" s="41" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="E2" s="41" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="F2" s="41"/>
       <c r="G2" s="40" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="13" customHeight="1">
@@ -7750,7 +7819,7 @@
         <v>797</v>
       </c>
       <c r="H3" s="43" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="13" customHeight="1">
@@ -7808,7 +7877,7 @@
         <v>820</v>
       </c>
       <c r="F7" s="43" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="G7" s="43" t="s">
         <v>821</v>
@@ -7822,25 +7891,25 @@
         <v>169</v>
       </c>
       <c r="B8" s="44" t="s">
+        <v>942</v>
+      </c>
+      <c r="C8" s="43" t="s">
+        <v>975</v>
+      </c>
+      <c r="D8" s="44" t="s">
+        <v>976</v>
+      </c>
+      <c r="E8" s="44" t="s">
+        <v>928</v>
+      </c>
+      <c r="F8" s="44" t="s">
+        <v>1051</v>
+      </c>
+      <c r="G8" s="44" t="s">
         <v>943</v>
       </c>
-      <c r="C8" s="43" t="s">
-        <v>976</v>
-      </c>
-      <c r="D8" s="44" t="s">
-        <v>977</v>
-      </c>
-      <c r="E8" s="44" t="s">
-        <v>929</v>
-      </c>
-      <c r="F8" s="44" t="s">
-        <v>1052</v>
-      </c>
-      <c r="G8" s="44" t="s">
-        <v>944</v>
-      </c>
       <c r="H8" s="44" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="13" customHeight="1">
@@ -7903,10 +7972,10 @@
         <v>475</v>
       </c>
       <c r="C12" s="43" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="D12" s="43" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="E12" s="33" t="s">
         <v>373</v>
@@ -7918,13 +7987,13 @@
         <v>468</v>
       </c>
       <c r="H12" s="43" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="13" customHeight="1">
       <c r="A13" s="42"/>
       <c r="C13" s="43" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="E13" s="33" t="s">
         <v>374</v>
@@ -7933,7 +8002,7 @@
     <row r="14" spans="1:8" ht="13" customHeight="1">
       <c r="A14" s="42"/>
       <c r="C14" s="43" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="E14" s="33" t="s">
         <v>375</v>
@@ -7979,61 +8048,61 @@
     <row r="19" spans="1:7" ht="13" customHeight="1">
       <c r="A19" s="42"/>
       <c r="B19" s="43" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="C19" s="44" t="s">
+        <v>1044</v>
+      </c>
+      <c r="D19" s="43" t="s">
+        <v>1013</v>
+      </c>
+      <c r="E19" s="44" t="s">
+        <v>924</v>
+      </c>
+      <c r="F19" s="43" t="s">
         <v>1045</v>
       </c>
-      <c r="D19" s="43" t="s">
-        <v>1014</v>
-      </c>
-      <c r="E19" s="44" t="s">
-        <v>925</v>
-      </c>
-      <c r="F19" s="43" t="s">
-        <v>1046</v>
-      </c>
       <c r="G19" s="43" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="13" customHeight="1">
       <c r="A20" s="42"/>
       <c r="B20" s="43" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="C20" s="44" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="D20" s="44" t="s">
+        <v>910</v>
+      </c>
+      <c r="E20" s="44" t="s">
+        <v>910</v>
+      </c>
+      <c r="F20" s="43" t="s">
+        <v>1043</v>
+      </c>
+      <c r="G20" s="43" t="s">
         <v>911</v>
-      </c>
-      <c r="E20" s="44" t="s">
-        <v>911</v>
-      </c>
-      <c r="F20" s="43" t="s">
-        <v>1044</v>
-      </c>
-      <c r="G20" s="43" t="s">
-        <v>912</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="13" customHeight="1">
       <c r="A21" s="42"/>
       <c r="B21" s="43" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C21" s="44" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="D21" s="44" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="E21" s="44" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="F21" s="43" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="G21" s="43" t="s">
         <v>395</v>
@@ -8042,79 +8111,79 @@
     <row r="22" spans="1:7" ht="13" customHeight="1">
       <c r="A22" s="42"/>
       <c r="B22" s="43" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="C22" s="44" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="D22" s="44" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="E22" s="44" t="s">
+        <v>939</v>
+      </c>
+      <c r="F22" s="44" t="s">
+        <v>1069</v>
+      </c>
+      <c r="G22" s="43" t="s">
         <v>940</v>
-      </c>
-      <c r="F22" s="44" t="s">
-        <v>1070</v>
-      </c>
-      <c r="G22" s="43" t="s">
-        <v>941</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="13" customHeight="1">
       <c r="A23" s="42"/>
       <c r="C23" s="43" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="E23" s="44" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="F23" s="44" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="13" customHeight="1">
       <c r="A24" s="42"/>
       <c r="C24" s="43" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="E24" s="44" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F24" s="43" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="13" customHeight="1">
       <c r="A25" s="42"/>
       <c r="C25" s="43" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="F25" s="43" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="13" customHeight="1">
       <c r="A26" s="42"/>
       <c r="C26" s="43" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="E26" s="44"/>
       <c r="F26" s="43" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="13" customHeight="1">
       <c r="A27" s="42"/>
       <c r="E27" s="44"/>
       <c r="F27" s="44" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="13" customHeight="1">
       <c r="A28" s="42"/>
       <c r="E28" s="44"/>
       <c r="F28" s="44" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="13" customHeight="1">
@@ -8135,7 +8204,7 @@
     <row r="31" spans="1:7" ht="13" customHeight="1">
       <c r="A31" s="42"/>
       <c r="B31" s="37" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="C31" s="44" t="s">
         <v>538</v>
@@ -8147,7 +8216,7 @@
     <row r="32" spans="1:7" ht="13" customHeight="1">
       <c r="A32" s="42"/>
       <c r="C32" s="44" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="E32" s="33" t="s">
         <v>378</v>
@@ -8156,7 +8225,7 @@
     <row r="33" spans="1:6" ht="13" customHeight="1">
       <c r="A33" s="42"/>
       <c r="C33" s="44" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="E33" s="33" t="s">
         <v>380</v>
@@ -8165,7 +8234,7 @@
     <row r="34" spans="1:6" ht="13" customHeight="1">
       <c r="A34" s="42"/>
       <c r="C34" s="44" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="13" customHeight="1">
@@ -8186,69 +8255,69 @@
     <row r="37" spans="1:6" ht="13" customHeight="1">
       <c r="A37" s="42"/>
       <c r="C37" s="33" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="D37" s="43" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="13" customHeight="1">
       <c r="A38" s="42"/>
       <c r="C38" s="43" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="D38" s="43" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="F38" s="44"/>
     </row>
     <row r="39" spans="1:6" ht="13" customHeight="1">
       <c r="A39" s="42"/>
       <c r="C39" s="43" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="D39" s="43" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="F39" s="44"/>
     </row>
     <row r="40" spans="1:6" ht="13" customHeight="1">
       <c r="A40" s="42"/>
       <c r="C40" s="33" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="D40" s="43" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="13" customHeight="1">
       <c r="A41" s="42"/>
       <c r="C41" s="33" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="D41" s="43" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="13" customHeight="1">
       <c r="A42" s="42"/>
       <c r="C42" s="43" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="D42" s="43" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="13" customHeight="1">
       <c r="A43" s="42"/>
       <c r="C43" s="43" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="13" customHeight="1">
       <c r="A44" s="42"/>
       <c r="C44" s="43" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="13" customHeight="1">
@@ -8293,13 +8362,13 @@
     <row r="51" spans="1:7" ht="13" customHeight="1">
       <c r="A51" s="42"/>
       <c r="C51" s="44" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="E51" s="43" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="F51" s="43" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="G51" s="43" t="s">
         <v>316</v>
@@ -8311,40 +8380,40 @@
         <v>197</v>
       </c>
       <c r="E52" s="43" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="F52" s="43" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="G52" s="43" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="13" customHeight="1">
       <c r="A53" s="42"/>
       <c r="C53" s="44" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="E53" s="43" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="F53" s="43" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="G53" s="43" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="13" customHeight="1">
       <c r="A54" s="42"/>
       <c r="C54" s="44" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="E54" s="43" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="F54" s="43" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="G54" s="43" t="s">
         <v>387</v>
@@ -8353,31 +8422,31 @@
     <row r="55" spans="1:7" ht="13" customHeight="1">
       <c r="A55" s="42"/>
       <c r="C55" s="44" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="E55" s="43" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="F55" s="43" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="G55" s="43" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="13" customHeight="1">
       <c r="A56" s="42"/>
       <c r="C56" s="44" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="E56" s="43" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="F56" s="43" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="G56" s="43" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="13" customHeight="1">
@@ -8386,10 +8455,10 @@
         <v>364</v>
       </c>
       <c r="E57" s="44" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="F57" s="43" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="13" customHeight="1">
@@ -8398,58 +8467,58 @@
         <v>197</v>
       </c>
       <c r="E58" s="44" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="F58" s="43" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="13" customHeight="1">
       <c r="A59" s="42"/>
       <c r="C59" s="44" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="E59" s="44" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="F59" s="43" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="13" customHeight="1">
       <c r="A60" s="42"/>
       <c r="C60" s="44" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="E60" s="44" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="F60" s="43" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="13" customHeight="1">
       <c r="A61" s="42"/>
       <c r="C61" s="44" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="E61" s="44" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="F61" s="43" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="13" customHeight="1">
       <c r="A62" s="42"/>
       <c r="C62" s="44" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="E62" s="44" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="F62" s="43" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="13" customHeight="1">
@@ -8458,7 +8527,7 @@
         <v>365</v>
       </c>
       <c r="F63" s="43" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="13" customHeight="1">
@@ -8467,91 +8536,91 @@
         <v>197</v>
       </c>
       <c r="F64" s="43" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="13" customHeight="1">
       <c r="A65" s="42"/>
       <c r="C65" s="44" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="F65" s="43" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="13" customHeight="1">
       <c r="A66" s="42"/>
       <c r="C66" s="44" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="F66" s="43" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="13" customHeight="1">
       <c r="A67" s="42"/>
       <c r="C67" s="44" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="F67" s="43" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="13" customHeight="1">
       <c r="A68" s="42"/>
       <c r="C68" s="44" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="F68" s="43" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="13" customHeight="1">
       <c r="A69" s="42"/>
       <c r="C69" s="44" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="E69" s="45"/>
     </row>
     <row r="70" spans="1:6" ht="13" customHeight="1">
       <c r="A70" s="42"/>
       <c r="C70" s="44" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="E70" s="45"/>
     </row>
     <row r="71" spans="1:6" ht="13" customHeight="1">
       <c r="A71" s="42"/>
       <c r="C71" s="44" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="E71" s="45"/>
     </row>
     <row r="72" spans="1:6" ht="13" customHeight="1">
       <c r="A72" s="42"/>
       <c r="C72" s="44" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="E72" s="45"/>
     </row>
     <row r="73" spans="1:6" ht="13" customHeight="1">
       <c r="A73" s="42"/>
       <c r="C73" s="44" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="E73" s="45"/>
     </row>
     <row r="74" spans="1:6" ht="13" customHeight="1">
       <c r="A74" s="42"/>
       <c r="C74" s="44" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="E74" s="45"/>
     </row>
     <row r="75" spans="1:6" ht="13" customHeight="1">
       <c r="A75" s="42"/>
       <c r="B75" s="43" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="C75" s="45" t="str">
         <f t="shared" ref="C75:C80" si="0">IF(ISBLANK($B75), "", $B75)</f>
@@ -8569,7 +8638,7 @@
     <row r="76" spans="1:6" ht="13" customHeight="1">
       <c r="A76" s="42"/>
       <c r="B76" s="43" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="C76" s="45" t="str">
         <f t="shared" si="0"/>
@@ -8587,7 +8656,7 @@
     <row r="77" spans="1:6" ht="13" customHeight="1">
       <c r="A77" s="42"/>
       <c r="B77" s="43" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="C77" s="45" t="str">
         <f t="shared" si="0"/>
@@ -8605,7 +8674,7 @@
     <row r="78" spans="1:6" ht="13" customHeight="1">
       <c r="A78" s="42"/>
       <c r="B78" s="43" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="C78" s="45" t="str">
         <f t="shared" si="0"/>
@@ -8623,7 +8692,7 @@
     <row r="79" spans="1:6" ht="13" customHeight="1">
       <c r="A79" s="42"/>
       <c r="B79" s="43" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="C79" s="45" t="str">
         <f t="shared" si="0"/>
@@ -8641,7 +8710,7 @@
     <row r="80" spans="1:6" ht="13" customHeight="1">
       <c r="A80" s="42"/>
       <c r="B80" s="43" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="C80" s="45" t="str">
         <f t="shared" si="0"/>
@@ -8672,7 +8741,7 @@
       <c r="A83" s="42"/>
       <c r="B83" s="44"/>
       <c r="C83" s="44" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="13" customHeight="1">
@@ -8686,7 +8755,7 @@
       <c r="A85" s="42"/>
       <c r="B85" s="44"/>
       <c r="C85" s="44" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="13" customHeight="1">
@@ -8752,13 +8821,13 @@
     <row r="1" spans="1:4" s="31" customFormat="1" ht="13">
       <c r="A1" s="30"/>
       <c r="B1" s="30" t="s">
+        <v>997</v>
+      </c>
+      <c r="C1" s="31" t="s">
         <v>998</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="D1" s="31" t="s">
         <v>999</v>
-      </c>
-      <c r="D1" s="31" t="s">
-        <v>1000</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="13">
@@ -8810,13 +8879,13 @@
         <v>169</v>
       </c>
       <c r="B7" s="11" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>1001</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="25" t="s">
         <v>1002</v>
-      </c>
-      <c r="D7" s="25" t="s">
-        <v>1003</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="28" customFormat="1" ht="13">
@@ -8857,21 +8926,21 @@
         <v>470</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="13">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="D12" s="25" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="13">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="D13" s="25" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="28" customFormat="1" ht="13">
@@ -8912,13 +8981,13 @@
     <row r="19" spans="1:5" ht="13">
       <c r="A19" s="2"/>
       <c r="B19" s="24" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>335</v>
@@ -8927,13 +8996,13 @@
     <row r="20" spans="1:5" ht="13">
       <c r="A20" s="2"/>
       <c r="B20" s="24" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="D20" s="24" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>336</v>
@@ -8942,28 +9011,28 @@
     <row r="21" spans="1:5" ht="13">
       <c r="A21" s="2"/>
       <c r="B21" s="24" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="D21" s="24" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="13">
       <c r="A22" s="2"/>
       <c r="B22" s="24" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="D22" s="24" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>334</v>
@@ -8973,7 +9042,7 @@
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="13">
@@ -9021,27 +9090,27 @@
         <v>217</v>
       </c>
       <c r="D30" s="24" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="13">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="D31" s="24" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="13">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="12" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="D32" s="24" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="13">
@@ -9107,7 +9176,7 @@
         <v>472</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="13">
@@ -9116,7 +9185,7 @@
         <v>471</v>
       </c>
       <c r="D46" s="25" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="13">
@@ -9125,42 +9194,42 @@
         <v>473</v>
       </c>
       <c r="D47" s="25" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="13">
       <c r="A48" s="2"/>
       <c r="B48" s="12"/>
       <c r="D48" s="2" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="13">
       <c r="A49" s="2"/>
       <c r="B49" s="12"/>
       <c r="D49" s="2" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="13">
       <c r="A50" s="2"/>
       <c r="B50" s="12"/>
       <c r="D50" s="25" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="13">
       <c r="A51" s="2"/>
       <c r="B51" s="12"/>
       <c r="D51" s="25" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="13">
       <c r="A52" s="2"/>
       <c r="B52" s="12"/>
       <c r="D52" s="25" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="53" spans="1:5" s="28" customFormat="1" ht="13">
@@ -9230,28 +9299,28 @@
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="E65" s="24" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="13">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="E66" s="24" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="13">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="E67" s="24" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="13">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="E68" s="24" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="13">
@@ -9272,70 +9341,70 @@
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="E71" s="24" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="13">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="E72" s="24" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="13">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="E73" s="24" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="13">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="E74" s="24" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="13">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="D75" s="25" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="13">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="D76" s="25" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="13">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="D77" s="25" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="13">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="D78" s="25" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="13">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="D79" s="25" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="13">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="D80" s="25" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="81" spans="1:4" s="28" customFormat="1" ht="13">
@@ -9358,20 +9427,20 @@
     <row r="83" spans="1:4" ht="13">
       <c r="A83" s="2"/>
       <c r="B83" s="2" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="D83" s="26"/>
     </row>
     <row r="84" spans="1:4" ht="13">
       <c r="A84" s="2"/>
       <c r="B84" s="2" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="13">
@@ -9514,12 +9583,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9947295B-8D1F-FB48-972A-B6AD7BBC4112}">
   <dimension ref="A1:Y153"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B10" sqref="B10"/>
       <selection pane="topRight" activeCell="B10" sqref="B10"/>
       <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
-      <selection pane="bottomRight" activeCell="F35" sqref="F35"/>
+      <selection pane="bottomRight" activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="46.83203125" defaultRowHeight="13" customHeight="1"/>
@@ -9553,7 +9622,7 @@
         <v>6</v>
       </c>
       <c r="I1" s="34" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="J1" s="34" t="s">
         <v>7</v>
@@ -9606,31 +9675,31 @@
     </row>
     <row r="2" spans="1:25" ht="13" customHeight="1">
       <c r="A2" s="36" t="s">
+        <v>1111</v>
+      </c>
+      <c r="F2" s="36" t="s">
         <v>1112</v>
       </c>
-      <c r="F2" s="36" t="s">
+      <c r="G2" s="36" t="s">
         <v>1113</v>
       </c>
-      <c r="G2" s="36" t="s">
+      <c r="H2" s="36" t="s">
         <v>1114</v>
       </c>
-      <c r="H2" s="36" t="s">
+      <c r="I2" s="36" t="s">
         <v>1115</v>
       </c>
-      <c r="I2" s="36" t="s">
+      <c r="K2" s="36" t="s">
         <v>1116</v>
-      </c>
-      <c r="K2" s="36" t="s">
-        <v>1117</v>
       </c>
       <c r="Q2" s="32"/>
       <c r="R2" s="32"/>
       <c r="S2" s="32"/>
       <c r="T2" s="36" t="s">
+        <v>1117</v>
+      </c>
+      <c r="U2" s="36" t="s">
         <v>1118</v>
-      </c>
-      <c r="U2" s="36" t="s">
-        <v>1119</v>
       </c>
     </row>
     <row r="3" spans="1:25" ht="13" customHeight="1">
@@ -9653,13 +9722,13 @@
         <v>811</v>
       </c>
       <c r="G3" s="36" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="H3" s="36" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="I3" s="36" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="J3" s="36" t="s">
         <v>800</v>
@@ -9740,10 +9809,10 @@
         <v>812</v>
       </c>
       <c r="G4" s="36" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="H4" s="36" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="J4" s="36" t="s">
         <v>799</v>
@@ -9803,37 +9872,37 @@
     </row>
     <row r="5" spans="1:25" ht="13" customHeight="1">
       <c r="A5" s="36" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="B5" s="36" t="s">
+        <v>1120</v>
+      </c>
+      <c r="C5" s="36" t="s">
         <v>1121</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="D5" s="36" t="s">
         <v>1122</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="E5" s="36" t="s">
         <v>1123</v>
       </c>
-      <c r="E5" s="36" t="s">
+      <c r="K5" s="36" t="s">
         <v>1124</v>
-      </c>
-      <c r="K5" s="36" t="s">
-        <v>1125</v>
       </c>
       <c r="Q5" s="32"/>
       <c r="R5" s="32"/>
       <c r="S5" s="32"/>
       <c r="T5" s="32"/>
       <c r="U5" s="36" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="6" spans="1:25" ht="13" customHeight="1">
       <c r="A6" s="36" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="C6" s="36" t="str">
         <f>IF(ISBLANK($B6), "", $B6)</f>
@@ -9848,13 +9917,13 @@
         <v>Updated: 2019-10-29</v>
       </c>
       <c r="F6" s="36" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="G6" s="36" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="H6" s="36" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="Q6" s="32"/>
       <c r="R6" s="32"/>
@@ -9940,7 +10009,7 @@
     </row>
     <row r="8" spans="1:25" ht="13" customHeight="1">
       <c r="A8" s="36" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="B8" s="33"/>
       <c r="C8" s="33"/>
@@ -9956,19 +10025,19 @@
       <c r="M8" s="33"/>
       <c r="N8" s="33"/>
       <c r="O8" s="33" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="P8" s="33" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="Q8" s="33" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="R8" s="33" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="S8" s="33" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="T8" s="33"/>
       <c r="U8" s="33"/>
@@ -10014,17 +10083,17 @@
         <v>820</v>
       </c>
       <c r="L10" s="36" t="s">
-        <v>838</v>
+        <v>1182</v>
       </c>
       <c r="M10" s="36" t="str">
         <f>IF(ISBLANK($L10), "", $L10)</f>
-        <v>PathIn:  [data, output]</v>
+        <v>PathIn:  [data, input]</v>
       </c>
       <c r="N10" s="33" t="s">
+        <v>838</v>
+      </c>
+      <c r="O10" s="33" t="s">
         <v>839</v>
-      </c>
-      <c r="O10" s="33" t="s">
-        <v>840</v>
       </c>
       <c r="P10" s="32" t="str">
         <f>IF(ISBLANK($O10), "", $O10)</f>
@@ -10043,22 +10112,22 @@
         <v>PathIn:  [data, datasources, SGF]</v>
       </c>
       <c r="T10" s="36" t="s">
-        <v>838</v>
+        <v>1182</v>
       </c>
       <c r="U10" s="36" t="s">
+        <v>840</v>
+      </c>
+      <c r="V10" s="33" t="s">
         <v>841</v>
       </c>
-      <c r="V10" s="33" t="s">
+      <c r="W10" s="33" t="s">
         <v>842</v>
       </c>
-      <c r="W10" s="33" t="s">
+      <c r="X10" s="33" t="s">
         <v>843</v>
       </c>
-      <c r="X10" s="33" t="s">
-        <v>844</v>
-      </c>
       <c r="Y10" s="33" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="11" spans="1:25" ht="13" customHeight="1">
@@ -10066,76 +10135,76 @@
         <v>169</v>
       </c>
       <c r="B11" s="36" t="s">
-        <v>767</v>
+        <v>1183</v>
       </c>
       <c r="C11" s="36" t="s">
-        <v>768</v>
+        <v>1184</v>
       </c>
       <c r="D11" s="36" t="s">
-        <v>769</v>
+        <v>1185</v>
       </c>
       <c r="E11" s="36" t="s">
-        <v>770</v>
+        <v>1186</v>
       </c>
       <c r="F11" s="36" t="s">
-        <v>771</v>
+        <v>1187</v>
       </c>
       <c r="G11" s="36" t="s">
-        <v>772</v>
+        <v>1188</v>
       </c>
       <c r="H11" s="36" t="s">
-        <v>773</v>
+        <v>1189</v>
       </c>
       <c r="I11" s="36" t="s">
-        <v>773</v>
+        <v>1189</v>
       </c>
       <c r="J11" s="36" t="s">
-        <v>774</v>
+        <v>1190</v>
       </c>
       <c r="K11" s="36" t="s">
-        <v>775</v>
+        <v>1191</v>
       </c>
       <c r="L11" s="36" t="s">
-        <v>776</v>
+        <v>1192</v>
       </c>
       <c r="M11" s="36" t="s">
-        <v>777</v>
+        <v>1193</v>
       </c>
       <c r="N11" s="36" t="s">
-        <v>778</v>
+        <v>1194</v>
       </c>
       <c r="O11" s="36" t="s">
-        <v>779</v>
+        <v>1195</v>
       </c>
       <c r="P11" s="32" t="s">
-        <v>780</v>
+        <v>1196</v>
       </c>
       <c r="Q11" s="36" t="s">
-        <v>781</v>
+        <v>1197</v>
       </c>
       <c r="R11" s="36" t="s">
-        <v>782</v>
+        <v>1198</v>
       </c>
       <c r="S11" s="36" t="s">
-        <v>783</v>
+        <v>1199</v>
       </c>
       <c r="T11" s="36" t="s">
-        <v>784</v>
+        <v>1200</v>
       </c>
       <c r="U11" s="36" t="s">
-        <v>785</v>
+        <v>1201</v>
       </c>
       <c r="V11" s="36" t="s">
-        <v>786</v>
+        <v>1202</v>
       </c>
       <c r="W11" s="36" t="s">
-        <v>787</v>
+        <v>1203</v>
       </c>
       <c r="X11" s="36" t="s">
-        <v>788</v>
+        <v>1204</v>
       </c>
       <c r="Y11" s="36" t="s">
-        <v>789</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="13" spans="1:25" ht="13" customHeight="1">
@@ -10236,7 +10305,7 @@
         <v>486</v>
       </c>
       <c r="H14" s="36" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="I14" s="36" t="s">
         <v>330</v>
@@ -10849,7 +10918,7 @@
         <v xml:space="preserve">  - {col: r,      type: String}</v>
       </c>
       <c r="H33" s="36" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="I33" s="36" t="s">
         <v>711</v>
@@ -11164,14 +11233,14 @@
         <v xml:space="preserve">  - {col: units,      type: String}</v>
       </c>
       <c r="F37" s="36" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="G37" s="36" t="str">
         <f>IF(ISBLANK($F37), "", $F37)</f>
         <v xml:space="preserve">  - {col: n,      type: String}</v>
       </c>
       <c r="H37" s="36" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="I37" s="36" t="s">
         <v>708</v>
@@ -11241,7 +11310,7 @@
         <v># - {col: desc,   type: String}</v>
       </c>
       <c r="H38" s="36" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="I38" s="36" t="s">
         <v>110</v>
@@ -11308,7 +11377,7 @@
         <v xml:space="preserve">  - {col: units,  type: String}</v>
       </c>
       <c r="H39" s="36" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="I39" s="36" t="s">
         <v>111</v>
@@ -12513,7 +12582,7 @@
         <v xml:space="preserve">  - {from: IndustryId,             to: si}</v>
       </c>
       <c r="H65" s="36" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="I65" s="36" t="s">
         <v>712</v>
@@ -12653,7 +12722,7 @@
       <c r="F78" s="33"/>
       <c r="G78" s="33"/>
       <c r="H78" s="36" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="I78" s="36" t="s">
         <v>698</v>
@@ -12711,7 +12780,7 @@
         <v>605</v>
       </c>
       <c r="H81" s="36" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="I81" s="36" t="s">
         <v>701</v>
@@ -12737,7 +12806,7 @@
         <v>607</v>
       </c>
       <c r="H83" s="36" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="I83" s="36" t="s">
         <v>703</v>
@@ -12747,13 +12816,13 @@
     </row>
     <row r="84" spans="1:24" customFormat="1" ht="13" customHeight="1">
       <c r="H84" s="33" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="85" spans="1:24" ht="13" customHeight="1">
       <c r="F85" s="33"/>
       <c r="H85" s="33" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="J85" s="33"/>
       <c r="N85" s="33"/>
@@ -12832,14 +12901,14 @@
         <v xml:space="preserve">  on:  [input_bea, input_desc]</v>
       </c>
       <c r="F89" s="36" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="G89" s="36" t="str">
         <f>IF(ISBLANK($F89), "", $F89)</f>
         <v xml:space="preserve">  on:  [r, gdpcat, si, units, n, desc]</v>
       </c>
       <c r="H89" s="36" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="I89" s="36" t="s">
         <v>704</v>
@@ -13298,14 +13367,14 @@
     </row>
     <row r="102" spans="1:25" ht="13" customHeight="1">
       <c r="B102" s="36" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="C102" s="36" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve">    to:     [bea_code, windc_code]</v>
       </c>
       <c r="D102" s="36" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="E102" s="36" t="str">
         <f t="shared" si="8"/>
@@ -13487,42 +13556,42 @@
     </row>
     <row r="105" spans="1:25" ht="13" customHeight="1">
       <c r="B105" s="36" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="C105" s="36" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve">    kind:   left</v>
       </c>
       <c r="D105" s="36" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="E105" s="36" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">    kind:   left</v>
       </c>
       <c r="F105" s="36" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="G105" s="36" t="str">
         <f t="shared" si="9"/>
         <v xml:space="preserve">    kind:   left</v>
       </c>
       <c r="H105" s="36" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="I105" s="36" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="J105" s="36" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="K105" s="36" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="L105" s="33"/>
       <c r="N105" s="37"/>
       <c r="O105" s="36" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="P105" s="32" t="str">
         <f t="shared" si="10"/>
@@ -13541,10 +13610,10 @@
         <v xml:space="preserve">    kind:   left</v>
       </c>
       <c r="X105" s="36" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="Y105" s="36" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="106" spans="1:25" ht="13" customHeight="1">
@@ -13631,7 +13700,7 @@
         <v>530</v>
       </c>
       <c r="H107" s="36" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="J107" s="36" t="s">
         <v>16</v>
@@ -13670,14 +13739,14 @@
     </row>
     <row r="108" spans="1:25" ht="13" customHeight="1">
       <c r="B108" s="36" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="C108" s="36" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve">    to:     windc_code</v>
       </c>
       <c r="D108" s="36" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="E108" s="36" t="str">
         <f t="shared" si="8"/>
@@ -13690,7 +13759,7 @@
         <v>531</v>
       </c>
       <c r="H108" s="36" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="J108" s="36" t="s">
         <v>17</v>
@@ -13749,7 +13818,7 @@
         <v>606</v>
       </c>
       <c r="H109" s="36" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="J109" s="36" t="s">
         <v>606</v>
@@ -13808,7 +13877,7 @@
         <v>618</v>
       </c>
       <c r="H110" s="36" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="J110" s="36" t="s">
         <v>607</v>
@@ -13847,40 +13916,40 @@
     </row>
     <row r="111" spans="1:25" ht="13" customHeight="1">
       <c r="B111" s="36" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="C111" s="36" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve">    kind:   left</v>
       </c>
       <c r="D111" s="36" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="E111" s="36" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">    kind:   left</v>
       </c>
       <c r="F111" s="36" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="G111" s="36" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="H111" s="36" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="J111" s="36" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="K111" s="36" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="L111" s="33"/>
       <c r="N111" s="36" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="P111" s="36" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="Q111" s="32" t="str">
         <f t="shared" si="11"/>
@@ -13895,18 +13964,18 @@
         <v xml:space="preserve">    kind:   left</v>
       </c>
       <c r="U111" s="36" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="W111" s="36" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="Y111" s="36" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="112" spans="1:25" ht="13" customHeight="1">
       <c r="H112" s="36" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="K112" s="36" t="s">
         <v>315</v>
@@ -13921,7 +13990,7 @@
     </row>
     <row r="113" spans="1:25" ht="13" customHeight="1">
       <c r="H113" s="36" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="K113" s="36" t="s">
         <v>16</v>
@@ -13933,7 +14002,7 @@
     </row>
     <row r="114" spans="1:25" ht="13" customHeight="1">
       <c r="H114" s="36" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="K114" s="36" t="s">
         <v>17</v>
@@ -13945,7 +14014,7 @@
     </row>
     <row r="115" spans="1:25" ht="13" customHeight="1">
       <c r="H115" s="36" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="K115" s="36" t="s">
         <v>54</v>
@@ -13957,7 +14026,7 @@
     </row>
     <row r="116" spans="1:25" ht="13" customHeight="1">
       <c r="H116" s="36" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="K116" s="36" t="s">
         <v>55</v>
@@ -13969,14 +14038,14 @@
     </row>
     <row r="117" spans="1:25" ht="13" customHeight="1">
       <c r="H117" s="36" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="K117" s="36" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="L117" s="33"/>
       <c r="U117" s="36" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="118" spans="1:25" ht="13" customHeight="1">
@@ -14334,7 +14403,7 @@
     </row>
     <row r="123" spans="1:25" ht="13" customHeight="1">
       <c r="B123" s="36" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="C123" s="36" t="str">
         <f t="shared" si="13"/>
@@ -14369,14 +14438,14 @@
         <v xml:space="preserve">    kind:   left</v>
       </c>
       <c r="K123" s="36" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="L123" s="33"/>
       <c r="N123" s="36" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="O123" s="36" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="P123" s="32" t="str">
         <f>IF(ISBLANK($O123), "", $O123)</f>
@@ -14395,7 +14464,7 @@
         <v xml:space="preserve">    kind:   left</v>
       </c>
       <c r="U123" s="36" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="Y123" s="36" t="str">
         <f t="shared" si="15"/>
@@ -14517,7 +14586,7 @@
     </row>
     <row r="127" spans="1:25" ht="13" customHeight="1">
       <c r="B127" s="36" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="C127" s="36" t="str">
         <f>IF(ISBLANK($B127), "", $B127)</f>
@@ -14761,7 +14830,7 @@
         <v>620</v>
       </c>
       <c r="H137" s="36" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="I137" s="36" t="s">
         <v>204</v>
@@ -14770,7 +14839,7 @@
         <v>631</v>
       </c>
       <c r="K137" s="36" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="N137" s="36" t="s">
         <v>791</v>
@@ -14904,7 +14973,7 @@
         <v>619</v>
       </c>
       <c r="H140" s="36" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="J140" s="36" t="s">
         <v>625</v>
@@ -14937,7 +15006,7 @@
         <v>22</v>
       </c>
       <c r="H141" s="36" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="J141" s="36" t="s">
         <v>626</v>
@@ -15639,12 +15708,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E388B376-25CD-114A-9979-B5C580A31165}">
   <dimension ref="A1:Y155"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B10" sqref="B10"/>
       <selection pane="topRight" activeCell="B10" sqref="B10"/>
       <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
-      <selection pane="bottomRight" activeCell="C18" sqref="C18"/>
+      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="46.83203125" defaultRowHeight="13" customHeight="1"/>
@@ -15657,7 +15726,7 @@
   <sheetData>
     <row r="1" spans="1:25" s="34" customFormat="1" ht="13" customHeight="1">
       <c r="B1" s="34" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="C1" s="34" t="s">
         <v>221</v>
@@ -15669,13 +15738,13 @@
         <v>224</v>
       </c>
       <c r="F1" s="34" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="P1" s="35"/>
     </row>
     <row r="2" spans="1:25" ht="13" customHeight="1">
       <c r="A2" s="36" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="Q2" s="32"/>
       <c r="R2" s="32"/>
@@ -15701,7 +15770,7 @@
     </row>
     <row r="5" spans="1:25" ht="13" customHeight="1">
       <c r="A5" s="36" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="Q5" s="32"/>
       <c r="R5" s="32"/>
@@ -15710,7 +15779,7 @@
     </row>
     <row r="6" spans="1:25" ht="13" customHeight="1">
       <c r="A6" s="36" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="Q6" s="32"/>
       <c r="R6" s="32"/>
@@ -15757,7 +15826,7 @@
     </row>
     <row r="8" spans="1:25" ht="13" customHeight="1">
       <c r="A8" s="36" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="B8" s="33"/>
       <c r="C8" s="33"/>
@@ -15789,23 +15858,23 @@
         <v>819</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>838</v>
+        <v>1182</v>
       </c>
       <c r="C10" s="36" t="str">
         <f>B10</f>
-        <v>PathIn:  [data, output]</v>
+        <v>PathIn:  [data, input]</v>
       </c>
       <c r="D10" s="36" t="str">
         <f>C10</f>
-        <v>PathIn:  [data, output]</v>
+        <v>PathIn:  [data, input]</v>
       </c>
       <c r="E10" s="36" t="str">
         <f>D10</f>
-        <v>PathIn:  [data, output]</v>
+        <v>PathIn:  [data, input]</v>
       </c>
       <c r="F10" s="36" t="str">
         <f>E10</f>
-        <v>PathIn:  [data, output]</v>
+        <v>PathIn:  [data, input]</v>
       </c>
       <c r="G10" s="33"/>
       <c r="H10" s="33"/>
@@ -15826,19 +15895,19 @@
         <v>169</v>
       </c>
       <c r="B11" s="36" t="s">
+        <v>1166</v>
+      </c>
+      <c r="C11" s="36" t="s">
+        <v>1168</v>
+      </c>
+      <c r="D11" s="36" t="s">
         <v>1167</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="E11" s="36" t="s">
+        <v>1181</v>
+      </c>
+      <c r="F11" s="36" t="s">
         <v>1169</v>
-      </c>
-      <c r="D11" s="36" t="s">
-        <v>1168</v>
-      </c>
-      <c r="E11" s="36" t="s">
-        <v>1182</v>
-      </c>
-      <c r="F11" s="36" t="s">
-        <v>1170</v>
       </c>
     </row>
     <row r="13" spans="1:25" ht="13" customHeight="1">
@@ -15865,19 +15934,19 @@
     </row>
     <row r="14" spans="1:25" ht="13" customHeight="1">
       <c r="B14" s="36" t="s">
+        <v>1141</v>
+      </c>
+      <c r="C14" s="36" t="s">
         <v>1142</v>
       </c>
-      <c r="C14" s="36" t="s">
+      <c r="D14" s="36" t="s">
         <v>1143</v>
       </c>
-      <c r="D14" s="36" t="s">
+      <c r="E14" s="36" t="s">
         <v>1144</v>
       </c>
-      <c r="E14" s="36" t="s">
+      <c r="F14" s="36" t="s">
         <v>1145</v>
-      </c>
-      <c r="F14" s="36" t="s">
-        <v>1146</v>
       </c>
       <c r="N14" s="37"/>
     </row>
@@ -15955,19 +16024,19 @@
     </row>
     <row r="20" spans="1:24" ht="13" customHeight="1">
       <c r="B20" s="36" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="C20" s="36" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="D20" s="36" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="E20" s="36" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="F20" s="36" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="21" spans="1:24" ht="13" customHeight="1">
@@ -15981,10 +16050,10 @@
         <v>147</v>
       </c>
       <c r="E21" s="36" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="F21" s="36" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="22" spans="1:24" ht="13" customHeight="1">
@@ -16011,7 +16080,7 @@
     </row>
     <row r="24" spans="1:24" ht="13" customHeight="1">
       <c r="F24" s="36" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="26" spans="1:24" ht="13" customHeight="1">
@@ -16118,7 +16187,7 @@
     <row r="35" spans="1:25" ht="13" customHeight="1">
       <c r="B35" s="33"/>
       <c r="F35" s="36" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="K35" s="33"/>
       <c r="L35" s="33"/>
@@ -16137,7 +16206,7 @@
     <row r="36" spans="1:25" ht="13" customHeight="1">
       <c r="B36" s="33"/>
       <c r="F36" s="36" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="K36" s="33"/>
       <c r="L36" s="33"/>
@@ -16199,19 +16268,19 @@
     <row r="39" spans="1:25" ht="13" customHeight="1">
       <c r="A39" s="38"/>
       <c r="B39" s="36" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="C39" s="36" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="D39" s="36" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="E39" s="36" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="F39" s="36" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="K39" s="33"/>
       <c r="L39" s="33"/>
@@ -16226,19 +16295,19 @@
     <row r="40" spans="1:25" ht="13" customHeight="1">
       <c r="A40" s="38"/>
       <c r="B40" s="36" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="C40" s="36" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="D40" s="36" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="E40" s="36" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="F40" s="36" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="K40" s="33"/>
       <c r="L40" s="33"/>
@@ -16253,19 +16322,19 @@
     <row r="41" spans="1:25" ht="13" customHeight="1">
       <c r="A41" s="38"/>
       <c r="B41" s="36" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="C41" s="36" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="D41" s="36" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="E41" s="36" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="F41" s="36" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="K41" s="33"/>
       <c r="L41" s="33"/>
@@ -16279,19 +16348,19 @@
     <row r="42" spans="1:25" ht="13" customHeight="1">
       <c r="A42" s="38"/>
       <c r="B42" s="36" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="C42" s="36" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="D42" s="36" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="E42" s="36" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="F42" s="36" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="K42" s="33"/>
       <c r="L42" s="33"/>
@@ -16307,19 +16376,19 @@
     <row r="43" spans="1:25" ht="13" customHeight="1">
       <c r="A43" s="38"/>
       <c r="B43" s="36" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="C43" s="36" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D43" s="36" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="E43" s="36" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="F43" s="36" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="L43" s="33"/>
       <c r="N43" s="33"/>
@@ -16334,7 +16403,7 @@
     <row r="44" spans="1:25" ht="13" customHeight="1">
       <c r="A44" s="38"/>
       <c r="B44" s="36" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="C44" s="36" t="str">
         <f>$B$44</f>
@@ -16422,7 +16491,7 @@
     <row r="49" spans="1:22" ht="13" customHeight="1">
       <c r="A49" s="38"/>
       <c r="B49" s="36" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="E49" s="36" t="str">
         <f>$B49</f>
@@ -16441,7 +16510,7 @@
     <row r="50" spans="1:22" ht="13" customHeight="1">
       <c r="A50" s="38"/>
       <c r="B50" s="36" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="E50" s="36" t="str">
         <f t="shared" ref="E50:E51" si="0">$B50</f>
@@ -16638,19 +16707,19 @@
     </row>
     <row r="58" spans="1:22" ht="13" customHeight="1">
       <c r="B58" s="36" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="C58" s="36" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="D58" s="36" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="E58" s="36" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="F58" s="36" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="K58" s="33"/>
       <c r="L58" s="33"/>
@@ -17198,27 +17267,27 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:N2 P2:XFD2 C17 A17 E3:XFD16 E25:XFD33 E24 A2:D10 A12:D16 A37:XFD1048576 A18:C19 D17:XFD19 F20:XFD24 A20:D33 B11:D11">
-    <cfRule type="expression" dxfId="4" priority="273">
+    <cfRule type="expression" dxfId="10" priority="273">
       <formula>AND(COUNTA($A2:$AA2)=0, NOT(ISBLANK($A3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:F15">
-    <cfRule type="expression" dxfId="3" priority="353">
+    <cfRule type="expression" dxfId="9" priority="353">
       <formula>AND(COUNTA($A17:$AA17)=0, NOT(ISBLANK($A18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36:XFD36">
-    <cfRule type="expression" dxfId="2" priority="361">
+    <cfRule type="expression" dxfId="8" priority="361">
       <formula>AND(COUNTA($A36:$AA36)=0, NOT(ISBLANK($A38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A34:XFD35">
-    <cfRule type="expression" dxfId="1" priority="368">
+    <cfRule type="expression" dxfId="7" priority="368">
       <formula>AND(COUNTA($A34:$AA34)=0, NOT(ISBLANK($A37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20:E22">
-    <cfRule type="expression" dxfId="0" priority="376">
+    <cfRule type="expression" dxfId="6" priority="376">
       <formula>AND(COUNTA($A21:$AA21)=0, NOT(ISBLANK($A22)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22634,32 +22703,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="expression" dxfId="10" priority="6">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>_xlfn.ISFORMULA(A1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G63:G67">
-    <cfRule type="expression" dxfId="9" priority="5">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>_xlfn.ISFORMULA(G63)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G30:G31">
-    <cfRule type="expression" dxfId="8" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>_xlfn.ISFORMULA(G30)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G26:G27">
-    <cfRule type="expression" dxfId="7" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>_xlfn.ISFORMULA(G26)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G33:G58">
-    <cfRule type="expression" dxfId="6" priority="3">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>_xlfn.ISFORMULA(G33)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M32">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>_xlfn.ISFORMULA(M32)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
disaggregation complete and verified against WiNDC benchmark
</commit_message>
<xml_diff>
--- a/data/readfiles/generate_yaml.xlsx
+++ b/data/readfiles/generate_yaml.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chughes/Documents/Git/SLiDE/data/readfiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F335D12-593A-C84C-9198-54AEA6F0E186}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{134DF1E9-EEE4-6547-9976-0A13C3586C7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18900" activeTab="5" xr2:uid="{ECEEE8D6-CC61-454D-945D-45D0FFF64D45}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="5" xr2:uid="{ECEEE8D6-CC61-454D-945D-45D0FFF64D45}"/>
   </bookViews>
   <sheets>
     <sheet name="map_bluenote" sheetId="5" state="hidden" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3110" uniqueCount="1206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3127" uniqueCount="1216">
   <si>
     <t>bea_supply</t>
   </si>
@@ -3658,6 +3658,36 @@
   </si>
   <si>
     <t>PathOut: [data, input, seds.csv]</t>
+  </si>
+  <si>
+    <t>PathOut: [data, coremaps, parse, fd.csv]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  name: fdcat.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  descriptor: final_demand</t>
+  </si>
+  <si>
+    <t>fd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - {col: code, type: String}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - {col: desc, type: String}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  name: statedisagg_fdmap.map</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  col:  [fd, fdcat, fd_desc]</t>
+  </si>
+  <si>
+    <t>PathIn:  [data, mapsources, WiNDC, windc_build, build_files]</t>
+  </si>
+  <si>
+    <t>PathOut: [data, coremaps, crosswalk, fd.csv]</t>
   </si>
 </sst>
 </file>
@@ -5352,14 +5382,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7AB9832-7F74-B245-B43D-5B870966A3CC}">
-  <dimension ref="A1:N91"/>
+  <dimension ref="A1:O91"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="I67" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="M11" sqref="M11"/>
       <selection pane="topRight" activeCell="M11" sqref="M11"/>
       <selection pane="bottomLeft" activeCell="M11" sqref="M11"/>
-      <selection pane="bottomRight" activeCell="I113" sqref="I113"/>
+      <selection pane="bottomRight" activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="40.83203125" defaultRowHeight="13" customHeight="1"/>
@@ -5368,7 +5398,7 @@
     <col min="2" max="16384" width="40.83203125" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="53" customFormat="1" ht="13" customHeight="1">
+    <row r="1" spans="1:15" s="53" customFormat="1" ht="13" customHeight="1">
       <c r="A1" s="52"/>
       <c r="B1" s="53" t="s">
         <v>362</v>
@@ -5380,53 +5410,56 @@
         <v>206</v>
       </c>
       <c r="E1" s="53" t="s">
+        <v>1209</v>
+      </c>
+      <c r="F1" s="53" t="s">
         <v>221</v>
       </c>
-      <c r="F1" s="53" t="s">
+      <c r="G1" s="53" t="s">
         <v>403</v>
       </c>
-      <c r="G1" s="53" t="s">
+      <c r="H1" s="53" t="s">
         <v>222</v>
       </c>
-      <c r="H1" s="53" t="s">
+      <c r="I1" s="53" t="s">
         <v>356</v>
       </c>
-      <c r="I1" s="53" t="s">
+      <c r="J1" s="53" t="s">
         <v>223</v>
       </c>
-      <c r="J1" s="53" t="s">
+      <c r="K1" s="53" t="s">
         <v>377</v>
       </c>
-      <c r="K1" s="53" t="s">
+      <c r="L1" s="53" t="s">
         <v>224</v>
       </c>
-      <c r="L1" s="53" t="s">
+      <c r="M1" s="53" t="s">
         <v>225</v>
       </c>
-      <c r="M1" s="53" t="s">
+      <c r="N1" s="53" t="s">
         <v>424</v>
       </c>
-      <c r="N1" s="53" t="s">
+      <c r="O1" s="53" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="13" customHeight="1">
+    <row r="2" spans="1:15" ht="13" customHeight="1">
       <c r="A2" s="49" t="s">
         <v>795</v>
       </c>
-      <c r="G2" s="33" t="s">
+      <c r="H2" s="33" t="s">
         <v>846</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="13" customHeight="1">
+    <row r="3" spans="1:15" ht="13" customHeight="1">
       <c r="A3" s="49" t="s">
         <v>796</v>
       </c>
-      <c r="G3" s="33" t="s">
+      <c r="H3" s="33" t="s">
         <v>845</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="13" customHeight="1">
+    <row r="4" spans="1:15" ht="13" customHeight="1">
       <c r="A4" s="49" t="s">
         <v>801</v>
       </c>
@@ -5469,13 +5502,16 @@
       <c r="N4" s="33" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" ht="13" customHeight="1">
+      <c r="O4" s="33" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="13" customHeight="1">
       <c r="A5" s="49" t="s">
         <v>969</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="13" customHeight="1">
+    <row r="7" spans="1:15" ht="13" customHeight="1">
       <c r="A7" s="49" t="s">
         <v>819</v>
       </c>
@@ -5489,37 +5525,40 @@
         <v>822</v>
       </c>
       <c r="E7" s="33" t="s">
+        <v>826</v>
+      </c>
+      <c r="F7" s="33" t="s">
         <v>823</v>
       </c>
-      <c r="F7" s="33" t="s">
+      <c r="G7" s="33" t="s">
         <v>822</v>
       </c>
-      <c r="G7" s="33" t="s">
+      <c r="H7" s="33" t="s">
         <v>824</v>
       </c>
-      <c r="H7" s="33" t="s">
+      <c r="I7" s="33" t="s">
         <v>825</v>
       </c>
-      <c r="I7" s="33" t="s">
+      <c r="J7" s="33" t="s">
         <v>823</v>
       </c>
-      <c r="J7" s="33" t="s">
+      <c r="K7" s="33" t="s">
         <v>820</v>
       </c>
-      <c r="K7" s="33" t="s">
+      <c r="L7" s="33" t="s">
         <v>822</v>
       </c>
-      <c r="L7" s="33" t="s">
+      <c r="M7" s="33" t="s">
         <v>825</v>
       </c>
-      <c r="M7" s="33" t="s">
+      <c r="N7" s="33" t="s">
         <v>826</v>
       </c>
-      <c r="N7" s="33" t="s">
+      <c r="O7" s="33" t="s">
         <v>823</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="13" customHeight="1">
+    <row r="8" spans="1:15" ht="13" customHeight="1">
       <c r="A8" s="49" t="s">
         <v>169</v>
       </c>
@@ -5533,37 +5572,40 @@
         <v>736</v>
       </c>
       <c r="E8" s="33" t="s">
+        <v>1206</v>
+      </c>
+      <c r="F8" s="33" t="s">
         <v>737</v>
       </c>
-      <c r="F8" s="33" t="s">
+      <c r="G8" s="33" t="s">
         <v>738</v>
       </c>
-      <c r="G8" s="33" t="s">
+      <c r="H8" s="33" t="s">
         <v>739</v>
       </c>
-      <c r="H8" s="33" t="s">
+      <c r="I8" s="33" t="s">
         <v>740</v>
       </c>
-      <c r="I8" s="33" t="s">
+      <c r="J8" s="33" t="s">
         <v>741</v>
       </c>
-      <c r="J8" s="33" t="s">
+      <c r="K8" s="33" t="s">
         <v>742</v>
       </c>
-      <c r="K8" s="33" t="s">
+      <c r="L8" s="33" t="s">
         <v>743</v>
       </c>
-      <c r="L8" s="33" t="s">
+      <c r="M8" s="33" t="s">
         <v>744</v>
       </c>
-      <c r="M8" s="33" t="s">
+      <c r="N8" s="33" t="s">
         <v>745</v>
       </c>
-      <c r="N8" s="33" t="s">
+      <c r="O8" s="33" t="s">
         <v>746</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="13" customHeight="1">
+    <row r="10" spans="1:15" ht="13" customHeight="1">
       <c r="A10" s="49" t="s">
         <v>170</v>
       </c>
@@ -5583,19 +5625,19 @@
         <v>8</v>
       </c>
       <c r="G10" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="33" t="s">
         <v>64</v>
-      </c>
-      <c r="H10" s="33" t="s">
-        <v>8</v>
       </c>
       <c r="I10" s="33" t="s">
         <v>8</v>
       </c>
       <c r="J10" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="K10" s="33" t="s">
         <v>64</v>
-      </c>
-      <c r="K10" s="33" t="s">
-        <v>8</v>
       </c>
       <c r="L10" s="33" t="s">
         <v>8</v>
@@ -5606,8 +5648,11 @@
       <c r="N10" s="33" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" ht="13" customHeight="1">
+      <c r="O10" s="33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="13" customHeight="1">
       <c r="B11" s="33" t="s">
         <v>368</v>
       </c>
@@ -5618,111 +5663,117 @@
         <v>338</v>
       </c>
       <c r="E11" s="33" t="s">
+        <v>1207</v>
+      </c>
+      <c r="F11" s="33" t="s">
         <v>353</v>
       </c>
-      <c r="F11" s="33" t="s">
+      <c r="G11" s="33" t="s">
         <v>402</v>
       </c>
-      <c r="G11" s="33" t="s">
+      <c r="H11" s="33" t="s">
         <v>209</v>
       </c>
-      <c r="H11" s="33" t="s">
+      <c r="I11" s="33" t="s">
         <v>357</v>
       </c>
-      <c r="I11" s="33" t="s">
+      <c r="J11" s="33" t="s">
         <v>359</v>
       </c>
-      <c r="J11" s="33" t="s">
+      <c r="K11" s="33" t="s">
         <v>372</v>
       </c>
-      <c r="K11" s="33" t="s">
+      <c r="L11" s="33" t="s">
         <v>207</v>
       </c>
-      <c r="L11" s="33" t="s">
+      <c r="M11" s="33" t="s">
         <v>214</v>
       </c>
-      <c r="M11" s="33" t="s">
+      <c r="N11" s="33" t="s">
         <v>422</v>
       </c>
-      <c r="N11" s="33" t="s">
+      <c r="O11" s="33" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="13" customHeight="1">
+    <row r="12" spans="1:15" ht="13" customHeight="1">
       <c r="D12" s="33" t="s">
         <v>215</v>
       </c>
       <c r="E12" s="33" t="s">
+        <v>1208</v>
+      </c>
+      <c r="F12" s="33" t="s">
         <v>354</v>
       </c>
-      <c r="F12" s="33" t="s">
+      <c r="G12" s="33" t="s">
         <v>119</v>
       </c>
-      <c r="G12" s="33" t="s">
+      <c r="H12" s="33" t="s">
         <v>210</v>
       </c>
-      <c r="H12" s="33" t="s">
+      <c r="I12" s="33" t="s">
         <v>358</v>
       </c>
-      <c r="I12" s="33" t="s">
+      <c r="J12" s="33" t="s">
         <v>360</v>
       </c>
-      <c r="J12" s="33" t="s">
+      <c r="K12" s="33" t="s">
         <v>373</v>
       </c>
-      <c r="K12" s="33" t="s">
+      <c r="L12" s="33" t="s">
         <v>208</v>
       </c>
-      <c r="L12" s="33" t="s">
+      <c r="M12" s="33" t="s">
         <v>216</v>
       </c>
-      <c r="M12" s="33" t="s">
+      <c r="N12" s="33" t="s">
         <v>423</v>
       </c>
-      <c r="N12" s="33" t="s">
+      <c r="O12" s="33" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="13" customHeight="1">
-      <c r="E13" s="33" t="s">
+    <row r="13" spans="1:15" ht="13" customHeight="1">
+      <c r="F13" s="33" t="s">
         <v>421</v>
       </c>
-      <c r="G13" s="33" t="s">
+      <c r="H13" s="33" t="s">
         <v>211</v>
       </c>
-      <c r="I13" s="33" t="s">
+      <c r="J13" s="33" t="s">
         <v>420</v>
       </c>
-      <c r="J13" s="33" t="s">
+      <c r="K13" s="33" t="s">
         <v>374</v>
       </c>
-      <c r="N13" s="33" t="s">
+      <c r="O13" s="33" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="13" customHeight="1">
-      <c r="E14" s="33" t="s">
+    <row r="14" spans="1:15" ht="13" customHeight="1">
+      <c r="F14" s="33" t="s">
         <v>355</v>
       </c>
-      <c r="G14" s="33" t="s">
+      <c r="H14" s="33" t="s">
         <v>212</v>
       </c>
-      <c r="I14" s="33" t="s">
+      <c r="J14" s="33" t="s">
         <v>361</v>
       </c>
-      <c r="J14" s="33" t="s">
+      <c r="K14" s="33" t="s">
         <v>375</v>
       </c>
-      <c r="N14" s="33" t="s">
+      <c r="O14" s="33" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="13" customHeight="1">
+    <row r="16" spans="1:15" ht="13" customHeight="1">
       <c r="A16" s="49" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="13" customHeight="1">
+    <row r="18" spans="1:15" ht="13" customHeight="1">
       <c r="A18" s="49" t="s">
         <v>172</v>
       </c>
@@ -5735,13 +5786,13 @@
       <c r="D18" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="F18" s="33" t="s">
+      <c r="E18" s="33" t="s">
         <v>9</v>
       </c>
       <c r="G18" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="I18" s="33" t="s">
+      <c r="H18" s="33" t="s">
         <v>9</v>
       </c>
       <c r="J18" s="33" t="s">
@@ -5750,11 +5801,14 @@
       <c r="K18" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="N18" s="33" t="s">
+      <c r="L18" s="33" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" ht="13" customHeight="1">
+      <c r="O18" s="33" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="13" customHeight="1">
       <c r="B19" s="33" t="s">
         <v>335</v>
       </c>
@@ -5764,26 +5818,29 @@
       <c r="D19" s="33" t="s">
         <v>335</v>
       </c>
-      <c r="F19" s="33" t="s">
+      <c r="E19" s="33" t="s">
+        <v>1210</v>
+      </c>
+      <c r="G19" s="33" t="s">
         <v>407</v>
       </c>
-      <c r="G19" s="33" t="s">
+      <c r="H19" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="I19" s="33" t="s">
+      <c r="J19" s="33" t="s">
         <v>496</v>
       </c>
-      <c r="J19" s="33" t="s">
+      <c r="K19" s="33" t="s">
         <v>924</v>
       </c>
-      <c r="K19" s="33" t="s">
+      <c r="L19" s="33" t="s">
         <v>394</v>
       </c>
-      <c r="N19" s="33" t="s">
+      <c r="O19" s="33" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="13" customHeight="1">
+    <row r="20" spans="1:15" ht="13" customHeight="1">
       <c r="B20" s="33" t="s">
         <v>336</v>
       </c>
@@ -5793,26 +5850,29 @@
       <c r="D20" s="33" t="s">
         <v>336</v>
       </c>
-      <c r="F20" s="33" t="s">
+      <c r="E20" s="33" t="s">
+        <v>1211</v>
+      </c>
+      <c r="G20" s="33" t="s">
         <v>406</v>
       </c>
-      <c r="G20" s="33" t="s">
+      <c r="H20" s="33" t="s">
         <v>342</v>
       </c>
-      <c r="I20" s="33" t="s">
+      <c r="J20" s="33" t="s">
         <v>497</v>
       </c>
-      <c r="J20" s="33" t="s">
+      <c r="K20" s="33" t="s">
         <v>376</v>
       </c>
-      <c r="K20" s="33" t="s">
+      <c r="L20" s="33" t="s">
         <v>395</v>
       </c>
-      <c r="N20" s="33" t="s">
+      <c r="O20" s="33" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="13" customHeight="1">
+    <row r="21" spans="1:15" ht="13" customHeight="1">
       <c r="B21" s="33" t="s">
         <v>911</v>
       </c>
@@ -5822,23 +5882,23 @@
       <c r="D21" s="33" t="s">
         <v>911</v>
       </c>
-      <c r="F21" s="33" t="s">
+      <c r="G21" s="33" t="s">
         <v>120</v>
       </c>
-      <c r="G21" s="33" t="s">
+      <c r="H21" s="33" t="s">
         <v>341</v>
       </c>
-      <c r="J21" s="33" t="s">
+      <c r="K21" s="33" t="s">
         <v>390</v>
       </c>
-      <c r="K21" s="33" t="s">
+      <c r="L21" s="33" t="s">
         <v>393</v>
       </c>
-      <c r="N21" s="33" t="s">
+      <c r="O21" s="33" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="13" customHeight="1">
+    <row r="22" spans="1:15" ht="13" customHeight="1">
       <c r="B22" s="33" t="s">
         <v>334</v>
       </c>
@@ -5848,32 +5908,32 @@
       <c r="D22" s="33" t="s">
         <v>334</v>
       </c>
-      <c r="F22" s="33" t="s">
+      <c r="G22" s="33" t="s">
         <v>405</v>
       </c>
-      <c r="K22" s="33" t="s">
+      <c r="L22" s="33" t="s">
         <v>389</v>
       </c>
-      <c r="N22" s="33" t="s">
+      <c r="O22" s="33" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="13" customHeight="1">
-      <c r="F23" s="33" t="s">
+    <row r="23" spans="1:15" ht="13" customHeight="1">
+      <c r="G23" s="33" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="13" customHeight="1">
-      <c r="F24" s="33" t="s">
+    <row r="24" spans="1:15" ht="13" customHeight="1">
+      <c r="G24" s="33" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="13" customHeight="1">
-      <c r="F25" s="33" t="s">
+    <row r="25" spans="1:15" ht="13" customHeight="1">
+      <c r="G25" s="33" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="13" customHeight="1">
+    <row r="28" spans="1:15" ht="13" customHeight="1">
       <c r="A28" s="49" t="s">
         <v>173</v>
       </c>
@@ -5886,20 +5946,20 @@
       <c r="D28" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="F28" s="33" t="s">
-        <v>10</v>
-      </c>
       <c r="G28" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="J28" s="33" t="s">
+      <c r="H28" s="33" t="s">
         <v>10</v>
       </c>
       <c r="K28" s="33" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" ht="13" customHeight="1">
+      <c r="L28" s="33" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="13" customHeight="1">
       <c r="B29" s="33" t="s">
         <v>337</v>
       </c>
@@ -5909,20 +5969,20 @@
       <c r="D29" s="33" t="s">
         <v>337</v>
       </c>
-      <c r="F29" s="33" t="s">
+      <c r="G29" s="33" t="s">
         <v>409</v>
       </c>
-      <c r="G29" s="33" t="s">
+      <c r="H29" s="33" t="s">
         <v>339</v>
       </c>
-      <c r="J29" s="33" t="s">
+      <c r="K29" s="33" t="s">
         <v>379</v>
       </c>
-      <c r="K29" s="33" t="s">
+      <c r="L29" s="33" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="13" customHeight="1">
+    <row r="30" spans="1:15" ht="13" customHeight="1">
       <c r="B30" s="33" t="s">
         <v>217</v>
       </c>
@@ -5932,17 +5992,17 @@
       <c r="D30" s="33" t="s">
         <v>217</v>
       </c>
-      <c r="F30" s="33" t="s">
+      <c r="G30" s="33" t="s">
         <v>408</v>
       </c>
-      <c r="G30" s="33" t="s">
+      <c r="H30" s="33" t="s">
         <v>340</v>
       </c>
-      <c r="J30" s="33" t="s">
+      <c r="K30" s="33" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="13" customHeight="1">
+    <row r="31" spans="1:15" ht="13" customHeight="1">
       <c r="B31" s="33" t="s">
         <v>979</v>
       </c>
@@ -5952,213 +6012,213 @@
       <c r="D31" s="33" t="s">
         <v>979</v>
       </c>
-      <c r="F31" s="33" t="s">
+      <c r="G31" s="33" t="s">
         <v>410</v>
       </c>
-      <c r="J31" s="33" t="s">
+      <c r="K31" s="33" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="13" customHeight="1">
-      <c r="F32" s="33" t="s">
+    <row r="32" spans="1:15" ht="13" customHeight="1">
+      <c r="G32" s="33" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="13" customHeight="1">
+    <row r="34" spans="1:13" ht="13" customHeight="1">
       <c r="A34" s="49" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="13" customHeight="1">
+    <row r="36" spans="1:13" ht="13" customHeight="1">
       <c r="A36" s="49" t="s">
         <v>950</v>
       </c>
-      <c r="K36" s="33" t="s">
+      <c r="L36" s="33" t="s">
         <v>951</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="13" customHeight="1">
-      <c r="K37" s="33" t="s">
+    <row r="37" spans="1:13" ht="13" customHeight="1">
+      <c r="L37" s="33" t="s">
         <v>952</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="13" customHeight="1">
-      <c r="K38" s="33" t="s">
+    <row r="38" spans="1:13" ht="13" customHeight="1">
+      <c r="L38" s="33" t="s">
         <v>953</v>
       </c>
-      <c r="L38" s="54"/>
-    </row>
-    <row r="39" spans="1:12" ht="13" customHeight="1">
-      <c r="K39" s="33" t="s">
+      <c r="M38" s="54"/>
+    </row>
+    <row r="39" spans="1:13" ht="13" customHeight="1">
+      <c r="L39" s="33" t="s">
         <v>954</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="13" customHeight="1">
+    <row r="41" spans="1:13" ht="13" customHeight="1">
       <c r="A41" s="49" t="s">
         <v>175</v>
       </c>
-      <c r="G41" s="33" t="s">
+      <c r="H41" s="33" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="13" customHeight="1">
-      <c r="G42" s="33" t="s">
+    <row r="42" spans="1:13" ht="13" customHeight="1">
+      <c r="H42" s="33" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="13" customHeight="1">
-      <c r="G43" s="33" t="s">
+    <row r="43" spans="1:13" ht="13" customHeight="1">
+      <c r="H43" s="33" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="13" customHeight="1">
-      <c r="G44" s="33" t="s">
+    <row r="44" spans="1:13" ht="13" customHeight="1">
+      <c r="H44" s="33" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="13" customHeight="1">
+    <row r="46" spans="1:13" ht="13" customHeight="1">
       <c r="A46" s="49" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="13" customHeight="1">
+    <row r="48" spans="1:13" ht="13" customHeight="1">
       <c r="A48" s="49" t="s">
         <v>177</v>
       </c>
-      <c r="G48" s="55" t="s">
+      <c r="H48" s="55" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="13" customHeight="1">
-      <c r="G49" s="55" t="s">
+    <row r="49" spans="1:15" ht="13" customHeight="1">
+      <c r="H49" s="55" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="13" customHeight="1">
-      <c r="G50" s="55" t="s">
+    <row r="50" spans="1:15" ht="13" customHeight="1">
+      <c r="H50" s="55" t="s">
         <v>944</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="13" customHeight="1">
+    <row r="52" spans="1:15" ht="13" customHeight="1">
       <c r="A52" s="49" t="s">
         <v>178</v>
       </c>
-      <c r="K52" s="33" t="s">
+      <c r="L52" s="33" t="s">
         <v>398</v>
       </c>
-      <c r="N52" s="33" t="s">
+      <c r="O52" s="33" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="13" customHeight="1">
-      <c r="K53" s="33" t="s">
+    <row r="53" spans="1:15" ht="13" customHeight="1">
+      <c r="L53" s="33" t="s">
         <v>385</v>
       </c>
-      <c r="N53" s="36" t="s">
+      <c r="O53" s="36" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="13" customHeight="1">
-      <c r="K54" s="33" t="s">
+    <row r="54" spans="1:15" ht="13" customHeight="1">
+      <c r="L54" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="N54" s="36" t="s">
+      <c r="O54" s="36" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="13" customHeight="1">
-      <c r="K55" s="33" t="s">
+    <row r="55" spans="1:15" ht="13" customHeight="1">
+      <c r="L55" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="N55" s="36" t="s">
+      <c r="O55" s="36" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="13" customHeight="1">
-      <c r="K56" s="33" t="s">
+    <row r="56" spans="1:15" ht="13" customHeight="1">
+      <c r="L56" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="N56" s="36" t="s">
+      <c r="O56" s="36" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="13" customHeight="1">
-      <c r="K57" s="33" t="s">
+    <row r="57" spans="1:15" ht="13" customHeight="1">
+      <c r="L57" s="33" t="s">
         <v>386</v>
       </c>
-      <c r="N57" s="36" t="s">
+      <c r="O57" s="36" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="13" customHeight="1">
-      <c r="K58" s="33" t="s">
+    <row r="58" spans="1:15" ht="13" customHeight="1">
+      <c r="L58" s="33" t="s">
         <v>925</v>
       </c>
-      <c r="N58" s="36" t="s">
+      <c r="O58" s="36" t="s">
         <v>925</v>
       </c>
     </row>
-    <row r="59" spans="1:14" ht="13" customHeight="1">
-      <c r="K59" s="33" t="s">
+    <row r="59" spans="1:15" ht="13" customHeight="1">
+      <c r="L59" s="33" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="60" spans="1:14" ht="13" customHeight="1">
-      <c r="K60" s="33" t="s">
+    <row r="60" spans="1:15" ht="13" customHeight="1">
+      <c r="L60" s="33" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="61" spans="1:14" ht="13" customHeight="1">
-      <c r="K61" s="33" t="s">
+    <row r="61" spans="1:15" ht="13" customHeight="1">
+      <c r="L61" s="33" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="62" spans="1:14" ht="13" customHeight="1">
-      <c r="K62" s="33" t="s">
+    <row r="62" spans="1:15" ht="13" customHeight="1">
+      <c r="L62" s="33" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="63" spans="1:14" ht="13" customHeight="1">
-      <c r="K63" s="33" t="s">
+    <row r="63" spans="1:15" ht="13" customHeight="1">
+      <c r="L63" s="33" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="64" spans="1:14" ht="13" customHeight="1">
-      <c r="K64" s="33" t="s">
+    <row r="64" spans="1:15" ht="13" customHeight="1">
+      <c r="L64" s="33" t="s">
         <v>925</v>
       </c>
     </row>
-    <row r="65" spans="1:14" ht="13" customHeight="1">
-      <c r="K65" s="33" t="s">
+    <row r="65" spans="1:15" ht="13" customHeight="1">
+      <c r="L65" s="33" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="66" spans="1:14" ht="13" customHeight="1">
-      <c r="K66" s="33" t="s">
+    <row r="66" spans="1:15" ht="13" customHeight="1">
+      <c r="L66" s="33" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="67" spans="1:14" ht="13" customHeight="1">
-      <c r="K67" s="33" t="s">
+    <row r="67" spans="1:15" ht="13" customHeight="1">
+      <c r="L67" s="33" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="68" spans="1:14" ht="13" customHeight="1">
-      <c r="K68" s="33" t="s">
+    <row r="68" spans="1:15" ht="13" customHeight="1">
+      <c r="L68" s="33" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="69" spans="1:14" ht="13" customHeight="1">
-      <c r="K69" s="33" t="s">
+    <row r="69" spans="1:15" ht="13" customHeight="1">
+      <c r="L69" s="33" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="70" spans="1:14" ht="13" customHeight="1">
-      <c r="K70" s="33" t="s">
+    <row r="70" spans="1:15" ht="13" customHeight="1">
+      <c r="L70" s="33" t="s">
         <v>925</v>
       </c>
     </row>
-    <row r="72" spans="1:14" ht="13" customHeight="1">
+    <row r="72" spans="1:15" ht="13" customHeight="1">
       <c r="A72" s="49" t="s">
         <v>179</v>
       </c>
@@ -6168,178 +6228,178 @@
       <c r="C72" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="G72" s="33" t="s">
+      <c r="H72" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="I72" s="33" t="s">
+      <c r="J72" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="N72" s="33" t="s">
+      <c r="O72" s="33" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="73" spans="1:14" ht="13" customHeight="1">
+    <row r="73" spans="1:15" ht="13" customHeight="1">
       <c r="B73" s="33" t="s">
         <v>557</v>
       </c>
       <c r="C73" s="33" t="s">
         <v>557</v>
       </c>
-      <c r="G73" s="33" t="s">
+      <c r="H73" s="33" t="s">
         <v>917</v>
       </c>
-      <c r="I73" s="33" t="s">
+      <c r="J73" s="33" t="s">
         <v>500</v>
       </c>
-      <c r="N73" s="33" t="s">
+      <c r="O73" s="33" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="74" spans="1:14" ht="13" customHeight="1">
+    <row r="74" spans="1:15" ht="13" customHeight="1">
       <c r="B74" s="33" t="s">
         <v>980</v>
       </c>
       <c r="C74" s="33" t="s">
         <v>980</v>
       </c>
-      <c r="G74" s="33" t="s">
+      <c r="H74" s="33" t="s">
         <v>913</v>
       </c>
-      <c r="I74" s="33" t="s">
+      <c r="J74" s="33" t="s">
         <v>498</v>
       </c>
-      <c r="N74" s="33" t="s">
+      <c r="O74" s="33" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="75" spans="1:14" ht="13" customHeight="1">
-      <c r="G75" s="33" t="s">
+    <row r="75" spans="1:15" ht="13" customHeight="1">
+      <c r="H75" s="33" t="s">
         <v>914</v>
       </c>
-      <c r="I75" s="33" t="s">
+      <c r="J75" s="33" t="s">
         <v>499</v>
       </c>
-      <c r="N75" s="33" t="s">
+      <c r="O75" s="33" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="76" spans="1:14" ht="13" customHeight="1">
-      <c r="G76" s="33" t="s">
+    <row r="76" spans="1:15" ht="13" customHeight="1">
+      <c r="H76" s="33" t="s">
         <v>915</v>
       </c>
-      <c r="N76" s="33" t="s">
+      <c r="O76" s="33" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="77" spans="1:14" ht="13" customHeight="1">
-      <c r="G77" s="33" t="s">
+    <row r="77" spans="1:15" ht="13" customHeight="1">
+      <c r="H77" s="33" t="s">
         <v>916</v>
       </c>
-      <c r="N77" s="33" t="s">
+      <c r="O77" s="33" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="78" spans="1:14" ht="13" customHeight="1">
-      <c r="G78" s="33" t="s">
+    <row r="78" spans="1:15" ht="13" customHeight="1">
+      <c r="H78" s="33" t="s">
         <v>919</v>
       </c>
-      <c r="N78" s="33" t="s">
+      <c r="O78" s="33" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="79" spans="1:14" ht="13" customHeight="1">
-      <c r="G79" s="33" t="s">
+    <row r="79" spans="1:15" ht="13" customHeight="1">
+      <c r="H79" s="33" t="s">
         <v>920</v>
       </c>
     </row>
-    <row r="80" spans="1:14" ht="13" customHeight="1">
-      <c r="G80" s="33" t="s">
+    <row r="80" spans="1:15" ht="13" customHeight="1">
+      <c r="H80" s="33" t="s">
         <v>921</v>
       </c>
     </row>
-    <row r="81" spans="1:14" ht="13" customHeight="1">
-      <c r="G81" s="33" t="s">
+    <row r="81" spans="1:15" ht="13" customHeight="1">
+      <c r="H81" s="33" t="s">
         <v>918</v>
       </c>
     </row>
-    <row r="82" spans="1:14" ht="13" customHeight="1">
-      <c r="G82" s="33" t="s">
+    <row r="82" spans="1:15" ht="13" customHeight="1">
+      <c r="H82" s="33" t="s">
         <v>923</v>
       </c>
     </row>
-    <row r="83" spans="1:14" ht="13" customHeight="1">
-      <c r="G83" s="33" t="s">
+    <row r="83" spans="1:15" ht="13" customHeight="1">
+      <c r="H83" s="33" t="s">
         <v>877</v>
       </c>
     </row>
-    <row r="85" spans="1:14" ht="13" customHeight="1">
+    <row r="85" spans="1:15" ht="13" customHeight="1">
       <c r="A85" s="49" t="s">
         <v>180</v>
       </c>
-      <c r="I85" s="33" t="s">
+      <c r="J85" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="K85" s="33" t="s">
+      <c r="L85" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="N85" s="33" t="s">
+      <c r="O85" s="33" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="86" spans="1:14" ht="13" customHeight="1">
-      <c r="K86" s="33" t="s">
+    <row r="86" spans="1:15" ht="13" customHeight="1">
+      <c r="L86" s="33" t="s">
         <v>948</v>
       </c>
-      <c r="N86" s="33" t="s">
+      <c r="O86" s="33" t="s">
         <v>533</v>
       </c>
     </row>
-    <row r="87" spans="1:14" ht="13" customHeight="1">
-      <c r="K87" s="33" t="s">
+    <row r="87" spans="1:15" ht="13" customHeight="1">
+      <c r="L87" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="N87" s="33" t="s">
+      <c r="O87" s="33" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="88" spans="1:14" ht="13" customHeight="1">
-      <c r="K88" s="33" t="s">
+    <row r="88" spans="1:15" ht="13" customHeight="1">
+      <c r="L88" s="33" t="s">
         <v>949</v>
       </c>
-      <c r="N88" s="33" t="s">
+      <c r="O88" s="33" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="89" spans="1:14" ht="13" customHeight="1">
-      <c r="I89" s="33" t="s">
+    <row r="89" spans="1:15" ht="13" customHeight="1">
+      <c r="J89" s="33" t="s">
         <v>220</v>
       </c>
-      <c r="K89" s="33" t="s">
+      <c r="L89" s="33" t="s">
         <v>220</v>
       </c>
-      <c r="N89" s="33" t="s">
+      <c r="O89" s="33" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="90" spans="1:14" ht="13" customHeight="1">
-      <c r="I90" s="33" t="s">
+    <row r="90" spans="1:15" ht="13" customHeight="1">
+      <c r="J90" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="K90" s="33" t="s">
+      <c r="L90" s="33" t="s">
         <v>532</v>
       </c>
-      <c r="N90" s="33" t="s">
+      <c r="O90" s="33" t="s">
         <v>532</v>
       </c>
     </row>
-    <row r="91" spans="1:14" ht="13" customHeight="1">
-      <c r="I91" s="33" t="s">
+    <row r="91" spans="1:15" ht="13" customHeight="1">
+      <c r="J91" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="K91" s="33" t="s">
+      <c r="L91" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="N91" s="33" t="s">
+      <c r="O91" s="33" t="s">
         <v>20</v>
       </c>
     </row>
@@ -7752,14 +7812,14 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCC9497B-7600-374B-8989-8C7FAD24A60F}">
-  <dimension ref="A1:H90"/>
+  <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B10" sqref="B10"/>
       <selection pane="topRight" activeCell="B10" sqref="B10"/>
       <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
-      <selection pane="bottomRight" activeCell="G8" sqref="G8"/>
+      <selection pane="bottomRight" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="40.83203125" defaultRowHeight="13" customHeight="1"/>
@@ -7768,7 +7828,7 @@
     <col min="2" max="16384" width="40.83203125" style="43"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="40" customFormat="1" ht="13" customHeight="1">
+    <row r="1" spans="1:9" s="40" customFormat="1" ht="13" customHeight="1">
       <c r="A1" s="39"/>
       <c r="B1" s="40" t="s">
         <v>222</v>
@@ -7791,8 +7851,11 @@
       <c r="H1" s="40" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" s="40" customFormat="1" ht="13" customHeight="1">
+      <c r="I1" s="40" t="s">
+        <v>1209</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="40" customFormat="1" ht="13" customHeight="1">
       <c r="A2" s="39"/>
       <c r="B2" s="40" t="s">
         <v>960</v>
@@ -7811,7 +7874,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="13" customHeight="1">
+    <row r="3" spans="1:9" ht="13" customHeight="1">
       <c r="A3" s="42" t="s">
         <v>795</v>
       </c>
@@ -7822,7 +7885,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="13" customHeight="1">
+    <row r="4" spans="1:9" ht="13" customHeight="1">
       <c r="A4" s="42" t="s">
         <v>796</v>
       </c>
@@ -7830,7 +7893,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="13" customHeight="1">
+    <row r="5" spans="1:9" ht="13" customHeight="1">
       <c r="A5" s="42" t="s">
         <v>801</v>
       </c>
@@ -7855,12 +7918,15 @@
       <c r="H5" s="43" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="13" customHeight="1">
+      <c r="I5" s="43" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="13" customHeight="1">
       <c r="A6" s="42"/>
       <c r="C6" s="44"/>
     </row>
-    <row r="7" spans="1:8" ht="13" customHeight="1">
+    <row r="7" spans="1:9" ht="13" customHeight="1">
       <c r="A7" s="42" t="s">
         <v>819</v>
       </c>
@@ -7885,8 +7951,11 @@
       <c r="H7" s="43" t="s">
         <v>821</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="13" customHeight="1">
+      <c r="I7" s="43" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="13" customHeight="1">
       <c r="A8" s="42" t="s">
         <v>169</v>
       </c>
@@ -7911,12 +7980,15 @@
       <c r="H8" s="44" t="s">
         <v>1067</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="13" customHeight="1">
+      <c r="I8" s="44" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="13" customHeight="1">
       <c r="A9" s="42"/>
       <c r="C9" s="44"/>
     </row>
-    <row r="10" spans="1:8" ht="13" customHeight="1">
+    <row r="10" spans="1:9" ht="13" customHeight="1">
       <c r="A10" s="42" t="s">
         <v>170</v>
       </c>
@@ -7941,8 +8013,11 @@
       <c r="H10" s="43" t="s">
         <v>457</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="13" customHeight="1">
+      <c r="I10" s="43" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="13" customHeight="1">
       <c r="A11" s="42"/>
       <c r="B11" s="43" t="s">
         <v>476</v>
@@ -7965,8 +8040,11 @@
       <c r="H11" s="43" t="s">
         <v>464</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="13" customHeight="1">
+      <c r="I11" s="43" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="13" customHeight="1">
       <c r="A12" s="42"/>
       <c r="B12" s="43" t="s">
         <v>475</v>
@@ -7989,8 +8067,11 @@
       <c r="H12" s="43" t="s">
         <v>1065</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="13" customHeight="1">
+      <c r="I12" s="43" t="s">
+        <v>1213</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="13" customHeight="1">
       <c r="A13" s="42"/>
       <c r="C13" s="43" t="s">
         <v>852</v>
@@ -7999,7 +8080,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="13" customHeight="1">
+    <row r="14" spans="1:9" ht="13" customHeight="1">
       <c r="A14" s="42"/>
       <c r="C14" s="43" t="s">
         <v>853</v>
@@ -8008,11 +8089,11 @@
         <v>375</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="13" customHeight="1">
+    <row r="15" spans="1:9" ht="13" customHeight="1">
       <c r="A15" s="42"/>
       <c r="C15" s="44"/>
     </row>
-    <row r="16" spans="1:8" ht="13" customHeight="1">
+    <row r="16" spans="1:9" ht="13" customHeight="1">
       <c r="A16" s="42" t="s">
         <v>171</v>
       </c>
@@ -9583,12 +9664,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9947295B-8D1F-FB48-972A-B6AD7BBC4112}">
   <dimension ref="A1:Y153"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B10" sqref="B10"/>
       <selection pane="topRight" activeCell="B10" sqref="B10"/>
       <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
-      <selection pane="bottomRight" activeCell="S13" sqref="S13"/>
+      <selection pane="bottomRight" activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="46.83203125" defaultRowHeight="13" customHeight="1"/>

</xml_diff>

<commit_message>
some usgs data added
</commit_message>
<xml_diff>
--- a/data/readfiles/generate_yaml.xlsx
+++ b/data/readfiles/generate_yaml.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chughes/Documents/Git/SLiDE/data/readfiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{134DF1E9-EEE4-6547-9976-0A13C3586C7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4794DD3C-2962-094C-97F6-E3958FF283D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="5" xr2:uid="{ECEEE8D6-CC61-454D-945D-45D0FFF64D45}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="7" xr2:uid="{ECEEE8D6-CC61-454D-945D-45D0FFF64D45}"/>
   </bookViews>
   <sheets>
-    <sheet name="map_bluenote" sheetId="5" state="hidden" r:id="rId1"/>
+    <sheet name="map_bluenote" sheetId="5" r:id="rId1"/>
     <sheet name="map_parse" sheetId="2" r:id="rId2"/>
     <sheet name="map_scale" sheetId="3" r:id="rId3"/>
     <sheet name="map_crosswalk" sheetId="7" r:id="rId4"/>
     <sheet name="map_experiment" sheetId="8" state="hidden" r:id="rId5"/>
-    <sheet name="parse" sheetId="4" r:id="rId6"/>
+    <sheet name="input" sheetId="4" r:id="rId6"/>
     <sheet name="share" sheetId="10" r:id="rId7"/>
-    <sheet name="parse (2)" sheetId="6" state="hidden" r:id="rId8"/>
+    <sheet name="experiment" sheetId="12" r:id="rId8"/>
+    <sheet name="parse (2)" sheetId="6" state="hidden" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3127" uniqueCount="1216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3281" uniqueCount="1275">
   <si>
     <t>bea_supply</t>
   </si>
@@ -3688,6 +3689,183 @@
   </si>
   <si>
     <t>PathOut: [data, coremaps, crosswalk, fd.csv]</t>
+  </si>
+  <si>
+    <t>usgs_water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  sheet: DataDictionary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  descriptor: data</t>
+  </si>
+  <si>
+    <t>PathIn:  [data, datasources, USGS]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  name:  usco2015v2.0.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  range: A1:B142</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - {from: Column Tag, to: code}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    val: [STATE, STATEFIPS, COUNTY, COUNTYFIPS, FIPS, YEAR]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - {from: Attribute,  to: desc}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - col: Column Tag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    output: [sector_code, source_code]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - on:     (?&lt;sector_code&gt;.*)-(?&lt;source_code&gt;.*)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    input:  code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - {col: code,        type: String}</t>
+  </si>
+  <si>
+    <t>PathIn:  [data, experiment]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  range: A2:EK3225</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  sheet: usco2015v2.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  descriptor: 2015</t>
+  </si>
+  <si>
+    <t>usgs_water_state</t>
+  </si>
+  <si>
+    <t>usgs_water_county</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - {col: sector,      type: String}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - {from: YEAR,   to: yr}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - {from: FIPS,   to: county}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - {from: STATE,  to: state}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - col: value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    from: [--, N/A]</t>
+  </si>
+  <si>
+    <t>PathOut: [data, experiment, usgs_water.csv]</t>
+  </si>
+  <si>
+    <t>PathOut: [data, experiment, usgs_water_state.csv]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  name: usgs_water.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  input:  [yr, r, sector]</t>
+  </si>
+  <si>
+    <t># - {col: desc,        type: String}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - on:     (?&lt;sector_desc&gt;Total|.*?(?=,)),*\s(?&lt;source_desc&gt;.*), in (?&lt;units&gt;.*)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    output: [sector_desc, source_desc, units]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - on:     (?&lt;source_desc&gt;.*), (?&lt;salinity&gt;.*)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    input:  source_desc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    output: [source_desc, salinity]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    from: ""</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    to:   missing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - on:     (?&lt;units&gt;.*?(?=\[)|.*$)(?&lt;notes&gt;.*)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    output: [units, notes]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - col: [salinity, notes]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - {col: notes,       type: String}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - {col: salinity,    type: String}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    from: lower</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - col: [sector_desc, source_desc, salinity]</t>
+  </si>
+  <si>
+    <t>usgs_dict</t>
+  </si>
+  <si>
+    <t>PathOut: [data, experiment, usgs_water_county.csv]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - {from: county, to: r}</t>
+  </si>
+  <si>
+    <t>PathOut: [data, coremaps, parse, usgs.csv]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - file:   [parse, usgs.csv]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - col: [STATEFIPS, COUNTY, COUNTYFIPS]</t>
+  </si>
+  <si>
+    <t># - {from: COUNTY, to: county_desc}</t>
+  </si>
+  <si>
+    <t># - {col: county_desc, type: String}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  on:  [yr, state, county]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  var: code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    from:   code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    to:     [sector_desc, source_desc, salinity, units]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    output: [sector, source, salinity, units]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - {col: source,      type: String}</t>
   </si>
 </sst>
 </file>
@@ -3824,7 +4002,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -3937,11 +4115,40 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="47">
+  <dxfs count="71">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="9"/>
@@ -3949,6 +4156,203 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4696,8 +5100,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{146E3C27-1365-884B-A69E-493300A2017A}">
   <dimension ref="A1:H85"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:E11"/>
+    <sheetView showGridLines="0" topLeftCell="C17" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -5389,7 +5793,7 @@
       <selection activeCell="M11" sqref="M11"/>
       <selection pane="topRight" activeCell="M11" sqref="M11"/>
       <selection pane="bottomLeft" activeCell="M11" sqref="M11"/>
-      <selection pane="bottomRight" activeCell="E28" sqref="E28"/>
+      <selection pane="bottomRight" activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="40.83203125" defaultRowHeight="13" customHeight="1"/>
@@ -6405,15 +6809,15 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="46" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="1" operator="equal">
       <formula>" "</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="3">
+    <cfRule type="expression" dxfId="69" priority="3">
       <formula>_xlfn.ISFORMULA(A1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:XFD1048576">
-    <cfRule type="expression" dxfId="44" priority="2">
+    <cfRule type="expression" dxfId="68" priority="2">
       <formula>AND(ISBLANK($A2), NOT(ISBLANK($A3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6427,11 +6831,11 @@
   <dimension ref="A1:L87"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B22" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B10" sqref="B10"/>
       <selection pane="topRight" activeCell="B10" sqref="B10"/>
       <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
-      <selection pane="bottomRight" activeCell="B13" sqref="B13"/>
+      <selection pane="bottomRight" activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="40.83203125" defaultRowHeight="13" customHeight="1"/>
@@ -7793,15 +8197,15 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="43" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="2" operator="equal">
       <formula>" "</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="56">
+    <cfRule type="expression" dxfId="66" priority="56">
       <formula>_xlfn.ISFORMULA(A1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:XFD1048576">
-    <cfRule type="expression" dxfId="41" priority="3">
+    <cfRule type="expression" dxfId="65" priority="3">
       <formula>AND(ISBLANK($A2), NOT(ISBLANK($A3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7819,7 +8223,7 @@
       <selection activeCell="B10" sqref="B10"/>
       <selection pane="topRight" activeCell="B10" sqref="B10"/>
       <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
-      <selection pane="bottomRight" activeCell="D23" sqref="D23"/>
+      <selection pane="bottomRight" activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="40.83203125" defaultRowHeight="13" customHeight="1"/>
@@ -8867,15 +9271,15 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="40" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="1" operator="equal">
       <formula>" "</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="36">
+    <cfRule type="expression" dxfId="63" priority="36">
       <formula>_xlfn.ISFORMULA(A1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:XFD1048576">
-    <cfRule type="expression" dxfId="38" priority="2">
+    <cfRule type="expression" dxfId="62" priority="2">
       <formula>AND(ISBLANK($A3), NOT(ISBLANK($A4)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9582,77 +9986,77 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D81:D83">
-    <cfRule type="expression" dxfId="37" priority="5">
+    <cfRule type="expression" dxfId="61" priority="5">
       <formula>_xlfn.ISFORMULA(D81)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:C7">
-    <cfRule type="expression" dxfId="36" priority="16">
+    <cfRule type="expression" dxfId="60" priority="16">
       <formula>_xlfn.ISFORMULA(C6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18:E22">
-    <cfRule type="expression" dxfId="35" priority="15">
+    <cfRule type="expression" dxfId="59" priority="15">
       <formula>_xlfn.ISFORMULA(E18)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:C31">
-    <cfRule type="expression" dxfId="34" priority="14">
+    <cfRule type="expression" dxfId="58" priority="14">
       <formula>_xlfn.ISFORMULA(C28)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C82:C84">
-    <cfRule type="expression" dxfId="33" priority="13">
+    <cfRule type="expression" dxfId="57" priority="13">
       <formula>_xlfn.ISFORMULA(C82)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="expression" dxfId="32" priority="11">
+    <cfRule type="expression" dxfId="56" priority="11">
       <formula>_xlfn.ISFORMULA(D7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="expression" dxfId="31" priority="12">
+    <cfRule type="expression" dxfId="55" priority="12">
       <formula>_xlfn.ISFORMULA(D6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9:D13">
-    <cfRule type="expression" dxfId="30" priority="10">
+    <cfRule type="expression" dxfId="54" priority="10">
       <formula>_xlfn.ISFORMULA(D9)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32">
-    <cfRule type="expression" dxfId="29" priority="9">
+    <cfRule type="expression" dxfId="53" priority="9">
       <formula>_xlfn.ISFORMULA(D32)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D28 D32">
-    <cfRule type="expression" dxfId="28" priority="8">
+    <cfRule type="expression" dxfId="52" priority="8">
       <formula>_xlfn.ISFORMULA(D28)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30">
-    <cfRule type="expression" dxfId="27" priority="7">
+    <cfRule type="expression" dxfId="51" priority="7">
       <formula>_xlfn.ISFORMULA(D30)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9:C10">
-    <cfRule type="expression" dxfId="26" priority="4">
+    <cfRule type="expression" dxfId="50" priority="4">
       <formula>_xlfn.ISFORMULA(C9)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D45 D48:D49">
-    <cfRule type="expression" dxfId="25" priority="3">
+    <cfRule type="expression" dxfId="49" priority="3">
       <formula>_xlfn.ISFORMULA(D45)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23">
-    <cfRule type="expression" dxfId="24" priority="2">
+    <cfRule type="expression" dxfId="48" priority="2">
       <formula>_xlfn.ISFORMULA(C23)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B82:B84">
-    <cfRule type="expression" dxfId="23" priority="1">
+    <cfRule type="expression" dxfId="47" priority="1">
       <formula>_xlfn.ISFORMULA(B82)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9664,12 +10068,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9947295B-8D1F-FB48-972A-B6AD7BBC4112}">
   <dimension ref="A1:Y153"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B77" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B10" sqref="B10"/>
       <selection pane="topRight" activeCell="B10" sqref="B10"/>
       <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
-      <selection pane="bottomRight" activeCell="T16" sqref="T16"/>
+      <selection pane="bottomRight" activeCell="B118" sqref="B118:B123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="46.83203125" defaultRowHeight="13" customHeight="1"/>
@@ -15767,17 +16171,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1 A3:XFD1048576 A2:N2 P2:XFD2">
-    <cfRule type="expression" dxfId="22" priority="1">
+    <cfRule type="expression" dxfId="46" priority="1">
       <formula>_xlfn.ISFORMULA(A1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:XFD1048576 A2:N2 P2:XFD2">
-    <cfRule type="expression" dxfId="21" priority="168">
+    <cfRule type="expression" dxfId="45" priority="168">
       <formula>AND(COUNTA($A2:$AA2)=0, NOT(ISBLANK($A3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1048576:XFD1048576">
-    <cfRule type="expression" dxfId="20" priority="181">
+    <cfRule type="expression" dxfId="44" priority="181">
       <formula>AND(COUNTA(#REF!)=0, NOT(ISBLANK($A1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15790,11 +16194,11 @@
   <dimension ref="A1:Y155"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B10" sqref="B10"/>
       <selection pane="topRight" activeCell="B10" sqref="B10"/>
       <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
-      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomRight" activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="46.83203125" defaultRowHeight="13" customHeight="1"/>
@@ -17303,72 +17707,72 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="P2:XFD2 C17 A79:B80 A17 A11:C11 G24:XFD24 A18:C21 H17:XFD23 A22:D23 A7:D10 A12:D15 E7:XFD15 A1:XFD1 A2:N2 D79:XFD80 A81:XFD1048576 A16:XFD16 A3:XFD6 A24:E24 A25:XFD78 E17:E22">
-    <cfRule type="expression" dxfId="19" priority="26">
+    <cfRule type="expression" dxfId="43" priority="26">
       <formula>_xlfn.ISFORMULA(A1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C79:C80">
-    <cfRule type="expression" dxfId="18" priority="22">
+    <cfRule type="expression" dxfId="42" priority="22">
       <formula>_xlfn.ISFORMULA(C79)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1048576:XFD1048576">
-    <cfRule type="expression" dxfId="17" priority="213">
+    <cfRule type="expression" dxfId="41" priority="213">
       <formula>AND(COUNTA(#REF!)=0, NOT(ISBLANK($A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="expression" dxfId="16" priority="20">
+    <cfRule type="expression" dxfId="40" priority="20">
       <formula>_xlfn.ISFORMULA(D11)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F17:F21">
-    <cfRule type="expression" dxfId="15" priority="18">
+    <cfRule type="expression" dxfId="39" priority="18">
       <formula>_xlfn.ISFORMULA(F17)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F22">
-    <cfRule type="expression" dxfId="14" priority="16">
+    <cfRule type="expression" dxfId="38" priority="16">
       <formula>_xlfn.ISFORMULA(F22)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F23:F24">
-    <cfRule type="expression" dxfId="13" priority="14">
+    <cfRule type="expression" dxfId="37" priority="14">
       <formula>_xlfn.ISFORMULA(F23)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G17:G23">
-    <cfRule type="expression" dxfId="12" priority="10">
+    <cfRule type="expression" dxfId="36" priority="10">
       <formula>_xlfn.ISFORMULA(G17)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17:D21">
-    <cfRule type="expression" dxfId="11" priority="8">
+    <cfRule type="expression" dxfId="35" priority="8">
       <formula>_xlfn.ISFORMULA(D17)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:N2 P2:XFD2 C17 A17 E3:XFD16 E25:XFD33 E24 A2:D10 A12:D16 A37:XFD1048576 A18:C19 D17:XFD19 F20:XFD24 A20:D33 B11:D11">
-    <cfRule type="expression" dxfId="10" priority="273">
+    <cfRule type="expression" dxfId="34" priority="273">
       <formula>AND(COUNTA($A2:$AA2)=0, NOT(ISBLANK($A3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:F15">
-    <cfRule type="expression" dxfId="9" priority="353">
+    <cfRule type="expression" dxfId="33" priority="353">
       <formula>AND(COUNTA($A17:$AA17)=0, NOT(ISBLANK($A18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36:XFD36">
-    <cfRule type="expression" dxfId="8" priority="361">
+    <cfRule type="expression" dxfId="32" priority="361">
       <formula>AND(COUNTA($A36:$AA36)=0, NOT(ISBLANK($A38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A34:XFD35">
-    <cfRule type="expression" dxfId="7" priority="368">
+    <cfRule type="expression" dxfId="31" priority="368">
       <formula>AND(COUNTA($A34:$AA34)=0, NOT(ISBLANK($A37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20:E22">
-    <cfRule type="expression" dxfId="6" priority="376">
+    <cfRule type="expression" dxfId="30" priority="376">
       <formula>AND(COUNTA($A21:$AA21)=0, NOT(ISBLANK($A22)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17377,6 +17781,1589 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{266920FD-CED0-424B-9125-46B736D1EB06}">
+  <dimension ref="A1:T156"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B31" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="B10" sqref="B10"/>
+      <selection pane="topRight" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomRight" activeCell="C79" sqref="C79"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="46.83203125" defaultRowHeight="13" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="14.83203125" style="56" customWidth="1"/>
+    <col min="2" max="10" width="46.83203125" style="56"/>
+    <col min="11" max="11" width="46.83203125" style="59"/>
+    <col min="12" max="16384" width="46.83203125" style="56"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" s="57" customFormat="1" ht="13" customHeight="1">
+      <c r="B1" s="57" t="s">
+        <v>1261</v>
+      </c>
+      <c r="C1" s="57" t="s">
+        <v>1216</v>
+      </c>
+      <c r="D1" s="57" t="s">
+        <v>1234</v>
+      </c>
+      <c r="E1" s="57" t="s">
+        <v>1235</v>
+      </c>
+      <c r="K1" s="58"/>
+    </row>
+    <row r="2" spans="1:20" ht="13" customHeight="1">
+      <c r="A2" s="56" t="s">
+        <v>1111</v>
+      </c>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+    </row>
+    <row r="3" spans="1:20" ht="13" customHeight="1">
+      <c r="A3" s="56" t="s">
+        <v>795</v>
+      </c>
+      <c r="L3" s="59"/>
+      <c r="M3" s="59"/>
+      <c r="N3" s="59"/>
+      <c r="O3" s="59"/>
+    </row>
+    <row r="4" spans="1:20" ht="13" customHeight="1">
+      <c r="A4" s="56" t="s">
+        <v>796</v>
+      </c>
+      <c r="L4" s="59"/>
+      <c r="M4" s="59"/>
+      <c r="N4" s="59"/>
+      <c r="O4" s="59"/>
+    </row>
+    <row r="5" spans="1:20" ht="13" customHeight="1">
+      <c r="A5" s="56" t="s">
+        <v>1087</v>
+      </c>
+      <c r="L5" s="59"/>
+      <c r="M5" s="59"/>
+      <c r="N5" s="59"/>
+      <c r="O5" s="59"/>
+    </row>
+    <row r="6" spans="1:20" ht="13" customHeight="1">
+      <c r="A6" s="56" t="s">
+        <v>1096</v>
+      </c>
+      <c r="L6" s="59"/>
+      <c r="M6" s="59"/>
+      <c r="N6" s="59"/>
+      <c r="O6" s="59"/>
+    </row>
+    <row r="7" spans="1:20" ht="13" customHeight="1">
+      <c r="A7" s="56" t="s">
+        <v>801</v>
+      </c>
+      <c r="B7" s="60" t="s">
+        <v>396</v>
+      </c>
+      <c r="C7" s="60" t="s">
+        <v>396</v>
+      </c>
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="60"/>
+      <c r="G7" s="60"/>
+      <c r="H7" s="60"/>
+      <c r="I7" s="60"/>
+      <c r="J7" s="60"/>
+      <c r="L7" s="60"/>
+      <c r="M7" s="60"/>
+      <c r="N7" s="60"/>
+      <c r="O7" s="60"/>
+      <c r="P7" s="60"/>
+      <c r="Q7" s="60"/>
+      <c r="R7" s="60"/>
+      <c r="S7" s="60"/>
+      <c r="T7" s="60"/>
+    </row>
+    <row r="8" spans="1:20" ht="13" customHeight="1">
+      <c r="A8" s="56" t="s">
+        <v>969</v>
+      </c>
+      <c r="B8" s="60"/>
+      <c r="C8" s="60"/>
+      <c r="D8" s="60"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="60"/>
+      <c r="G8" s="60"/>
+      <c r="H8" s="60"/>
+      <c r="I8" s="60"/>
+      <c r="J8" s="60"/>
+      <c r="K8" s="60"/>
+      <c r="L8" s="60"/>
+      <c r="M8" s="60"/>
+      <c r="N8" s="60"/>
+      <c r="O8" s="60"/>
+      <c r="P8" s="60"/>
+      <c r="Q8" s="60"/>
+      <c r="R8" s="60"/>
+      <c r="S8" s="60"/>
+      <c r="T8" s="60"/>
+    </row>
+    <row r="10" spans="1:20" ht="13" customHeight="1">
+      <c r="A10" s="56" t="s">
+        <v>819</v>
+      </c>
+      <c r="B10" s="56" t="s">
+        <v>1219</v>
+      </c>
+      <c r="C10" s="56" t="s">
+        <v>1219</v>
+      </c>
+      <c r="D10" s="60" t="s">
+        <v>1230</v>
+      </c>
+      <c r="E10" s="60" t="s">
+        <v>1230</v>
+      </c>
+      <c r="I10" s="60"/>
+      <c r="J10" s="60"/>
+      <c r="L10" s="59"/>
+      <c r="M10" s="59"/>
+      <c r="N10" s="59"/>
+      <c r="Q10" s="60"/>
+      <c r="R10" s="60"/>
+      <c r="S10" s="60"/>
+      <c r="T10" s="60"/>
+    </row>
+    <row r="11" spans="1:20" ht="13" customHeight="1">
+      <c r="A11" s="56" t="s">
+        <v>169</v>
+      </c>
+      <c r="B11" s="56" t="s">
+        <v>1264</v>
+      </c>
+      <c r="C11" s="56" t="s">
+        <v>1242</v>
+      </c>
+      <c r="D11" s="56" t="s">
+        <v>1243</v>
+      </c>
+      <c r="E11" s="56" t="s">
+        <v>1262</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="13" customHeight="1">
+      <c r="A13" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="B13" s="56" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="56" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="56" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="56" t="s">
+        <v>8</v>
+      </c>
+      <c r="I13" s="61"/>
+      <c r="S13" s="60"/>
+    </row>
+    <row r="14" spans="1:20" ht="13" customHeight="1">
+      <c r="B14" s="56" t="s">
+        <v>1220</v>
+      </c>
+      <c r="C14" s="56" t="s">
+        <v>1220</v>
+      </c>
+      <c r="D14" s="56" t="s">
+        <v>1244</v>
+      </c>
+      <c r="E14" s="56" t="str">
+        <f>D14</f>
+        <v xml:space="preserve">  name: usgs_water.csv</v>
+      </c>
+      <c r="I14" s="61"/>
+    </row>
+    <row r="15" spans="1:20" ht="13" customHeight="1">
+      <c r="B15" s="56" t="s">
+        <v>1221</v>
+      </c>
+      <c r="C15" s="56" t="s">
+        <v>1231</v>
+      </c>
+      <c r="D15" s="56" t="s">
+        <v>1233</v>
+      </c>
+      <c r="E15" s="56" t="str">
+        <f>D15</f>
+        <v xml:space="preserve">  descriptor: 2015</v>
+      </c>
+      <c r="I15" s="61"/>
+    </row>
+    <row r="16" spans="1:20" ht="13" customHeight="1">
+      <c r="B16" s="56" t="s">
+        <v>1217</v>
+      </c>
+      <c r="C16" s="56" t="s">
+        <v>1232</v>
+      </c>
+      <c r="I16" s="61"/>
+    </row>
+    <row r="17" spans="1:16" ht="13" customHeight="1">
+      <c r="B17" s="56" t="s">
+        <v>1218</v>
+      </c>
+      <c r="C17" s="56" t="s">
+        <v>1233</v>
+      </c>
+      <c r="I17" s="61"/>
+    </row>
+    <row r="19" spans="1:16" ht="13" customHeight="1">
+      <c r="A19" s="56" t="s">
+        <v>172</v>
+      </c>
+      <c r="B19" s="56" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="56" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="56" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="56" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="13" customHeight="1">
+      <c r="B20" s="56" t="s">
+        <v>1229</v>
+      </c>
+      <c r="C20" s="56" t="s">
+        <v>572</v>
+      </c>
+      <c r="D20" s="56" t="s">
+        <v>585</v>
+      </c>
+      <c r="E20" s="56" t="str">
+        <f>D20</f>
+        <v xml:space="preserve">  - {col: yr,     type: Int}</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="13" customHeight="1">
+      <c r="B21" s="56" t="s">
+        <v>121</v>
+      </c>
+      <c r="C21" s="56" t="s">
+        <v>108</v>
+      </c>
+      <c r="D21" s="56" t="s">
+        <v>614</v>
+      </c>
+      <c r="E21" s="56" t="str">
+        <f t="shared" ref="E21:E23" si="0">D21</f>
+        <v xml:space="preserve">  - {col: r,      type: String}</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="13" customHeight="1">
+      <c r="B22" s="56" t="s">
+        <v>120</v>
+      </c>
+      <c r="C22" s="56" t="s">
+        <v>710</v>
+      </c>
+      <c r="D22" s="56" t="s">
+        <v>584</v>
+      </c>
+      <c r="E22" s="56" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  - {col: sector, type: String}</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="13" customHeight="1">
+      <c r="B23" s="56" t="s">
+        <v>1246</v>
+      </c>
+      <c r="C23" s="56" t="s">
+        <v>1268</v>
+      </c>
+      <c r="D23" s="56" t="s">
+        <v>149</v>
+      </c>
+      <c r="E23" s="56" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  - {col: value,  type: Float64}</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="13" customHeight="1">
+      <c r="B24" s="56" t="s">
+        <v>404</v>
+      </c>
+      <c r="C24" s="56" t="s">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="13" customHeight="1">
+      <c r="B25" s="56" t="s">
+        <v>405</v>
+      </c>
+      <c r="C25" s="56" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="13" customHeight="1">
+      <c r="B26" s="56" t="s">
+        <v>1258</v>
+      </c>
+      <c r="C26" s="56" t="s">
+        <v>1274</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="13" customHeight="1">
+      <c r="B27" s="56" t="s">
+        <v>110</v>
+      </c>
+      <c r="C27" s="56" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" ht="13" customHeight="1">
+      <c r="B28" s="56" t="s">
+        <v>1257</v>
+      </c>
+      <c r="C28" s="56" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" ht="13" customHeight="1">
+      <c r="A30" s="56" t="s">
+        <v>173</v>
+      </c>
+      <c r="B30" s="56" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" s="56" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" s="56" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="56" t="s">
+        <v>10</v>
+      </c>
+      <c r="J30" s="60"/>
+      <c r="L30" s="59"/>
+      <c r="M30" s="59"/>
+      <c r="N30" s="60"/>
+      <c r="P30" s="60"/>
+    </row>
+    <row r="31" spans="1:16" ht="13" customHeight="1">
+      <c r="B31" s="56" t="s">
+        <v>1222</v>
+      </c>
+      <c r="C31" s="56" t="s">
+        <v>1237</v>
+      </c>
+      <c r="D31" s="56" t="s">
+        <v>663</v>
+      </c>
+      <c r="E31" s="56" t="s">
+        <v>1263</v>
+      </c>
+      <c r="J31" s="60"/>
+      <c r="L31" s="59"/>
+      <c r="M31" s="59"/>
+      <c r="N31" s="60"/>
+      <c r="P31" s="60"/>
+    </row>
+    <row r="32" spans="1:16" ht="13" customHeight="1">
+      <c r="B32" s="56" t="s">
+        <v>1224</v>
+      </c>
+      <c r="C32" s="56" t="s">
+        <v>1239</v>
+      </c>
+      <c r="J32" s="60"/>
+      <c r="L32" s="60"/>
+    </row>
+    <row r="33" spans="1:20" ht="13" customHeight="1">
+      <c r="B33" s="56" t="s">
+        <v>1224</v>
+      </c>
+      <c r="C33" s="56" t="s">
+        <v>1267</v>
+      </c>
+      <c r="F33" s="60"/>
+      <c r="G33" s="60"/>
+      <c r="H33" s="60"/>
+      <c r="I33" s="60"/>
+      <c r="J33" s="60"/>
+      <c r="L33" s="59"/>
+      <c r="M33" s="59"/>
+      <c r="N33" s="59"/>
+      <c r="O33" s="59"/>
+      <c r="P33" s="60"/>
+      <c r="Q33" s="60"/>
+      <c r="R33" s="60"/>
+      <c r="S33" s="60"/>
+    </row>
+    <row r="34" spans="1:20" ht="13" customHeight="1">
+      <c r="C34" s="56" t="s">
+        <v>1238</v>
+      </c>
+      <c r="F34" s="60"/>
+      <c r="I34" s="60"/>
+      <c r="J34" s="60"/>
+      <c r="L34" s="59"/>
+      <c r="M34" s="59"/>
+      <c r="N34" s="59"/>
+      <c r="O34" s="59"/>
+      <c r="P34" s="60"/>
+      <c r="Q34" s="60"/>
+      <c r="R34" s="60"/>
+      <c r="S34" s="60"/>
+    </row>
+    <row r="35" spans="1:20" ht="13" customHeight="1">
+      <c r="B35" s="60"/>
+      <c r="F35" s="60"/>
+      <c r="G35" s="60"/>
+      <c r="H35" s="60"/>
+      <c r="I35" s="60"/>
+      <c r="J35" s="60"/>
+      <c r="L35" s="59"/>
+      <c r="M35" s="59"/>
+      <c r="N35" s="59"/>
+      <c r="O35" s="59"/>
+      <c r="P35" s="60"/>
+      <c r="Q35" s="60"/>
+      <c r="R35" s="60"/>
+      <c r="S35" s="60"/>
+      <c r="T35" s="60"/>
+    </row>
+    <row r="36" spans="1:20" ht="13" customHeight="1">
+      <c r="B36" s="60"/>
+      <c r="F36" s="60"/>
+      <c r="G36" s="60"/>
+      <c r="H36" s="60"/>
+      <c r="I36" s="60"/>
+      <c r="L36" s="59"/>
+      <c r="M36" s="59"/>
+      <c r="N36" s="59"/>
+      <c r="O36" s="59"/>
+      <c r="P36" s="60"/>
+      <c r="Q36" s="60"/>
+      <c r="R36" s="60"/>
+      <c r="S36" s="60"/>
+      <c r="T36" s="60"/>
+    </row>
+    <row r="37" spans="1:20" ht="13" customHeight="1">
+      <c r="A37" s="56" t="s">
+        <v>175</v>
+      </c>
+      <c r="B37" s="60" t="s">
+        <v>13</v>
+      </c>
+      <c r="F37" s="60"/>
+      <c r="G37" s="60"/>
+      <c r="H37" s="60"/>
+      <c r="I37" s="60"/>
+      <c r="L37" s="59"/>
+      <c r="M37" s="59"/>
+      <c r="N37" s="59"/>
+      <c r="O37" s="59"/>
+      <c r="P37" s="60"/>
+      <c r="Q37" s="60"/>
+      <c r="R37" s="60"/>
+      <c r="S37" s="60"/>
+      <c r="T37" s="60"/>
+    </row>
+    <row r="38" spans="1:20" ht="13" customHeight="1">
+      <c r="B38" s="60" t="s">
+        <v>1227</v>
+      </c>
+      <c r="F38" s="60"/>
+      <c r="G38" s="60"/>
+      <c r="H38" s="60"/>
+      <c r="I38" s="60"/>
+      <c r="L38" s="59"/>
+      <c r="M38" s="59"/>
+      <c r="N38" s="59"/>
+      <c r="O38" s="59"/>
+      <c r="P38" s="60"/>
+      <c r="Q38" s="60"/>
+      <c r="R38" s="60"/>
+      <c r="S38" s="60"/>
+      <c r="T38" s="60"/>
+    </row>
+    <row r="39" spans="1:20" ht="13" customHeight="1">
+      <c r="B39" s="60" t="s">
+        <v>1228</v>
+      </c>
+      <c r="F39" s="60"/>
+      <c r="G39" s="60"/>
+      <c r="H39" s="60"/>
+      <c r="J39" s="60"/>
+      <c r="L39" s="59"/>
+      <c r="M39" s="59"/>
+      <c r="N39" s="59"/>
+      <c r="O39" s="59"/>
+      <c r="P39" s="60"/>
+      <c r="R39" s="60"/>
+      <c r="S39" s="60"/>
+    </row>
+    <row r="40" spans="1:20" ht="13" customHeight="1">
+      <c r="B40" s="60" t="s">
+        <v>1226</v>
+      </c>
+      <c r="F40" s="60"/>
+      <c r="J40" s="60"/>
+      <c r="L40" s="59"/>
+      <c r="M40" s="59"/>
+      <c r="N40" s="59"/>
+      <c r="O40" s="59"/>
+      <c r="P40" s="60"/>
+      <c r="R40" s="60"/>
+      <c r="S40" s="60"/>
+    </row>
+    <row r="41" spans="1:20" ht="13" customHeight="1">
+      <c r="B41" s="60" t="s">
+        <v>1247</v>
+      </c>
+      <c r="F41" s="60"/>
+      <c r="G41" s="60"/>
+      <c r="H41" s="60"/>
+      <c r="J41" s="60"/>
+      <c r="L41" s="59"/>
+      <c r="M41" s="59"/>
+      <c r="N41" s="59"/>
+      <c r="O41" s="59"/>
+      <c r="P41" s="60"/>
+    </row>
+    <row r="42" spans="1:20" ht="13" customHeight="1">
+      <c r="B42" s="60" t="s">
+        <v>634</v>
+      </c>
+      <c r="F42" s="60"/>
+      <c r="G42" s="60"/>
+      <c r="H42" s="60"/>
+      <c r="J42" s="60"/>
+      <c r="L42" s="59"/>
+      <c r="M42" s="59"/>
+      <c r="N42" s="59"/>
+      <c r="O42" s="59"/>
+      <c r="P42" s="60"/>
+    </row>
+    <row r="43" spans="1:20" ht="13" customHeight="1">
+      <c r="B43" s="56" t="s">
+        <v>1248</v>
+      </c>
+      <c r="F43" s="60"/>
+      <c r="G43" s="60"/>
+      <c r="H43" s="60"/>
+      <c r="J43" s="60"/>
+      <c r="L43" s="59"/>
+      <c r="M43" s="59"/>
+      <c r="N43" s="59"/>
+      <c r="O43" s="59"/>
+    </row>
+    <row r="44" spans="1:20" ht="13" customHeight="1">
+      <c r="B44" s="56" t="s">
+        <v>1249</v>
+      </c>
+      <c r="F44" s="60"/>
+      <c r="G44" s="60"/>
+      <c r="H44" s="60"/>
+      <c r="I44" s="60"/>
+      <c r="J44" s="60"/>
+      <c r="L44" s="59"/>
+      <c r="M44" s="59"/>
+      <c r="N44" s="59"/>
+      <c r="O44" s="59"/>
+      <c r="P44" s="60"/>
+    </row>
+    <row r="45" spans="1:20" ht="13" customHeight="1">
+      <c r="B45" s="56" t="s">
+        <v>1250</v>
+      </c>
+      <c r="G45" s="60"/>
+      <c r="I45" s="60"/>
+      <c r="J45" s="60"/>
+      <c r="L45" s="59"/>
+      <c r="M45" s="59"/>
+      <c r="N45" s="59"/>
+      <c r="O45" s="59"/>
+      <c r="P45" s="60"/>
+      <c r="T45" s="60"/>
+    </row>
+    <row r="46" spans="1:20" ht="13" customHeight="1">
+      <c r="B46" s="56" t="s">
+        <v>1251</v>
+      </c>
+      <c r="F46" s="60"/>
+      <c r="G46" s="60"/>
+      <c r="H46" s="60"/>
+      <c r="L46" s="59"/>
+      <c r="M46" s="59"/>
+      <c r="N46" s="59"/>
+      <c r="O46" s="59"/>
+      <c r="T46" s="60"/>
+    </row>
+    <row r="47" spans="1:20" ht="13" customHeight="1">
+      <c r="B47" s="56" t="s">
+        <v>1254</v>
+      </c>
+      <c r="F47" s="60"/>
+      <c r="G47" s="60"/>
+      <c r="H47" s="60"/>
+      <c r="J47" s="60"/>
+      <c r="L47" s="59"/>
+      <c r="M47" s="59"/>
+      <c r="N47" s="59"/>
+      <c r="O47" s="59"/>
+    </row>
+    <row r="48" spans="1:20" ht="13" customHeight="1">
+      <c r="A48" s="62"/>
+      <c r="B48" s="60" t="s">
+        <v>369</v>
+      </c>
+      <c r="F48" s="60"/>
+      <c r="G48" s="60"/>
+      <c r="H48" s="60"/>
+      <c r="J48" s="60"/>
+      <c r="L48" s="59"/>
+      <c r="M48" s="59"/>
+      <c r="N48" s="59"/>
+      <c r="O48" s="59"/>
+      <c r="P48" s="60"/>
+    </row>
+    <row r="49" spans="1:17" ht="13" customHeight="1">
+      <c r="A49" s="62"/>
+      <c r="B49" s="60" t="s">
+        <v>1255</v>
+      </c>
+      <c r="F49" s="60"/>
+      <c r="G49" s="60"/>
+      <c r="H49" s="60"/>
+      <c r="J49" s="60"/>
+      <c r="L49" s="59"/>
+      <c r="M49" s="59"/>
+      <c r="N49" s="59"/>
+      <c r="O49" s="59"/>
+      <c r="P49" s="60"/>
+    </row>
+    <row r="50" spans="1:17" ht="13" customHeight="1">
+      <c r="A50" s="62"/>
+      <c r="F50" s="60"/>
+      <c r="G50" s="60"/>
+      <c r="H50" s="60"/>
+      <c r="J50" s="60"/>
+      <c r="L50" s="59"/>
+      <c r="M50" s="59"/>
+      <c r="N50" s="59"/>
+      <c r="O50" s="59"/>
+      <c r="P50" s="60"/>
+    </row>
+    <row r="51" spans="1:17" ht="13" customHeight="1">
+      <c r="A51" s="56" t="s">
+        <v>176</v>
+      </c>
+      <c r="B51" s="60"/>
+      <c r="C51" s="56" t="s">
+        <v>14</v>
+      </c>
+      <c r="F51" s="60"/>
+      <c r="G51" s="60"/>
+      <c r="H51" s="60"/>
+      <c r="J51" s="60"/>
+      <c r="L51" s="59"/>
+      <c r="M51" s="59"/>
+      <c r="N51" s="59"/>
+      <c r="O51" s="59"/>
+      <c r="P51" s="60"/>
+    </row>
+    <row r="52" spans="1:17" ht="13" customHeight="1">
+      <c r="B52" s="60"/>
+      <c r="C52" s="56" t="s">
+        <v>1269</v>
+      </c>
+      <c r="F52" s="60"/>
+      <c r="G52" s="60"/>
+      <c r="H52" s="60"/>
+      <c r="J52" s="60"/>
+      <c r="L52" s="59"/>
+      <c r="M52" s="59"/>
+      <c r="N52" s="59"/>
+      <c r="O52" s="59"/>
+      <c r="P52" s="60"/>
+    </row>
+    <row r="53" spans="1:17" ht="13" customHeight="1">
+      <c r="A53" s="62"/>
+      <c r="C53" s="56" t="s">
+        <v>1270</v>
+      </c>
+      <c r="G53" s="60"/>
+      <c r="J53" s="60"/>
+      <c r="L53" s="59"/>
+      <c r="M53" s="59"/>
+      <c r="N53" s="59"/>
+      <c r="O53" s="59"/>
+      <c r="P53" s="60"/>
+    </row>
+    <row r="54" spans="1:17" ht="13" customHeight="1">
+      <c r="B54" s="60"/>
+      <c r="C54" s="56" t="s">
+        <v>15</v>
+      </c>
+      <c r="F54" s="60"/>
+      <c r="G54" s="60"/>
+      <c r="H54" s="60"/>
+      <c r="J54" s="60"/>
+      <c r="L54" s="59"/>
+      <c r="M54" s="59"/>
+      <c r="N54" s="59"/>
+      <c r="O54" s="59"/>
+      <c r="P54" s="60"/>
+    </row>
+    <row r="55" spans="1:17" ht="13" customHeight="1">
+      <c r="B55" s="60"/>
+      <c r="F55" s="60"/>
+      <c r="G55" s="60"/>
+      <c r="H55" s="60"/>
+      <c r="J55" s="60"/>
+      <c r="L55" s="59"/>
+      <c r="M55" s="59"/>
+      <c r="N55" s="59"/>
+      <c r="O55" s="59"/>
+      <c r="P55" s="60"/>
+    </row>
+    <row r="56" spans="1:17" ht="13" customHeight="1">
+      <c r="A56" s="56" t="s">
+        <v>178</v>
+      </c>
+      <c r="B56" s="60" t="s">
+        <v>398</v>
+      </c>
+      <c r="C56" s="36" t="s">
+        <v>398</v>
+      </c>
+      <c r="F56" s="60"/>
+      <c r="G56" s="60"/>
+      <c r="H56" s="60"/>
+      <c r="J56" s="60"/>
+      <c r="L56" s="59"/>
+      <c r="M56" s="59"/>
+      <c r="N56" s="59"/>
+      <c r="O56" s="59"/>
+      <c r="P56" s="60"/>
+    </row>
+    <row r="57" spans="1:17" ht="13" customHeight="1">
+      <c r="B57" s="36" t="s">
+        <v>366</v>
+      </c>
+      <c r="C57" s="36" t="s">
+        <v>315</v>
+      </c>
+      <c r="F57" s="36" t="s">
+        <v>366</v>
+      </c>
+      <c r="G57" s="60"/>
+      <c r="H57" s="60"/>
+      <c r="J57" s="60"/>
+      <c r="L57" s="59"/>
+      <c r="M57" s="59"/>
+      <c r="N57" s="59"/>
+      <c r="O57" s="59"/>
+      <c r="P57" s="60"/>
+    </row>
+    <row r="58" spans="1:17" ht="13" customHeight="1">
+      <c r="B58" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="C58" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="F58" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="G58" s="60"/>
+      <c r="H58" s="60"/>
+      <c r="J58" s="60"/>
+      <c r="L58" s="59"/>
+      <c r="M58" s="59"/>
+      <c r="N58" s="59"/>
+      <c r="O58" s="59"/>
+      <c r="P58" s="60"/>
+    </row>
+    <row r="59" spans="1:17" ht="13" customHeight="1">
+      <c r="A59" s="62"/>
+      <c r="B59" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="C59" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="F59" s="36" t="s">
+        <v>448</v>
+      </c>
+      <c r="G59" s="60"/>
+      <c r="H59" s="60"/>
+      <c r="J59" s="60"/>
+      <c r="L59" s="59"/>
+      <c r="M59" s="59"/>
+      <c r="N59" s="59"/>
+      <c r="O59" s="59"/>
+      <c r="P59" s="60"/>
+    </row>
+    <row r="60" spans="1:17" ht="13" customHeight="1">
+      <c r="A60" s="62"/>
+      <c r="B60" s="36" t="s">
+        <v>369</v>
+      </c>
+      <c r="C60" s="36" t="s">
+        <v>93</v>
+      </c>
+      <c r="F60" s="36" t="s">
+        <v>369</v>
+      </c>
+      <c r="G60" s="60"/>
+      <c r="H60" s="60"/>
+      <c r="J60" s="60"/>
+      <c r="L60" s="59"/>
+      <c r="M60" s="59"/>
+      <c r="N60" s="59"/>
+      <c r="O60" s="59"/>
+      <c r="P60" s="60"/>
+    </row>
+    <row r="61" spans="1:17" ht="13" customHeight="1">
+      <c r="A61" s="62"/>
+      <c r="B61" s="36" t="s">
+        <v>370</v>
+      </c>
+      <c r="C61" s="36" t="s">
+        <v>94</v>
+      </c>
+      <c r="F61" s="36" t="s">
+        <v>449</v>
+      </c>
+      <c r="G61" s="60"/>
+      <c r="H61" s="60"/>
+      <c r="J61" s="60"/>
+      <c r="L61" s="59"/>
+      <c r="M61" s="59"/>
+      <c r="N61" s="59"/>
+      <c r="O61" s="59"/>
+      <c r="P61" s="60"/>
+    </row>
+    <row r="62" spans="1:17" ht="13" customHeight="1">
+      <c r="A62" s="62"/>
+      <c r="B62" s="36" t="s">
+        <v>925</v>
+      </c>
+      <c r="C62" s="36" t="s">
+        <v>925</v>
+      </c>
+      <c r="F62" s="36" t="s">
+        <v>925</v>
+      </c>
+      <c r="G62" s="60"/>
+      <c r="H62" s="60"/>
+      <c r="J62" s="60"/>
+      <c r="L62" s="59"/>
+      <c r="M62" s="59"/>
+      <c r="N62" s="59"/>
+      <c r="O62" s="59"/>
+      <c r="P62" s="60"/>
+    </row>
+    <row r="63" spans="1:17" ht="13" customHeight="1">
+      <c r="A63" s="62"/>
+      <c r="C63" s="56" t="s">
+        <v>1265</v>
+      </c>
+      <c r="J63" s="60"/>
+      <c r="L63" s="60"/>
+      <c r="M63" s="60"/>
+      <c r="N63" s="60"/>
+      <c r="O63" s="60"/>
+      <c r="P63" s="60"/>
+    </row>
+    <row r="64" spans="1:17" ht="13" customHeight="1">
+      <c r="A64" s="62"/>
+      <c r="C64" s="56" t="s">
+        <v>1271</v>
+      </c>
+      <c r="F64" s="60"/>
+      <c r="G64" s="60"/>
+      <c r="H64" s="60"/>
+      <c r="Q64" s="60"/>
+    </row>
+    <row r="65" spans="1:17" ht="13" customHeight="1">
+      <c r="A65" s="62"/>
+      <c r="C65" s="56" t="s">
+        <v>1272</v>
+      </c>
+      <c r="F65" s="60"/>
+      <c r="G65" s="60"/>
+      <c r="H65" s="60"/>
+      <c r="Q65" s="60"/>
+    </row>
+    <row r="66" spans="1:17" ht="13" customHeight="1">
+      <c r="A66" s="62"/>
+      <c r="C66" s="56" t="s">
+        <v>1228</v>
+      </c>
+      <c r="F66" s="60"/>
+      <c r="G66" s="60"/>
+      <c r="H66" s="60"/>
+      <c r="Q66" s="60"/>
+    </row>
+    <row r="67" spans="1:17" ht="13" customHeight="1">
+      <c r="A67" s="62"/>
+      <c r="C67" s="56" t="s">
+        <v>1273</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" ht="13" customHeight="1">
+      <c r="A68" s="62"/>
+      <c r="C68" s="56" t="s">
+        <v>925</v>
+      </c>
+      <c r="Q68" s="60"/>
+    </row>
+    <row r="69" spans="1:17" ht="13" customHeight="1">
+      <c r="A69" s="62"/>
+    </row>
+    <row r="70" spans="1:17" ht="13" customHeight="1">
+      <c r="A70" s="62" t="s">
+        <v>179</v>
+      </c>
+      <c r="B70" s="56" t="s">
+        <v>25</v>
+      </c>
+      <c r="C70" s="56" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" ht="13" customHeight="1">
+      <c r="A71" s="62"/>
+      <c r="B71" s="56" t="s">
+        <v>1256</v>
+      </c>
+      <c r="C71" s="56" t="s">
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" ht="13" customHeight="1">
+      <c r="A72" s="62"/>
+      <c r="B72" s="56" t="s">
+        <v>1252</v>
+      </c>
+      <c r="C72" s="56" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" ht="13" customHeight="1">
+      <c r="A73" s="62"/>
+      <c r="B73" s="56" t="s">
+        <v>1253</v>
+      </c>
+      <c r="C73" s="56" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" ht="13" customHeight="1">
+      <c r="A74" s="62"/>
+      <c r="B74" s="56" t="s">
+        <v>1260</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" ht="13" customHeight="1">
+      <c r="A75" s="62"/>
+      <c r="B75" s="56" t="s">
+        <v>1259</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" ht="13" customHeight="1">
+      <c r="A76" s="62"/>
+      <c r="B76" s="56" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" ht="13" customHeight="1">
+      <c r="A77" s="62"/>
+    </row>
+    <row r="78" spans="1:17" ht="13" customHeight="1">
+      <c r="A78" s="62" t="s">
+        <v>180</v>
+      </c>
+      <c r="B78" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="C78" s="56" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" ht="13" customHeight="1">
+      <c r="A79" s="62"/>
+      <c r="B79" s="56" t="s">
+        <v>1225</v>
+      </c>
+      <c r="C79" s="56" t="s">
+        <v>1266</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" ht="13" customHeight="1">
+      <c r="A80" s="62"/>
+      <c r="B80" s="56" t="s">
+        <v>1223</v>
+      </c>
+      <c r="C80" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="I80" s="60"/>
+    </row>
+    <row r="81" spans="1:19" ht="13" customHeight="1">
+      <c r="A81" s="62"/>
+      <c r="B81" s="56" t="s">
+        <v>20</v>
+      </c>
+      <c r="C81" s="56" t="s">
+        <v>20</v>
+      </c>
+      <c r="I81" s="60"/>
+    </row>
+    <row r="82" spans="1:19" ht="13" customHeight="1">
+      <c r="A82" s="62"/>
+      <c r="I82" s="60"/>
+    </row>
+    <row r="83" spans="1:19" ht="13" customHeight="1">
+      <c r="A83" s="62" t="s">
+        <v>427</v>
+      </c>
+      <c r="C83" s="36"/>
+      <c r="D83" s="36" t="s">
+        <v>436</v>
+      </c>
+      <c r="E83" s="56" t="str">
+        <f>D83</f>
+        <v>Operate:</v>
+      </c>
+      <c r="I83" s="60"/>
+    </row>
+    <row r="84" spans="1:19" ht="13" customHeight="1">
+      <c r="C84" s="36"/>
+      <c r="D84" s="36" t="s">
+        <v>522</v>
+      </c>
+      <c r="E84" s="56" t="str">
+        <f t="shared" ref="E84:E89" si="1">D84</f>
+        <v xml:space="preserve">  operation: sum</v>
+      </c>
+      <c r="I84" s="60"/>
+    </row>
+    <row r="85" spans="1:19" ht="13" customHeight="1">
+      <c r="C85" s="36"/>
+      <c r="D85" s="36" t="s">
+        <v>523</v>
+      </c>
+      <c r="E85" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  axis:   row</v>
+      </c>
+      <c r="I85" s="60"/>
+    </row>
+    <row r="86" spans="1:19" ht="13" customHeight="1">
+      <c r="C86" s="36"/>
+      <c r="D86" s="36" t="s">
+        <v>525</v>
+      </c>
+      <c r="E86" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  from:   nothing</v>
+      </c>
+      <c r="I86" s="60"/>
+    </row>
+    <row r="87" spans="1:19" s="63" customFormat="1" ht="13" customHeight="1">
+      <c r="A87" s="56"/>
+      <c r="B87" s="56"/>
+      <c r="C87" s="36"/>
+      <c r="D87" s="36" t="s">
+        <v>524</v>
+      </c>
+      <c r="E87" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  to:     nothing</v>
+      </c>
+    </row>
+    <row r="88" spans="1:19" ht="13" customHeight="1">
+      <c r="C88" s="36"/>
+      <c r="D88" s="36" t="s">
+        <v>1245</v>
+      </c>
+      <c r="E88" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  input:  [yr, r, sector]</v>
+      </c>
+      <c r="I88" s="60"/>
+    </row>
+    <row r="89" spans="1:19" ht="13" customHeight="1">
+      <c r="C89" s="36"/>
+      <c r="D89" s="36" t="s">
+        <v>440</v>
+      </c>
+      <c r="E89" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  output: value</v>
+      </c>
+      <c r="I89" s="60"/>
+    </row>
+    <row r="91" spans="1:19" ht="13" customHeight="1">
+      <c r="L91" s="59"/>
+      <c r="R91" s="60"/>
+      <c r="S91" s="60"/>
+    </row>
+    <row r="92" spans="1:19" ht="13" customHeight="1">
+      <c r="L92" s="59"/>
+      <c r="R92" s="60"/>
+      <c r="S92" s="60"/>
+    </row>
+    <row r="93" spans="1:19" ht="13" customHeight="1">
+      <c r="L93" s="59"/>
+      <c r="R93" s="60"/>
+      <c r="S93" s="60"/>
+    </row>
+    <row r="94" spans="1:19" ht="13" customHeight="1">
+      <c r="L94" s="59"/>
+      <c r="R94" s="60"/>
+      <c r="S94" s="60"/>
+    </row>
+    <row r="96" spans="1:19" ht="13" customHeight="1">
+      <c r="R96" s="60"/>
+    </row>
+    <row r="97" spans="6:19" ht="13" customHeight="1">
+      <c r="R97" s="60"/>
+    </row>
+    <row r="98" spans="6:19" ht="13" customHeight="1">
+      <c r="R98" s="60"/>
+    </row>
+    <row r="99" spans="6:19" ht="13" customHeight="1">
+      <c r="R99" s="60"/>
+    </row>
+    <row r="100" spans="6:19" ht="13" customHeight="1">
+      <c r="R100" s="60"/>
+    </row>
+    <row r="102" spans="6:19" ht="13" customHeight="1">
+      <c r="F102" s="60"/>
+      <c r="G102" s="60"/>
+      <c r="L102" s="59"/>
+      <c r="M102" s="59"/>
+      <c r="N102" s="59"/>
+      <c r="S102" s="60"/>
+    </row>
+    <row r="103" spans="6:19" ht="13" customHeight="1">
+      <c r="G103" s="60"/>
+      <c r="I103" s="61"/>
+      <c r="L103" s="59"/>
+      <c r="M103" s="59"/>
+      <c r="N103" s="59"/>
+      <c r="P103" s="61"/>
+      <c r="S103" s="60"/>
+    </row>
+    <row r="104" spans="6:19" ht="13" customHeight="1">
+      <c r="G104" s="60"/>
+      <c r="I104" s="61"/>
+      <c r="L104" s="59"/>
+      <c r="M104" s="59"/>
+      <c r="N104" s="59"/>
+      <c r="P104" s="61"/>
+      <c r="S104" s="60"/>
+    </row>
+    <row r="105" spans="6:19" ht="13" customHeight="1">
+      <c r="G105" s="60"/>
+      <c r="I105" s="61"/>
+      <c r="L105" s="59"/>
+      <c r="M105" s="59"/>
+      <c r="N105" s="59"/>
+      <c r="P105" s="61"/>
+      <c r="S105" s="60"/>
+    </row>
+    <row r="106" spans="6:19" ht="13" customHeight="1">
+      <c r="G106" s="60"/>
+      <c r="I106" s="61"/>
+      <c r="L106" s="59"/>
+      <c r="M106" s="59"/>
+      <c r="N106" s="59"/>
+      <c r="P106" s="61"/>
+      <c r="S106" s="60"/>
+    </row>
+    <row r="107" spans="6:19" ht="13" customHeight="1">
+      <c r="G107" s="60"/>
+      <c r="I107" s="61"/>
+      <c r="L107" s="59"/>
+      <c r="M107" s="59"/>
+      <c r="N107" s="59"/>
+      <c r="P107" s="61"/>
+      <c r="S107" s="60"/>
+    </row>
+    <row r="108" spans="6:19" ht="13" customHeight="1">
+      <c r="G108" s="60"/>
+      <c r="I108" s="61"/>
+      <c r="L108" s="59"/>
+      <c r="M108" s="59"/>
+      <c r="N108" s="59"/>
+    </row>
+    <row r="109" spans="6:19" ht="13" customHeight="1">
+      <c r="G109" s="60"/>
+      <c r="I109" s="61"/>
+      <c r="L109" s="59"/>
+      <c r="M109" s="59"/>
+      <c r="N109" s="59"/>
+    </row>
+    <row r="110" spans="6:19" ht="13" customHeight="1">
+      <c r="G110" s="60"/>
+      <c r="I110" s="61"/>
+      <c r="L110" s="59"/>
+      <c r="M110" s="59"/>
+      <c r="N110" s="59"/>
+    </row>
+    <row r="111" spans="6:19" ht="13" customHeight="1">
+      <c r="G111" s="60"/>
+      <c r="I111" s="61"/>
+      <c r="L111" s="59"/>
+      <c r="M111" s="59"/>
+      <c r="N111" s="59"/>
+    </row>
+    <row r="112" spans="6:19" ht="13" customHeight="1">
+      <c r="G112" s="60"/>
+      <c r="I112" s="61"/>
+      <c r="L112" s="59"/>
+      <c r="M112" s="59"/>
+      <c r="N112" s="59"/>
+    </row>
+    <row r="113" spans="5:14" ht="13" customHeight="1">
+      <c r="G113" s="60"/>
+      <c r="I113" s="61"/>
+      <c r="L113" s="59"/>
+      <c r="M113" s="59"/>
+      <c r="N113" s="59"/>
+    </row>
+    <row r="114" spans="5:14" ht="13" customHeight="1">
+      <c r="G114" s="60"/>
+      <c r="K114" s="56"/>
+      <c r="L114" s="59"/>
+      <c r="M114" s="59"/>
+      <c r="N114" s="59"/>
+    </row>
+    <row r="115" spans="5:14" ht="13" customHeight="1">
+      <c r="G115" s="60"/>
+      <c r="L115" s="59"/>
+      <c r="M115" s="59"/>
+      <c r="N115" s="59"/>
+    </row>
+    <row r="116" spans="5:14" ht="13" customHeight="1">
+      <c r="G116" s="60"/>
+    </row>
+    <row r="117" spans="5:14" ht="13" customHeight="1">
+      <c r="G117" s="60"/>
+    </row>
+    <row r="118" spans="5:14" ht="13" customHeight="1">
+      <c r="G118" s="60"/>
+    </row>
+    <row r="119" spans="5:14" ht="13" customHeight="1">
+      <c r="G119" s="60"/>
+    </row>
+    <row r="120" spans="5:14" ht="13" customHeight="1">
+      <c r="G120" s="60"/>
+    </row>
+    <row r="121" spans="5:14" ht="13" customHeight="1">
+      <c r="G121" s="60"/>
+      <c r="L121" s="59"/>
+      <c r="M121" s="59"/>
+      <c r="N121" s="59"/>
+    </row>
+    <row r="122" spans="5:14" ht="13" customHeight="1">
+      <c r="G122" s="60"/>
+      <c r="L122" s="59"/>
+      <c r="M122" s="59"/>
+      <c r="N122" s="59"/>
+    </row>
+    <row r="123" spans="5:14" ht="13" customHeight="1">
+      <c r="G123" s="60"/>
+      <c r="L123" s="59"/>
+      <c r="M123" s="59"/>
+      <c r="N123" s="59"/>
+    </row>
+    <row r="124" spans="5:14" ht="13" customHeight="1">
+      <c r="G124" s="60"/>
+      <c r="L124" s="59"/>
+      <c r="M124" s="59"/>
+      <c r="N124" s="59"/>
+    </row>
+    <row r="125" spans="5:14" ht="13" customHeight="1">
+      <c r="G125" s="60"/>
+      <c r="L125" s="59"/>
+      <c r="M125" s="59"/>
+      <c r="N125" s="59"/>
+    </row>
+    <row r="126" spans="5:14" ht="13" customHeight="1">
+      <c r="G126" s="60"/>
+      <c r="L126" s="59"/>
+      <c r="M126" s="59"/>
+      <c r="N126" s="59"/>
+    </row>
+    <row r="128" spans="5:14" ht="13" customHeight="1">
+      <c r="E128" s="60"/>
+      <c r="I128" s="60"/>
+    </row>
+    <row r="129" spans="3:14" ht="13" customHeight="1">
+      <c r="E129" s="60"/>
+      <c r="I129" s="60"/>
+    </row>
+    <row r="130" spans="3:14" ht="13" customHeight="1">
+      <c r="E130" s="60"/>
+      <c r="I130" s="60"/>
+    </row>
+    <row r="131" spans="3:14" ht="13" customHeight="1">
+      <c r="E131" s="60"/>
+      <c r="I131" s="60"/>
+    </row>
+    <row r="132" spans="3:14" ht="13" customHeight="1">
+      <c r="C132" s="60"/>
+      <c r="E132" s="60"/>
+      <c r="I132" s="60"/>
+    </row>
+    <row r="133" spans="3:14" ht="13" customHeight="1">
+      <c r="C133" s="60"/>
+      <c r="E133" s="60"/>
+      <c r="I133" s="60"/>
+    </row>
+    <row r="134" spans="3:14" ht="13" customHeight="1">
+      <c r="C134" s="60"/>
+      <c r="E134" s="60"/>
+      <c r="I134" s="60"/>
+    </row>
+    <row r="135" spans="3:14" ht="13" customHeight="1">
+      <c r="C135" s="60"/>
+      <c r="D135" s="60"/>
+      <c r="E135" s="60"/>
+      <c r="I135" s="60"/>
+    </row>
+    <row r="136" spans="3:14" ht="13" customHeight="1">
+      <c r="C136" s="60"/>
+      <c r="D136" s="60"/>
+      <c r="E136" s="60"/>
+      <c r="I136" s="60"/>
+    </row>
+    <row r="137" spans="3:14" ht="13" customHeight="1">
+      <c r="C137" s="60"/>
+      <c r="D137" s="60"/>
+      <c r="E137" s="60"/>
+      <c r="I137" s="60"/>
+    </row>
+    <row r="139" spans="3:14" ht="13" customHeight="1">
+      <c r="J139" s="60"/>
+      <c r="L139" s="60"/>
+    </row>
+    <row r="140" spans="3:14" ht="13" customHeight="1">
+      <c r="J140" s="60"/>
+      <c r="L140" s="60"/>
+    </row>
+    <row r="141" spans="3:14" ht="13" customHeight="1">
+      <c r="J141" s="60"/>
+      <c r="L141" s="60"/>
+    </row>
+    <row r="142" spans="3:14" ht="13" customHeight="1">
+      <c r="J142" s="60"/>
+      <c r="L142" s="60"/>
+      <c r="M142" s="60"/>
+      <c r="N142" s="60"/>
+    </row>
+    <row r="143" spans="3:14" ht="13" customHeight="1">
+      <c r="I143" s="61"/>
+      <c r="L143" s="59"/>
+      <c r="M143" s="59"/>
+      <c r="N143" s="59"/>
+    </row>
+    <row r="144" spans="3:14" ht="13" customHeight="1">
+      <c r="I144" s="61"/>
+      <c r="L144" s="59"/>
+      <c r="M144" s="59"/>
+      <c r="N144" s="59"/>
+    </row>
+    <row r="145" spans="1:15" ht="13" customHeight="1">
+      <c r="L145" s="59"/>
+      <c r="M145" s="59"/>
+      <c r="N145" s="59"/>
+    </row>
+    <row r="146" spans="1:15" ht="13" customHeight="1">
+      <c r="J146" s="60"/>
+      <c r="L146" s="59"/>
+      <c r="M146" s="59"/>
+      <c r="N146" s="59"/>
+      <c r="O146" s="60"/>
+    </row>
+    <row r="147" spans="1:15" ht="13" customHeight="1">
+      <c r="J147" s="60"/>
+      <c r="L147" s="59"/>
+      <c r="M147" s="59"/>
+      <c r="N147" s="59"/>
+      <c r="O147" s="60"/>
+    </row>
+    <row r="148" spans="1:15" ht="13" customHeight="1">
+      <c r="J148" s="60"/>
+      <c r="L148" s="59"/>
+      <c r="M148" s="59"/>
+      <c r="N148" s="59"/>
+      <c r="O148" s="60"/>
+    </row>
+    <row r="150" spans="1:15" ht="13" customHeight="1">
+      <c r="L150" s="59"/>
+      <c r="M150" s="59"/>
+      <c r="N150" s="59"/>
+    </row>
+    <row r="151" spans="1:15" ht="13" customHeight="1">
+      <c r="L151" s="59"/>
+      <c r="M151" s="59"/>
+      <c r="N151" s="59"/>
+    </row>
+    <row r="152" spans="1:15" ht="13" customHeight="1">
+      <c r="L152" s="59"/>
+      <c r="M152" s="59"/>
+      <c r="N152" s="59"/>
+    </row>
+    <row r="153" spans="1:15" ht="13" customHeight="1">
+      <c r="A153" s="62"/>
+      <c r="L153" s="59"/>
+      <c r="M153" s="59"/>
+      <c r="N153" s="59"/>
+    </row>
+    <row r="154" spans="1:15" ht="13" customHeight="1">
+      <c r="A154" s="62"/>
+      <c r="L154" s="59"/>
+      <c r="M154" s="59"/>
+      <c r="N154" s="59"/>
+    </row>
+    <row r="155" spans="1:15" ht="13" customHeight="1">
+      <c r="A155" s="62"/>
+      <c r="L155" s="59"/>
+      <c r="M155" s="59"/>
+      <c r="N155" s="59"/>
+    </row>
+    <row r="156" spans="1:15" ht="13" customHeight="1">
+      <c r="A156" s="62"/>
+      <c r="L156" s="59"/>
+      <c r="M156" s="59"/>
+      <c r="N156" s="59"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D51:XFD54 E74:XFD77 D56:XFD56 A55:XFD55 A63:XFD73 A40:B56 A57:A62 D57:E62 G57:XFD62 F78:XFD83 E80:E83 A69:E79 A78:D83 A63:B89 A84:XFD1048576 A1:XFD50">
+    <cfRule type="expression" dxfId="1" priority="29">
+      <formula>_xlfn.ISFORMULA(A1)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56:C62">
+    <cfRule type="expression" dxfId="29" priority="10">
+      <formula>_xlfn.ISFORMULA(C56)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B63:B81">
+    <cfRule type="expression" dxfId="28" priority="18">
+      <formula>_xlfn.ISFORMULA(B63)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51:C54">
+    <cfRule type="expression" dxfId="27" priority="16">
+      <formula>_xlfn.ISFORMULA(C51)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C74:C89">
+    <cfRule type="expression" dxfId="26" priority="14">
+      <formula>_xlfn.ISFORMULA(C74)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D74:D89">
+    <cfRule type="expression" dxfId="25" priority="12">
+      <formula>_xlfn.ISFORMULA(D74)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D54:XFD54 A54:B54">
+    <cfRule type="expression" dxfId="24" priority="428">
+      <formula>AND(COUNTA($A54:$V54)=0, NOT(ISBLANK(#REF!)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B54:C54">
+    <cfRule type="expression" dxfId="23" priority="441">
+      <formula>AND(COUNTA($A54:$Z54)=0, NOT(ISBLANK(#REF!)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C55:XFD55 E74:XFD77 C63:XFD73 D56:XFD56 D51:XFD53 A40:B53 A55:B56 A57:A62 D57:E62 G57:XFD62 F78:XFD83 E80:E83 C69:E79 C78:D83 A63:B1048574 C84:XFD1048574 A2:XFD50">
+    <cfRule type="expression" dxfId="0" priority="454">
+      <formula>AND(COUNTA($A2:$V2)=0, NOT(ISBLANK($A3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B52:B53 C51:C53 C56:C62 B49 B55:B56 C74:D89 B63:B81">
+    <cfRule type="expression" dxfId="16" priority="504">
+      <formula>AND(COUNTA($A49:$Z49)=0, NOT(ISBLANK($A50)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1048576:XFD1048576">
+    <cfRule type="expression" dxfId="15" priority="512">
+      <formula>AND(COUNTA($A:$V)=0, NOT(ISBLANK($A2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1048575:XFD1048575">
+    <cfRule type="expression" dxfId="14" priority="515">
+      <formula>AND(COUNTA($A1048575:$V1048576)=0, NOT(ISBLANK($A1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B57:B62">
+    <cfRule type="expression" dxfId="13" priority="7">
+      <formula>_xlfn.ISFORMULA(B57)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B57:B62">
+    <cfRule type="expression" dxfId="12" priority="8">
+      <formula>AND(COUNTA($A57:$AA57)=0, NOT(ISBLANK($A58)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F57:F62">
+    <cfRule type="expression" dxfId="7" priority="5">
+      <formula>_xlfn.ISFORMULA(F57)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F57:F62">
+    <cfRule type="expression" dxfId="6" priority="6">
+      <formula>AND(COUNTA($A57:$AA57)=0, NOT(ISBLANK($A58)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E78:E83">
+    <cfRule type="expression" dxfId="5" priority="3">
+      <formula>_xlfn.ISFORMULA(E78)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E78:E83">
+    <cfRule type="expression" dxfId="4" priority="4">
+      <formula>AND(COUNTA($A78:$V78)=0, NOT(ISBLANK($A79)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E84:E89">
+    <cfRule type="expression" dxfId="3" priority="1">
+      <formula>_xlfn.ISFORMULA(E84)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E84:E89">
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>AND(COUNTA($A84:$V84)=0, NOT(ISBLANK($A85)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BE5A693-F7F5-4E49-9BB0-AEC7C8F410F3}">
   <dimension ref="A1:X145"/>
   <sheetViews>
@@ -22784,32 +24771,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="22" priority="6">
       <formula>_xlfn.ISFORMULA(A1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G63:G67">
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="21" priority="5">
       <formula>_xlfn.ISFORMULA(G63)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G30:G31">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="20" priority="4">
       <formula>_xlfn.ISFORMULA(G30)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G26:G27">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="19" priority="2">
       <formula>_xlfn.ISFORMULA(G26)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G33:G58">
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="18" priority="3">
       <formula>_xlfn.ISFORMULA(G33)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M32">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="17" priority="1">
       <formula>_xlfn.ISFORMULA(M32)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
sharing script -> functions
</commit_message>
<xml_diff>
--- a/data/readfiles/generate_yaml.xlsx
+++ b/data/readfiles/generate_yaml.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chughes/Documents/Git/SLiDE/data/readfiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4794DD3C-2962-094C-97F6-E3958FF283D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F4C0413-2062-ED49-9B05-4211DBDD12EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="7" xr2:uid="{ECEEE8D6-CC61-454D-945D-45D0FFF64D45}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="6" xr2:uid="{ECEEE8D6-CC61-454D-945D-45D0FFF64D45}"/>
   </bookViews>
   <sheets>
     <sheet name="map_bluenote" sheetId="5" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3281" uniqueCount="1275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3283" uniqueCount="1278">
   <si>
     <t>bea_supply</t>
   </si>
@@ -3496,9 +3496,6 @@
     <t xml:space="preserve">    output: s</t>
   </si>
   <si>
-    <t xml:space="preserve">    kind:   inner</t>
-  </si>
-  <si>
     <t xml:space="preserve">    input:  sg</t>
   </si>
   <si>
@@ -3508,12 +3505,6 @@
     <t xml:space="preserve">  input:  [orig_state, dest_state, g, units]</t>
   </si>
   <si>
-    <t xml:space="preserve">  col: g</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  val: missing</t>
-  </si>
-  <si>
     <t xml:space="preserve">  - file:   [crosswalk, pce.csv]</t>
   </si>
   <si>
@@ -3866,6 +3857,24 @@
   </si>
   <si>
     <t xml:space="preserve">  - {col: source,      type: String}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  col: sg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  val: [0, 99]</t>
+  </si>
+  <si>
+    <t># - {col: units,      type: String}</t>
+  </si>
+  <si>
+    <t># - {col: sg,         type: Any}</t>
+  </si>
+  <si>
+    <t># - {col: n,          type: String}</t>
+  </si>
+  <si>
+    <t># - {col: units,  type: String}</t>
   </si>
 </sst>
 </file>
@@ -4177,9 +4186,52 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4283,62 +4335,9 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color theme="9"/>
-      </font>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4353,6 +4352,16 @@
       <fill>
         <patternFill>
           <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5814,7 +5823,7 @@
         <v>206</v>
       </c>
       <c r="E1" s="53" t="s">
-        <v>1209</v>
+        <v>1206</v>
       </c>
       <c r="F1" s="53" t="s">
         <v>221</v>
@@ -5976,7 +5985,7 @@
         <v>736</v>
       </c>
       <c r="E8" s="33" t="s">
-        <v>1206</v>
+        <v>1203</v>
       </c>
       <c r="F8" s="33" t="s">
         <v>737</v>
@@ -6067,7 +6076,7 @@
         <v>338</v>
       </c>
       <c r="E11" s="33" t="s">
-        <v>1207</v>
+        <v>1204</v>
       </c>
       <c r="F11" s="33" t="s">
         <v>353</v>
@@ -6105,7 +6114,7 @@
         <v>215</v>
       </c>
       <c r="E12" s="33" t="s">
-        <v>1208</v>
+        <v>1205</v>
       </c>
       <c r="F12" s="33" t="s">
         <v>354</v>
@@ -6223,7 +6232,7 @@
         <v>335</v>
       </c>
       <c r="E19" s="33" t="s">
-        <v>1210</v>
+        <v>1207</v>
       </c>
       <c r="G19" s="33" t="s">
         <v>407</v>
@@ -6255,7 +6264,7 @@
         <v>336</v>
       </c>
       <c r="E20" s="33" t="s">
-        <v>1211</v>
+        <v>1208</v>
       </c>
       <c r="G20" s="33" t="s">
         <v>406</v>
@@ -8256,7 +8265,7 @@
         <v>356</v>
       </c>
       <c r="I1" s="40" t="s">
-        <v>1209</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="40" customFormat="1" ht="13" customHeight="1">
@@ -8356,7 +8365,7 @@
         <v>821</v>
       </c>
       <c r="I7" s="43" t="s">
-        <v>1214</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="13" customHeight="1">
@@ -8385,7 +8394,7 @@
         <v>1067</v>
       </c>
       <c r="I8" s="44" t="s">
-        <v>1215</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="13" customHeight="1">
@@ -8445,7 +8454,7 @@
         <v>464</v>
       </c>
       <c r="I11" s="43" t="s">
-        <v>1212</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="13" customHeight="1">
@@ -8472,7 +8481,7 @@
         <v>1065</v>
       </c>
       <c r="I12" s="43" t="s">
-        <v>1213</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="13" customHeight="1">
@@ -10568,7 +10577,7 @@
         <v>820</v>
       </c>
       <c r="L10" s="36" t="s">
-        <v>1182</v>
+        <v>1179</v>
       </c>
       <c r="M10" s="36" t="str">
         <f>IF(ISBLANK($L10), "", $L10)</f>
@@ -10597,7 +10606,7 @@
         <v>PathIn:  [data, datasources, SGF]</v>
       </c>
       <c r="T10" s="36" t="s">
-        <v>1182</v>
+        <v>1179</v>
       </c>
       <c r="U10" s="36" t="s">
         <v>840</v>
@@ -10620,76 +10629,76 @@
         <v>169</v>
       </c>
       <c r="B11" s="36" t="s">
+        <v>1180</v>
+      </c>
+      <c r="C11" s="36" t="s">
+        <v>1181</v>
+      </c>
+      <c r="D11" s="36" t="s">
+        <v>1182</v>
+      </c>
+      <c r="E11" s="36" t="s">
         <v>1183</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="F11" s="36" t="s">
         <v>1184</v>
       </c>
-      <c r="D11" s="36" t="s">
+      <c r="G11" s="36" t="s">
         <v>1185</v>
       </c>
-      <c r="E11" s="36" t="s">
+      <c r="H11" s="36" t="s">
         <v>1186</v>
       </c>
-      <c r="F11" s="36" t="s">
+      <c r="I11" s="36" t="s">
+        <v>1186</v>
+      </c>
+      <c r="J11" s="36" t="s">
         <v>1187</v>
       </c>
-      <c r="G11" s="36" t="s">
+      <c r="K11" s="36" t="s">
         <v>1188</v>
       </c>
-      <c r="H11" s="36" t="s">
+      <c r="L11" s="36" t="s">
         <v>1189</v>
       </c>
-      <c r="I11" s="36" t="s">
-        <v>1189</v>
-      </c>
-      <c r="J11" s="36" t="s">
+      <c r="M11" s="36" t="s">
         <v>1190</v>
       </c>
-      <c r="K11" s="36" t="s">
+      <c r="N11" s="36" t="s">
         <v>1191</v>
       </c>
-      <c r="L11" s="36" t="s">
+      <c r="O11" s="36" t="s">
         <v>1192</v>
       </c>
-      <c r="M11" s="36" t="s">
+      <c r="P11" s="32" t="s">
         <v>1193</v>
       </c>
-      <c r="N11" s="36" t="s">
+      <c r="Q11" s="36" t="s">
         <v>1194</v>
       </c>
-      <c r="O11" s="36" t="s">
+      <c r="R11" s="36" t="s">
         <v>1195</v>
       </c>
-      <c r="P11" s="32" t="s">
+      <c r="S11" s="36" t="s">
         <v>1196</v>
       </c>
-      <c r="Q11" s="36" t="s">
+      <c r="T11" s="36" t="s">
         <v>1197</v>
       </c>
-      <c r="R11" s="36" t="s">
+      <c r="U11" s="36" t="s">
         <v>1198</v>
       </c>
-      <c r="S11" s="36" t="s">
+      <c r="V11" s="36" t="s">
         <v>1199</v>
       </c>
-      <c r="T11" s="36" t="s">
+      <c r="W11" s="36" t="s">
         <v>1200</v>
       </c>
-      <c r="U11" s="36" t="s">
+      <c r="X11" s="36" t="s">
         <v>1201</v>
       </c>
-      <c r="V11" s="36" t="s">
+      <c r="Y11" s="36" t="s">
         <v>1202</v>
-      </c>
-      <c r="W11" s="36" t="s">
-        <v>1203</v>
-      </c>
-      <c r="X11" s="36" t="s">
-        <v>1204</v>
-      </c>
-      <c r="Y11" s="36" t="s">
-        <v>1205</v>
       </c>
     </row>
     <row r="13" spans="1:25" ht="13" customHeight="1">
@@ -16193,12 +16202,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E388B376-25CD-114A-9979-B5C580A31165}">
   <dimension ref="A1:Y155"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B10" sqref="B10"/>
       <selection pane="topRight" activeCell="B10" sqref="B10"/>
       <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
-      <selection pane="bottomRight" activeCell="E56" sqref="E56"/>
+      <selection pane="bottomRight" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="46.83203125" defaultRowHeight="13" customHeight="1"/>
@@ -16343,7 +16352,7 @@
         <v>819</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>1182</v>
+        <v>1179</v>
       </c>
       <c r="C10" s="36" t="str">
         <f>B10</f>
@@ -16380,19 +16389,19 @@
         <v>169</v>
       </c>
       <c r="B11" s="36" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C11" s="36" t="s">
+        <v>1165</v>
+      </c>
+      <c r="D11" s="36" t="s">
+        <v>1164</v>
+      </c>
+      <c r="E11" s="36" t="s">
+        <v>1178</v>
+      </c>
+      <c r="F11" s="36" t="s">
         <v>1166</v>
-      </c>
-      <c r="C11" s="36" t="s">
-        <v>1168</v>
-      </c>
-      <c r="D11" s="36" t="s">
-        <v>1167</v>
-      </c>
-      <c r="E11" s="36" t="s">
-        <v>1181</v>
-      </c>
-      <c r="F11" s="36" t="s">
-        <v>1169</v>
       </c>
     </row>
     <row r="13" spans="1:25" ht="13" customHeight="1">
@@ -16509,24 +16518,24 @@
     </row>
     <row r="20" spans="1:24" ht="13" customHeight="1">
       <c r="B20" s="36" t="s">
-        <v>1178</v>
+        <v>1276</v>
       </c>
       <c r="C20" s="36" t="s">
-        <v>1177</v>
+        <v>1174</v>
       </c>
       <c r="D20" s="36" t="s">
-        <v>1171</v>
+        <v>1168</v>
       </c>
       <c r="E20" s="36" t="s">
-        <v>1171</v>
+        <v>1168</v>
       </c>
       <c r="F20" s="36" t="s">
-        <v>1173</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="21" spans="1:24" ht="13" customHeight="1">
       <c r="B21" s="36" t="s">
-        <v>515</v>
+        <v>1275</v>
       </c>
       <c r="C21" s="36" t="s">
         <v>612</v>
@@ -16535,27 +16544,30 @@
         <v>147</v>
       </c>
       <c r="E21" s="36" t="s">
-        <v>1180</v>
+        <v>1177</v>
       </c>
       <c r="F21" s="36" t="s">
-        <v>1172</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="22" spans="1:24" ht="13" customHeight="1">
       <c r="B22" s="36" t="s">
-        <v>516</v>
+        <v>1175</v>
       </c>
       <c r="C22" s="36" t="s">
-        <v>148</v>
+        <v>1277</v>
       </c>
       <c r="E22" s="36" t="s">
         <v>147</v>
       </c>
       <c r="F22" s="36" t="s">
-        <v>145</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="23" spans="1:24" ht="13" customHeight="1">
+      <c r="B23" s="36" t="s">
+        <v>1274</v>
+      </c>
       <c r="C23" s="36" t="s">
         <v>149</v>
       </c>
@@ -16564,8 +16576,11 @@
       </c>
     </row>
     <row r="24" spans="1:24" ht="13" customHeight="1">
+      <c r="B24" s="36" t="s">
+        <v>516</v>
+      </c>
       <c r="F24" s="36" t="s">
-        <v>1179</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="26" spans="1:24" ht="13" customHeight="1">
@@ -16672,7 +16687,7 @@
     <row r="35" spans="1:25" ht="13" customHeight="1">
       <c r="B35" s="33"/>
       <c r="F35" s="36" t="s">
-        <v>1164</v>
+        <v>1161</v>
       </c>
       <c r="K35" s="33"/>
       <c r="L35" s="33"/>
@@ -16691,7 +16706,7 @@
     <row r="36" spans="1:25" ht="13" customHeight="1">
       <c r="B36" s="33"/>
       <c r="F36" s="36" t="s">
-        <v>1165</v>
+        <v>1162</v>
       </c>
       <c r="K36" s="33"/>
       <c r="L36" s="33"/>
@@ -16759,13 +16774,13 @@
         <v>1052</v>
       </c>
       <c r="D39" s="36" t="s">
-        <v>1157</v>
+        <v>1154</v>
       </c>
       <c r="E39" s="36" t="s">
-        <v>1174</v>
+        <v>1171</v>
       </c>
       <c r="F39" s="36" t="s">
-        <v>1162</v>
+        <v>1159</v>
       </c>
       <c r="K39" s="33"/>
       <c r="L39" s="33"/>
@@ -16786,7 +16801,7 @@
         <v>1148</v>
       </c>
       <c r="D40" s="36" t="s">
-        <v>1158</v>
+        <v>1155</v>
       </c>
       <c r="E40" s="36" t="s">
         <v>956</v>
@@ -16813,7 +16828,7 @@
         <v>983</v>
       </c>
       <c r="D41" s="36" t="s">
-        <v>1159</v>
+        <v>1156</v>
       </c>
       <c r="E41" s="36" t="s">
         <v>983</v>
@@ -16833,19 +16848,19 @@
     <row r="42" spans="1:25" ht="13" customHeight="1">
       <c r="A42" s="38"/>
       <c r="B42" s="36" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="C42" s="36" t="s">
         <v>1149</v>
       </c>
       <c r="D42" s="36" t="s">
+        <v>1157</v>
+      </c>
+      <c r="E42" s="36" t="s">
+        <v>1172</v>
+      </c>
+      <c r="F42" s="36" t="s">
         <v>1160</v>
-      </c>
-      <c r="E42" s="36" t="s">
-        <v>1175</v>
-      </c>
-      <c r="F42" s="36" t="s">
-        <v>1163</v>
       </c>
       <c r="K42" s="33"/>
       <c r="L42" s="33"/>
@@ -16861,16 +16876,16 @@
     <row r="43" spans="1:25" ht="13" customHeight="1">
       <c r="A43" s="38"/>
       <c r="B43" s="36" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="C43" s="36" t="s">
         <v>1150</v>
       </c>
       <c r="D43" s="36" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="E43" s="36" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="F43" s="36" t="s">
         <v>1150</v>
@@ -16888,23 +16903,23 @@
     <row r="44" spans="1:25" ht="13" customHeight="1">
       <c r="A44" s="38"/>
       <c r="B44" s="36" t="s">
-        <v>1151</v>
+        <v>925</v>
       </c>
       <c r="C44" s="36" t="str">
         <f>$B$44</f>
-        <v xml:space="preserve">    kind:   inner</v>
+        <v xml:space="preserve">    kind:   left</v>
       </c>
       <c r="D44" s="36" t="str">
         <f>$B$44</f>
-        <v xml:space="preserve">    kind:   inner</v>
+        <v xml:space="preserve">    kind:   left</v>
       </c>
       <c r="E44" s="36" t="str">
         <f>$B$44</f>
-        <v xml:space="preserve">    kind:   inner</v>
+        <v xml:space="preserve">    kind:   left</v>
       </c>
       <c r="F44" s="36" t="str">
         <f>$B$44</f>
-        <v xml:space="preserve">    kind:   inner</v>
+        <v xml:space="preserve">    kind:   left</v>
       </c>
       <c r="K44" s="33"/>
       <c r="L44" s="33"/>
@@ -16976,11 +16991,11 @@
     <row r="49" spans="1:22" ht="13" customHeight="1">
       <c r="A49" s="38"/>
       <c r="B49" s="36" t="s">
-        <v>1155</v>
+        <v>1272</v>
       </c>
       <c r="E49" s="36" t="str">
         <f>$B49</f>
-        <v xml:space="preserve">  col: g</v>
+        <v xml:space="preserve">  col: sg</v>
       </c>
       <c r="K49" s="33"/>
       <c r="L49" s="33"/>
@@ -16995,11 +17010,11 @@
     <row r="50" spans="1:22" ht="13" customHeight="1">
       <c r="A50" s="38"/>
       <c r="B50" s="36" t="s">
-        <v>1156</v>
+        <v>1273</v>
       </c>
       <c r="E50" s="36" t="str">
         <f t="shared" ref="E50:E51" si="0">$B50</f>
-        <v xml:space="preserve">  val: missing</v>
+        <v xml:space="preserve">  val: [0, 99]</v>
       </c>
       <c r="K50" s="33"/>
       <c r="L50" s="33"/>
@@ -17104,19 +17119,19 @@
         <v>523</v>
       </c>
       <c r="C55" s="36" t="str">
-        <f t="shared" ref="C55:F57" si="1">$B55</f>
+        <f>$B55</f>
         <v xml:space="preserve">  axis:   row</v>
       </c>
       <c r="D55" s="36" t="str">
-        <f t="shared" si="1"/>
+        <f>$B55</f>
         <v xml:space="preserve">  axis:   row</v>
       </c>
       <c r="E55" s="36" t="str">
-        <f t="shared" si="1"/>
+        <f>$B55</f>
         <v xml:space="preserve">  axis:   row</v>
       </c>
       <c r="F55" s="36" t="str">
-        <f t="shared" si="1"/>
+        <f>$B55</f>
         <v xml:space="preserve">  axis:   row</v>
       </c>
       <c r="K55" s="33"/>
@@ -17135,19 +17150,19 @@
         <v>525</v>
       </c>
       <c r="C56" s="36" t="str">
-        <f t="shared" si="1"/>
+        <f>$B56</f>
         <v xml:space="preserve">  from:   nothing</v>
       </c>
       <c r="D56" s="36" t="str">
-        <f t="shared" si="1"/>
+        <f>$B56</f>
         <v xml:space="preserve">  from:   nothing</v>
       </c>
       <c r="E56" s="36" t="str">
-        <f t="shared" si="1"/>
+        <f>$B56</f>
         <v xml:space="preserve">  from:   nothing</v>
       </c>
       <c r="F56" s="36" t="str">
-        <f t="shared" si="1"/>
+        <f>$B56</f>
         <v xml:space="preserve">  from:   nothing</v>
       </c>
       <c r="K56" s="33"/>
@@ -17165,19 +17180,19 @@
         <v>524</v>
       </c>
       <c r="C57" s="36" t="str">
-        <f t="shared" si="1"/>
+        <f>$B57</f>
         <v xml:space="preserve">  to:     nothing</v>
       </c>
       <c r="D57" s="36" t="str">
-        <f t="shared" si="1"/>
+        <f>$B57</f>
         <v xml:space="preserve">  to:     nothing</v>
       </c>
       <c r="E57" s="36" t="str">
-        <f t="shared" si="1"/>
+        <f>$B57</f>
         <v xml:space="preserve">  to:     nothing</v>
       </c>
       <c r="F57" s="36" t="str">
-        <f t="shared" si="1"/>
+        <f>$B57</f>
         <v xml:space="preserve">  to:     nothing</v>
       </c>
       <c r="K57" s="33"/>
@@ -17192,19 +17207,19 @@
     </row>
     <row r="58" spans="1:22" ht="13" customHeight="1">
       <c r="B58" s="36" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="C58" s="36" t="s">
-        <v>1176</v>
+        <v>1173</v>
       </c>
       <c r="D58" s="36" t="s">
-        <v>1161</v>
+        <v>1158</v>
       </c>
       <c r="E58" s="36" t="s">
-        <v>1161</v>
+        <v>1158</v>
       </c>
       <c r="F58" s="36" t="s">
-        <v>1170</v>
+        <v>1167</v>
       </c>
       <c r="K58" s="33"/>
       <c r="L58" s="33"/>
@@ -17706,74 +17721,94 @@
       <c r="S155" s="32"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="P2:XFD2 C17 A79:B80 A17 A11:C11 G24:XFD24 A18:C21 H17:XFD23 A22:D23 A7:D10 A12:D15 E7:XFD15 A1:XFD1 A2:N2 D79:XFD80 A81:XFD1048576 A16:XFD16 A3:XFD6 A24:E24 A25:XFD78 E17:E22">
-    <cfRule type="expression" dxfId="43" priority="26">
+  <conditionalFormatting sqref="P2:XFD2 C17 A79:B80 A17 A11:C11 G24:XFD24 A18:C21 H17:XFD23 A22:D23 A7:D10 A12:D15 E7:XFD15 A1:XFD1 A2:N2 D79:XFD80 A81:XFD1048576 A16:XFD16 A3:XFD6 A24:E24 E17:E22 A58:XFD58 A60:XFD78 B21:B24 D54:XFD57 A54:B57 D59:XFD59 A59:B59 A25:XFD53">
+    <cfRule type="expression" dxfId="43" priority="30">
       <formula>_xlfn.ISFORMULA(A1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C79:C80">
-    <cfRule type="expression" dxfId="42" priority="22">
+    <cfRule type="expression" dxfId="42" priority="26">
       <formula>_xlfn.ISFORMULA(C79)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1048576:XFD1048576">
-    <cfRule type="expression" dxfId="41" priority="213">
+    <cfRule type="expression" dxfId="41" priority="217">
       <formula>AND(COUNTA(#REF!)=0, NOT(ISBLANK($A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="expression" dxfId="40" priority="20">
+    <cfRule type="expression" dxfId="40" priority="24">
       <formula>_xlfn.ISFORMULA(D11)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F17:F21">
-    <cfRule type="expression" dxfId="39" priority="18">
+    <cfRule type="expression" dxfId="39" priority="22">
       <formula>_xlfn.ISFORMULA(F17)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F22">
-    <cfRule type="expression" dxfId="38" priority="16">
+    <cfRule type="expression" dxfId="38" priority="20">
       <formula>_xlfn.ISFORMULA(F22)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F23:F24">
-    <cfRule type="expression" dxfId="37" priority="14">
+    <cfRule type="expression" dxfId="37" priority="18">
       <formula>_xlfn.ISFORMULA(F23)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G17:G23">
-    <cfRule type="expression" dxfId="36" priority="10">
+    <cfRule type="expression" dxfId="36" priority="14">
       <formula>_xlfn.ISFORMULA(G17)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17:D21">
-    <cfRule type="expression" dxfId="35" priority="8">
+    <cfRule type="expression" dxfId="35" priority="12">
       <formula>_xlfn.ISFORMULA(D17)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:N2 P2:XFD2 C17 A17 E3:XFD16 E25:XFD33 E24 A2:D10 A12:D16 A37:XFD1048576 A18:C19 D17:XFD19 F20:XFD24 A20:D33 B11:D11">
-    <cfRule type="expression" dxfId="34" priority="273">
+  <conditionalFormatting sqref="E2:N2 P2:XFD2 C17 A17 E3:XFD16 E25:XFD33 E24 A2:D10 A12:D16 A18:C19 D17:XFD19 F20:XFD24 B11:D11 A60:XFD1048576 A20:D33 D54:XFD57 A54:B57 A58:XFD58 A59:B59 D59:XFD59 A37:XFD53">
+    <cfRule type="expression" dxfId="34" priority="277">
       <formula>AND(COUNTA($A2:$AA2)=0, NOT(ISBLANK($A3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:F15">
-    <cfRule type="expression" dxfId="33" priority="353">
+    <cfRule type="expression" dxfId="33" priority="357">
       <formula>AND(COUNTA($A17:$AA17)=0, NOT(ISBLANK($A18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36:XFD36">
-    <cfRule type="expression" dxfId="32" priority="361">
+    <cfRule type="expression" dxfId="32" priority="365">
       <formula>AND(COUNTA($A36:$AA36)=0, NOT(ISBLANK($A38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A34:XFD35">
-    <cfRule type="expression" dxfId="31" priority="368">
+    <cfRule type="expression" dxfId="31" priority="372">
       <formula>AND(COUNTA($A34:$AA34)=0, NOT(ISBLANK($A37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20:E22">
-    <cfRule type="expression" dxfId="30" priority="376">
+    <cfRule type="expression" dxfId="30" priority="380">
       <formula>AND(COUNTA($A21:$AA21)=0, NOT(ISBLANK($A22)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54:C57">
+    <cfRule type="expression" dxfId="3" priority="3">
+      <formula>_xlfn.ISFORMULA(C54)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54:C57">
+    <cfRule type="expression" dxfId="2" priority="4">
+      <formula>AND(COUNTA($A54:$AA54)=0, NOT(ISBLANK($A55)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>_xlfn.ISFORMULA(C59)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59">
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>AND(COUNTA($A59:$AA59)=0, NOT(ISBLANK($A60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17784,12 +17819,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{266920FD-CED0-424B-9125-46B736D1EB06}">
   <dimension ref="A1:T156"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B31" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B10" sqref="B10"/>
       <selection pane="topRight" activeCell="B10" sqref="B10"/>
       <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
-      <selection pane="bottomRight" activeCell="C79" sqref="C79"/>
+      <selection pane="bottomRight" activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="46.83203125" defaultRowHeight="13" customHeight="1"/>
@@ -17802,16 +17837,16 @@
   <sheetData>
     <row r="1" spans="1:20" s="57" customFormat="1" ht="13" customHeight="1">
       <c r="B1" s="57" t="s">
-        <v>1261</v>
+        <v>1258</v>
       </c>
       <c r="C1" s="57" t="s">
-        <v>1216</v>
+        <v>1213</v>
       </c>
       <c r="D1" s="57" t="s">
-        <v>1234</v>
+        <v>1231</v>
       </c>
       <c r="E1" s="57" t="s">
-        <v>1235</v>
+        <v>1232</v>
       </c>
       <c r="K1" s="58"/>
     </row>
@@ -17915,16 +17950,16 @@
         <v>819</v>
       </c>
       <c r="B10" s="56" t="s">
-        <v>1219</v>
+        <v>1216</v>
       </c>
       <c r="C10" s="56" t="s">
-        <v>1219</v>
+        <v>1216</v>
       </c>
       <c r="D10" s="60" t="s">
-        <v>1230</v>
+        <v>1227</v>
       </c>
       <c r="E10" s="60" t="s">
-        <v>1230</v>
+        <v>1227</v>
       </c>
       <c r="I10" s="60"/>
       <c r="J10" s="60"/>
@@ -17941,16 +17976,16 @@
         <v>169</v>
       </c>
       <c r="B11" s="56" t="s">
-        <v>1264</v>
+        <v>1261</v>
       </c>
       <c r="C11" s="56" t="s">
-        <v>1242</v>
+        <v>1239</v>
       </c>
       <c r="D11" s="56" t="s">
-        <v>1243</v>
+        <v>1240</v>
       </c>
       <c r="E11" s="56" t="s">
-        <v>1262</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="13" customHeight="1">
@@ -17974,13 +18009,13 @@
     </row>
     <row r="14" spans="1:20" ht="13" customHeight="1">
       <c r="B14" s="56" t="s">
-        <v>1220</v>
+        <v>1217</v>
       </c>
       <c r="C14" s="56" t="s">
-        <v>1220</v>
+        <v>1217</v>
       </c>
       <c r="D14" s="56" t="s">
-        <v>1244</v>
+        <v>1241</v>
       </c>
       <c r="E14" s="56" t="str">
         <f>D14</f>
@@ -17990,13 +18025,13 @@
     </row>
     <row r="15" spans="1:20" ht="13" customHeight="1">
       <c r="B15" s="56" t="s">
-        <v>1221</v>
+        <v>1218</v>
       </c>
       <c r="C15" s="56" t="s">
-        <v>1231</v>
+        <v>1228</v>
       </c>
       <c r="D15" s="56" t="s">
-        <v>1233</v>
+        <v>1230</v>
       </c>
       <c r="E15" s="56" t="str">
         <f>D15</f>
@@ -18006,19 +18041,19 @@
     </row>
     <row r="16" spans="1:20" ht="13" customHeight="1">
       <c r="B16" s="56" t="s">
-        <v>1217</v>
+        <v>1214</v>
       </c>
       <c r="C16" s="56" t="s">
-        <v>1232</v>
+        <v>1229</v>
       </c>
       <c r="I16" s="61"/>
     </row>
     <row r="17" spans="1:16" ht="13" customHeight="1">
       <c r="B17" s="56" t="s">
-        <v>1218</v>
+        <v>1215</v>
       </c>
       <c r="C17" s="56" t="s">
-        <v>1233</v>
+        <v>1230</v>
       </c>
       <c r="I17" s="61"/>
     </row>
@@ -18041,7 +18076,7 @@
     </row>
     <row r="20" spans="1:16" ht="13" customHeight="1">
       <c r="B20" s="56" t="s">
-        <v>1229</v>
+        <v>1226</v>
       </c>
       <c r="C20" s="56" t="s">
         <v>572</v>
@@ -18086,10 +18121,10 @@
     </row>
     <row r="23" spans="1:16" ht="13" customHeight="1">
       <c r="B23" s="56" t="s">
-        <v>1246</v>
+        <v>1243</v>
       </c>
       <c r="C23" s="56" t="s">
-        <v>1268</v>
+        <v>1265</v>
       </c>
       <c r="D23" s="56" t="s">
         <v>149</v>
@@ -18104,7 +18139,7 @@
         <v>404</v>
       </c>
       <c r="C24" s="56" t="s">
-        <v>1229</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="13" customHeight="1">
@@ -18112,15 +18147,15 @@
         <v>405</v>
       </c>
       <c r="C25" s="56" t="s">
-        <v>1236</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="13" customHeight="1">
       <c r="B26" s="56" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="C26" s="56" t="s">
-        <v>1274</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="13" customHeight="1">
@@ -18133,7 +18168,7 @@
     </row>
     <row r="28" spans="1:16" ht="13" customHeight="1">
       <c r="B28" s="56" t="s">
-        <v>1257</v>
+        <v>1254</v>
       </c>
       <c r="C28" s="56" t="s">
         <v>111</v>
@@ -18163,16 +18198,16 @@
     </row>
     <row r="31" spans="1:16" ht="13" customHeight="1">
       <c r="B31" s="56" t="s">
-        <v>1222</v>
+        <v>1219</v>
       </c>
       <c r="C31" s="56" t="s">
-        <v>1237</v>
+        <v>1234</v>
       </c>
       <c r="D31" s="56" t="s">
         <v>663</v>
       </c>
       <c r="E31" s="56" t="s">
-        <v>1263</v>
+        <v>1260</v>
       </c>
       <c r="J31" s="60"/>
       <c r="L31" s="59"/>
@@ -18182,20 +18217,20 @@
     </row>
     <row r="32" spans="1:16" ht="13" customHeight="1">
       <c r="B32" s="56" t="s">
-        <v>1224</v>
+        <v>1221</v>
       </c>
       <c r="C32" s="56" t="s">
-        <v>1239</v>
+        <v>1236</v>
       </c>
       <c r="J32" s="60"/>
       <c r="L32" s="60"/>
     </row>
     <row r="33" spans="1:20" ht="13" customHeight="1">
       <c r="B33" s="56" t="s">
-        <v>1224</v>
+        <v>1221</v>
       </c>
       <c r="C33" s="56" t="s">
-        <v>1267</v>
+        <v>1264</v>
       </c>
       <c r="F33" s="60"/>
       <c r="G33" s="60"/>
@@ -18213,7 +18248,7 @@
     </row>
     <row r="34" spans="1:20" ht="13" customHeight="1">
       <c r="C34" s="56" t="s">
-        <v>1238</v>
+        <v>1235</v>
       </c>
       <c r="F34" s="60"/>
       <c r="I34" s="60"/>
@@ -18283,7 +18318,7 @@
     </row>
     <row r="38" spans="1:20" ht="13" customHeight="1">
       <c r="B38" s="60" t="s">
-        <v>1227</v>
+        <v>1224</v>
       </c>
       <c r="F38" s="60"/>
       <c r="G38" s="60"/>
@@ -18301,7 +18336,7 @@
     </row>
     <row r="39" spans="1:20" ht="13" customHeight="1">
       <c r="B39" s="60" t="s">
-        <v>1228</v>
+        <v>1225</v>
       </c>
       <c r="F39" s="60"/>
       <c r="G39" s="60"/>
@@ -18317,7 +18352,7 @@
     </row>
     <row r="40" spans="1:20" ht="13" customHeight="1">
       <c r="B40" s="60" t="s">
-        <v>1226</v>
+        <v>1223</v>
       </c>
       <c r="F40" s="60"/>
       <c r="J40" s="60"/>
@@ -18331,7 +18366,7 @@
     </row>
     <row r="41" spans="1:20" ht="13" customHeight="1">
       <c r="B41" s="60" t="s">
-        <v>1247</v>
+        <v>1244</v>
       </c>
       <c r="F41" s="60"/>
       <c r="G41" s="60"/>
@@ -18359,7 +18394,7 @@
     </row>
     <row r="43" spans="1:20" ht="13" customHeight="1">
       <c r="B43" s="56" t="s">
-        <v>1248</v>
+        <v>1245</v>
       </c>
       <c r="F43" s="60"/>
       <c r="G43" s="60"/>
@@ -18372,7 +18407,7 @@
     </row>
     <row r="44" spans="1:20" ht="13" customHeight="1">
       <c r="B44" s="56" t="s">
-        <v>1249</v>
+        <v>1246</v>
       </c>
       <c r="F44" s="60"/>
       <c r="G44" s="60"/>
@@ -18387,7 +18422,7 @@
     </row>
     <row r="45" spans="1:20" ht="13" customHeight="1">
       <c r="B45" s="56" t="s">
-        <v>1250</v>
+        <v>1247</v>
       </c>
       <c r="G45" s="60"/>
       <c r="I45" s="60"/>
@@ -18401,7 +18436,7 @@
     </row>
     <row r="46" spans="1:20" ht="13" customHeight="1">
       <c r="B46" s="56" t="s">
-        <v>1251</v>
+        <v>1248</v>
       </c>
       <c r="F46" s="60"/>
       <c r="G46" s="60"/>
@@ -18414,7 +18449,7 @@
     </row>
     <row r="47" spans="1:20" ht="13" customHeight="1">
       <c r="B47" s="56" t="s">
-        <v>1254</v>
+        <v>1251</v>
       </c>
       <c r="F47" s="60"/>
       <c r="G47" s="60"/>
@@ -18443,7 +18478,7 @@
     <row r="49" spans="1:17" ht="13" customHeight="1">
       <c r="A49" s="62"/>
       <c r="B49" s="60" t="s">
-        <v>1255</v>
+        <v>1252</v>
       </c>
       <c r="F49" s="60"/>
       <c r="G49" s="60"/>
@@ -18488,7 +18523,7 @@
     <row r="52" spans="1:17" ht="13" customHeight="1">
       <c r="B52" s="60"/>
       <c r="C52" s="56" t="s">
-        <v>1269</v>
+        <v>1266</v>
       </c>
       <c r="F52" s="60"/>
       <c r="G52" s="60"/>
@@ -18503,7 +18538,7 @@
     <row r="53" spans="1:17" ht="13" customHeight="1">
       <c r="A53" s="62"/>
       <c r="C53" s="56" t="s">
-        <v>1270</v>
+        <v>1267</v>
       </c>
       <c r="G53" s="60"/>
       <c r="J53" s="60"/>
@@ -18681,7 +18716,7 @@
     <row r="63" spans="1:17" ht="13" customHeight="1">
       <c r="A63" s="62"/>
       <c r="C63" s="56" t="s">
-        <v>1265</v>
+        <v>1262</v>
       </c>
       <c r="J63" s="60"/>
       <c r="L63" s="60"/>
@@ -18693,7 +18728,7 @@
     <row r="64" spans="1:17" ht="13" customHeight="1">
       <c r="A64" s="62"/>
       <c r="C64" s="56" t="s">
-        <v>1271</v>
+        <v>1268</v>
       </c>
       <c r="F64" s="60"/>
       <c r="G64" s="60"/>
@@ -18703,7 +18738,7 @@
     <row r="65" spans="1:17" ht="13" customHeight="1">
       <c r="A65" s="62"/>
       <c r="C65" s="56" t="s">
-        <v>1272</v>
+        <v>1269</v>
       </c>
       <c r="F65" s="60"/>
       <c r="G65" s="60"/>
@@ -18713,7 +18748,7 @@
     <row r="66" spans="1:17" ht="13" customHeight="1">
       <c r="A66" s="62"/>
       <c r="C66" s="56" t="s">
-        <v>1228</v>
+        <v>1225</v>
       </c>
       <c r="F66" s="60"/>
       <c r="G66" s="60"/>
@@ -18723,7 +18758,7 @@
     <row r="67" spans="1:17" ht="13" customHeight="1">
       <c r="A67" s="62"/>
       <c r="C67" s="56" t="s">
-        <v>1273</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="68" spans="1:17" ht="13" customHeight="1">
@@ -18750,25 +18785,25 @@
     <row r="71" spans="1:17" ht="13" customHeight="1">
       <c r="A71" s="62"/>
       <c r="B71" s="56" t="s">
-        <v>1256</v>
+        <v>1253</v>
       </c>
       <c r="C71" s="56" t="s">
-        <v>1240</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="72" spans="1:17" ht="13" customHeight="1">
       <c r="A72" s="62"/>
       <c r="B72" s="56" t="s">
-        <v>1252</v>
+        <v>1249</v>
       </c>
       <c r="C72" s="56" t="s">
-        <v>1241</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="73" spans="1:17" ht="13" customHeight="1">
       <c r="A73" s="62"/>
       <c r="B73" s="56" t="s">
-        <v>1253</v>
+        <v>1250</v>
       </c>
       <c r="C73" s="56" t="s">
         <v>430</v>
@@ -18777,13 +18812,13 @@
     <row r="74" spans="1:17" ht="13" customHeight="1">
       <c r="A74" s="62"/>
       <c r="B74" s="56" t="s">
-        <v>1260</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="75" spans="1:17" ht="13" customHeight="1">
       <c r="A75" s="62"/>
       <c r="B75" s="56" t="s">
-        <v>1259</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="76" spans="1:17" ht="13" customHeight="1">
@@ -18809,16 +18844,16 @@
     <row r="79" spans="1:17" ht="13" customHeight="1">
       <c r="A79" s="62"/>
       <c r="B79" s="56" t="s">
-        <v>1225</v>
+        <v>1222</v>
       </c>
       <c r="C79" s="56" t="s">
-        <v>1266</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="80" spans="1:17" ht="13" customHeight="1">
       <c r="A80" s="62"/>
       <c r="B80" s="56" t="s">
-        <v>1223</v>
+        <v>1220</v>
       </c>
       <c r="C80" s="56" t="s">
         <v>19</v>
@@ -18901,7 +18936,7 @@
     <row r="88" spans="1:19" ht="13" customHeight="1">
       <c r="C88" s="36"/>
       <c r="D88" s="36" t="s">
-        <v>1245</v>
+        <v>1242</v>
       </c>
       <c r="E88" s="56" t="str">
         <f t="shared" si="1"/>
@@ -19260,102 +19295,102 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D51:XFD54 E74:XFD77 D56:XFD56 A55:XFD55 A63:XFD73 A40:B56 A57:A62 D57:E62 G57:XFD62 F78:XFD83 E80:E83 A69:E79 A78:D83 A63:B89 A84:XFD1048576 A1:XFD50">
-    <cfRule type="expression" dxfId="1" priority="29">
+    <cfRule type="expression" dxfId="29" priority="29">
       <formula>_xlfn.ISFORMULA(A1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56:C62">
-    <cfRule type="expression" dxfId="29" priority="10">
+    <cfRule type="expression" dxfId="28" priority="10">
       <formula>_xlfn.ISFORMULA(C56)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B63:B81">
-    <cfRule type="expression" dxfId="28" priority="18">
+    <cfRule type="expression" dxfId="27" priority="18">
       <formula>_xlfn.ISFORMULA(B63)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C51:C54">
-    <cfRule type="expression" dxfId="27" priority="16">
+    <cfRule type="expression" dxfId="26" priority="16">
       <formula>_xlfn.ISFORMULA(C51)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C74:C89">
-    <cfRule type="expression" dxfId="26" priority="14">
+    <cfRule type="expression" dxfId="25" priority="14">
       <formula>_xlfn.ISFORMULA(C74)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D74:D89">
-    <cfRule type="expression" dxfId="25" priority="12">
+    <cfRule type="expression" dxfId="24" priority="12">
       <formula>_xlfn.ISFORMULA(D74)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D54:XFD54 A54:B54">
-    <cfRule type="expression" dxfId="24" priority="428">
+    <cfRule type="expression" dxfId="23" priority="428">
       <formula>AND(COUNTA($A54:$V54)=0, NOT(ISBLANK(#REF!)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B54:C54">
-    <cfRule type="expression" dxfId="23" priority="441">
+    <cfRule type="expression" dxfId="22" priority="441">
       <formula>AND(COUNTA($A54:$Z54)=0, NOT(ISBLANK(#REF!)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:XFD55 E74:XFD77 C63:XFD73 D56:XFD56 D51:XFD53 A40:B53 A55:B56 A57:A62 D57:E62 G57:XFD62 F78:XFD83 E80:E83 C69:E79 C78:D83 A63:B1048574 C84:XFD1048574 A2:XFD50">
-    <cfRule type="expression" dxfId="0" priority="454">
+    <cfRule type="expression" dxfId="21" priority="454">
       <formula>AND(COUNTA($A2:$V2)=0, NOT(ISBLANK($A3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B52:B53 C51:C53 C56:C62 B49 B55:B56 C74:D89 B63:B81">
-    <cfRule type="expression" dxfId="16" priority="504">
+    <cfRule type="expression" dxfId="20" priority="504">
       <formula>AND(COUNTA($A49:$Z49)=0, NOT(ISBLANK($A50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1048576:XFD1048576">
-    <cfRule type="expression" dxfId="15" priority="512">
+    <cfRule type="expression" dxfId="19" priority="512">
       <formula>AND(COUNTA($A:$V)=0, NOT(ISBLANK($A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1048575:XFD1048575">
-    <cfRule type="expression" dxfId="14" priority="515">
+    <cfRule type="expression" dxfId="18" priority="515">
       <formula>AND(COUNTA($A1048575:$V1048576)=0, NOT(ISBLANK($A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B57:B62">
-    <cfRule type="expression" dxfId="13" priority="7">
+    <cfRule type="expression" dxfId="17" priority="7">
       <formula>_xlfn.ISFORMULA(B57)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B57:B62">
-    <cfRule type="expression" dxfId="12" priority="8">
+    <cfRule type="expression" dxfId="16" priority="8">
       <formula>AND(COUNTA($A57:$AA57)=0, NOT(ISBLANK($A58)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F57:F62">
-    <cfRule type="expression" dxfId="7" priority="5">
+    <cfRule type="expression" dxfId="15" priority="5">
       <formula>_xlfn.ISFORMULA(F57)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F57:F62">
-    <cfRule type="expression" dxfId="6" priority="6">
+    <cfRule type="expression" dxfId="14" priority="6">
       <formula>AND(COUNTA($A57:$AA57)=0, NOT(ISBLANK($A58)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E78:E83">
-    <cfRule type="expression" dxfId="5" priority="3">
+    <cfRule type="expression" dxfId="13" priority="3">
       <formula>_xlfn.ISFORMULA(E78)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E78:E83">
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="12" priority="4">
       <formula>AND(COUNTA($A78:$V78)=0, NOT(ISBLANK($A79)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E84:E89">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="11" priority="1">
       <formula>_xlfn.ISFORMULA(E84)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E84:E89">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="10" priority="2">
       <formula>AND(COUNTA($A84:$V84)=0, NOT(ISBLANK($A85)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24771,32 +24806,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="expression" dxfId="22" priority="6">
+    <cfRule type="expression" dxfId="9" priority="6">
       <formula>_xlfn.ISFORMULA(A1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G63:G67">
-    <cfRule type="expression" dxfId="21" priority="5">
+    <cfRule type="expression" dxfId="8" priority="5">
       <formula>_xlfn.ISFORMULA(G63)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G30:G31">
-    <cfRule type="expression" dxfId="20" priority="4">
+    <cfRule type="expression" dxfId="7" priority="4">
       <formula>_xlfn.ISFORMULA(G30)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G26:G27">
-    <cfRule type="expression" dxfId="19" priority="2">
+    <cfRule type="expression" dxfId="6" priority="2">
       <formula>_xlfn.ISFORMULA(G26)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G33:G58">
-    <cfRule type="expression" dxfId="18" priority="3">
+    <cfRule type="expression" dxfId="5" priority="3">
       <formula>_xlfn.ISFORMULA(G33)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M32">
-    <cfRule type="expression" dxfId="17" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>_xlfn.ISFORMULA(M32)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>